<commit_message>
time schedule is generated and button to run one right now
</commit_message>
<xml_diff>
--- a/data/AlertsToSimulate.xlsx
+++ b/data/AlertsToSimulate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brice/Developer/public/alertsimulator/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F50DCA3-4094-014F-9C10-BAD1EBFBA14E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82AD1468-7D32-F544-94ED-8E2DF8676A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1040" yWindow="800" windowWidth="24940" windowHeight="18800" xr2:uid="{11BBE7C0-3DF5-4C46-A363-C7759B687477}"/>
   </bookViews>
@@ -666,7 +666,7 @@
   <dimension ref="A1:H76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
id for notification and alert
</commit_message>
<xml_diff>
--- a/data/AlertsToSimulate.xlsx
+++ b/data/AlertsToSimulate.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brice/Developer/public/alertsimulator/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F18E1CB7-3A44-1B46-BCBB-7A4EE7192E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A545592-B042-A24F-9844-EC99D0C23908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="800" windowWidth="32220" windowHeight="18800" xr2:uid="{11BBE7C0-3DF5-4C46-A363-C7759B687477}"/>
+    <workbookView xWindow="0" yWindow="800" windowWidth="30240" windowHeight="18800" xr2:uid="{11BBE7C0-3DF5-4C46-A363-C7759B687477}"/>
   </bookViews>
   <sheets>
     <sheet name="Alerts" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Alerts!$A$1:$E$85</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Alerts!$B$1:$F$85</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="145">
   <si>
     <t>OIL PRESS</t>
   </si>
@@ -472,6 +472,9 @@
   </si>
   <si>
     <t>AP/PFD DIF AHRS</t>
+  </si>
+  <si>
+    <t>uid</t>
   </si>
 </sst>
 </file>
@@ -850,1939 +853,2192 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B50ED21-1FB3-1647-9374-5C9653EBF4CC}">
-  <dimension ref="A1:H85"/>
+  <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" customWidth="1"/>
-    <col min="8" max="8" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
+    <col min="9" max="9" width="24.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" t="s">
         <v>48</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>49</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>52</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>53</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>54</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>50</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>73</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>56</v>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" t="s">
         <v>63</v>
       </c>
-      <c r="E2" t="s">
-        <v>47</v>
-      </c>
       <c r="F2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>56</v>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" t="s">
         <v>63</v>
       </c>
-      <c r="E3" t="s">
-        <v>47</v>
-      </c>
       <c r="F3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>56</v>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" t="s">
         <v>63</v>
       </c>
-      <c r="E4" t="s">
-        <v>47</v>
-      </c>
       <c r="F4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" t="s">
         <v>4</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>56</v>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" t="s">
         <v>63</v>
       </c>
-      <c r="E5" t="s">
-        <v>47</v>
-      </c>
       <c r="F5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" t="s">
         <v>22</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>56</v>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" t="s">
         <v>59</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>65</v>
       </c>
-      <c r="E6" t="s">
-        <v>47</v>
-      </c>
       <c r="F6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" t="s">
         <v>23</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>56</v>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" t="s">
         <v>63</v>
       </c>
-      <c r="E7" t="s">
-        <v>47</v>
-      </c>
       <c r="F7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" t="s">
         <v>20</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>56</v>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C8" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" t="s">
         <v>63</v>
       </c>
-      <c r="E8" t="s">
-        <v>47</v>
-      </c>
       <c r="F8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" t="s">
         <v>20</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>56</v>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" t="s">
         <v>59</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>65</v>
       </c>
-      <c r="E9" t="s">
-        <v>47</v>
-      </c>
       <c r="F9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" t="s">
         <v>19</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>56</v>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" t="s">
         <v>59</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>65</v>
       </c>
-      <c r="E10" t="s">
-        <v>47</v>
-      </c>
       <c r="F10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" t="s">
         <v>19</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>56</v>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" t="s">
         <v>60</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>63</v>
       </c>
-      <c r="E11" t="s">
-        <v>47</v>
-      </c>
       <c r="F11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" t="s">
         <v>21</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>56</v>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" t="s">
         <v>60</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>63</v>
       </c>
-      <c r="E12" t="s">
-        <v>47</v>
-      </c>
       <c r="F12" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" t="s">
         <v>21</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>56</v>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C13" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D13" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" t="s">
         <v>63</v>
       </c>
-      <c r="E13" t="s">
-        <v>47</v>
-      </c>
       <c r="F13" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" t="s">
         <v>18</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>56</v>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C14" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" t="s">
         <v>63</v>
       </c>
-      <c r="E14" t="s">
-        <v>47</v>
-      </c>
       <c r="F14" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" t="s">
         <v>24</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>56</v>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" t="s">
         <v>63</v>
       </c>
-      <c r="E15" t="s">
-        <v>47</v>
-      </c>
       <c r="F15" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" t="s">
         <v>141</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>56</v>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C16" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" t="s">
         <v>63</v>
       </c>
-      <c r="E16" t="s">
-        <v>47</v>
-      </c>
       <c r="F16" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" t="s">
         <v>142</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>56</v>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C17" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" t="s">
         <v>63</v>
       </c>
-      <c r="E17" t="s">
-        <v>47</v>
-      </c>
       <c r="F17" t="s">
+        <v>47</v>
+      </c>
+      <c r="G17" t="s">
         <v>143</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>56</v>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C18" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D18" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" t="s">
         <v>63</v>
       </c>
-      <c r="E18" t="s">
-        <v>47</v>
-      </c>
       <c r="F18" t="s">
+        <v>47</v>
+      </c>
+      <c r="G18" t="s">
         <v>116</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>56</v>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C19" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" t="s">
         <v>63</v>
       </c>
-      <c r="E19" t="s">
-        <v>47</v>
-      </c>
       <c r="F19" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" t="s">
         <v>9</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>56</v>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" t="s">
         <v>59</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>65</v>
       </c>
-      <c r="E20" t="s">
-        <v>47</v>
-      </c>
       <c r="F20" t="s">
+        <v>47</v>
+      </c>
+      <c r="G20" t="s">
         <v>15</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>56</v>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C21" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" t="s">
         <v>59</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>65</v>
       </c>
-      <c r="E21" t="s">
-        <v>47</v>
-      </c>
       <c r="F21" t="s">
+        <v>47</v>
+      </c>
+      <c r="G21" t="s">
         <v>79</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>56</v>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C22" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" t="s">
         <v>60</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>63</v>
       </c>
-      <c r="E22" t="s">
-        <v>47</v>
-      </c>
       <c r="F22" t="s">
+        <v>47</v>
+      </c>
+      <c r="G22" t="s">
         <v>119</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>56</v>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C23" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" t="s">
         <v>59</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>65</v>
       </c>
-      <c r="E23" t="s">
-        <v>47</v>
-      </c>
       <c r="F23" t="s">
+        <v>47</v>
+      </c>
+      <c r="G23" t="s">
         <v>6</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="H23" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>56</v>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" t="s">
         <v>60</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>63</v>
       </c>
-      <c r="E24" t="s">
-        <v>47</v>
-      </c>
       <c r="F24" t="s">
+        <v>47</v>
+      </c>
+      <c r="G24" t="s">
         <v>5</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="H24" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>56</v>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" t="s">
         <v>60</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>63</v>
       </c>
-      <c r="E25" t="s">
-        <v>47</v>
-      </c>
       <c r="F25" t="s">
+        <v>47</v>
+      </c>
+      <c r="G25" t="s">
         <v>122</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>56</v>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C26" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" t="s">
         <v>60</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>63</v>
       </c>
-      <c r="E26" t="s">
-        <v>47</v>
-      </c>
       <c r="F26" t="s">
+        <v>47</v>
+      </c>
+      <c r="G26" t="s">
         <v>124</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>56</v>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C27" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" t="s">
         <v>60</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>63</v>
       </c>
-      <c r="E27" t="s">
-        <v>47</v>
-      </c>
       <c r="F27" t="s">
+        <v>47</v>
+      </c>
+      <c r="G27" t="s">
         <v>126</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>56</v>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C28" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D28" t="s">
+        <v>61</v>
+      </c>
+      <c r="E28" t="s">
         <v>63</v>
       </c>
-      <c r="E28" t="s">
-        <v>47</v>
-      </c>
       <c r="F28" t="s">
+        <v>47</v>
+      </c>
+      <c r="G28" t="s">
         <v>7</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>56</v>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C29" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D29" t="s">
+        <v>61</v>
+      </c>
+      <c r="E29" t="s">
         <v>63</v>
       </c>
-      <c r="E29" t="s">
-        <v>47</v>
-      </c>
       <c r="F29" t="s">
+        <v>47</v>
+      </c>
+      <c r="G29" t="s">
         <v>8</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>56</v>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C30" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D30" t="s">
+        <v>61</v>
+      </c>
+      <c r="E30" t="s">
         <v>64</v>
       </c>
-      <c r="E30" t="s">
-        <v>47</v>
-      </c>
       <c r="F30" t="s">
+        <v>47</v>
+      </c>
+      <c r="G30" t="s">
         <v>2</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>56</v>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C31" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D31" t="s">
+        <v>61</v>
+      </c>
+      <c r="E31" t="s">
         <v>64</v>
       </c>
-      <c r="E31" t="s">
-        <v>47</v>
-      </c>
       <c r="F31" t="s">
+        <v>47</v>
+      </c>
+      <c r="G31" t="s">
         <v>138</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>56</v>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C32" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D32" t="s">
+        <v>61</v>
+      </c>
+      <c r="E32" t="s">
         <v>64</v>
       </c>
-      <c r="E32" t="s">
-        <v>47</v>
-      </c>
       <c r="F32" t="s">
+        <v>47</v>
+      </c>
+      <c r="G32" t="s">
         <v>139</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>56</v>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C33" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D33" t="s">
+        <v>61</v>
+      </c>
+      <c r="E33" t="s">
         <v>64</v>
       </c>
-      <c r="E33" t="s">
-        <v>47</v>
-      </c>
       <c r="F33" t="s">
+        <v>47</v>
+      </c>
+      <c r="G33" t="s">
         <v>0</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>56</v>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C34" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D34" t="s">
+        <v>61</v>
+      </c>
+      <c r="E34" t="s">
         <v>64</v>
       </c>
-      <c r="E34" t="s">
-        <v>47</v>
-      </c>
       <c r="F34" t="s">
+        <v>47</v>
+      </c>
+      <c r="G34" t="s">
         <v>1</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>56</v>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C35" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" t="s">
         <v>59</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>65</v>
       </c>
-      <c r="E35" t="s">
-        <v>47</v>
-      </c>
       <c r="F35" t="s">
+        <v>47</v>
+      </c>
+      <c r="G35" t="s">
         <v>16</v>
       </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>56</v>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C36" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D36" t="s">
+        <v>61</v>
+      </c>
+      <c r="E36" t="s">
         <v>63</v>
       </c>
-      <c r="E36" t="s">
-        <v>47</v>
-      </c>
       <c r="F36" t="s">
+        <v>47</v>
+      </c>
+      <c r="G36" t="s">
         <v>17</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H36" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>56</v>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C37" t="s">
+        <v>55</v>
+      </c>
+      <c r="D37" t="s">
         <v>59</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>65</v>
       </c>
-      <c r="E37" t="s">
-        <v>47</v>
-      </c>
       <c r="F37" t="s">
+        <v>47</v>
+      </c>
+      <c r="G37" t="s">
         <v>25</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>56</v>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C38" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D38" t="s">
+        <v>61</v>
+      </c>
+      <c r="E38" t="s">
         <v>64</v>
       </c>
-      <c r="E38" t="s">
-        <v>47</v>
-      </c>
       <c r="F38" t="s">
+        <v>47</v>
+      </c>
+      <c r="G38" t="s">
         <v>12</v>
       </c>
-      <c r="G38" t="s">
+      <c r="H38" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>56</v>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C39" t="s">
+        <v>55</v>
+      </c>
+      <c r="D39" t="s">
         <v>59</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>65</v>
       </c>
-      <c r="E39" t="s">
-        <v>47</v>
-      </c>
       <c r="F39" t="s">
+        <v>47</v>
+      </c>
+      <c r="G39" t="s">
         <v>13</v>
       </c>
-      <c r="G39" t="s">
+      <c r="H39" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>56</v>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C40" t="s">
+        <v>55</v>
+      </c>
+      <c r="D40" t="s">
         <v>59</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>65</v>
       </c>
-      <c r="E40" t="s">
-        <v>47</v>
-      </c>
       <c r="F40" t="s">
+        <v>47</v>
+      </c>
+      <c r="G40" t="s">
         <v>133</v>
       </c>
-      <c r="G40" t="s">
+      <c r="H40" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>56</v>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C41" t="s">
+        <v>55</v>
+      </c>
+      <c r="D41" t="s">
         <v>59</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>65</v>
       </c>
-      <c r="E41" t="s">
-        <v>47</v>
-      </c>
       <c r="F41" t="s">
+        <v>47</v>
+      </c>
+      <c r="G41" t="s">
         <v>135</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>56</v>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C42" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D42" t="s">
+        <v>61</v>
+      </c>
+      <c r="E42" t="s">
         <v>63</v>
       </c>
-      <c r="E42" t="s">
-        <v>47</v>
-      </c>
       <c r="F42" t="s">
+        <v>47</v>
+      </c>
+      <c r="G42" t="s">
         <v>3</v>
       </c>
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>56</v>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C43" t="s">
+        <v>55</v>
+      </c>
+      <c r="D43" t="s">
         <v>59</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
         <v>65</v>
       </c>
-      <c r="E43" t="s">
-        <v>47</v>
-      </c>
       <c r="F43" t="s">
+        <v>47</v>
+      </c>
+      <c r="G43" t="s">
         <v>14</v>
       </c>
-      <c r="G43" t="s">
+      <c r="H43" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>57</v>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C44" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D44" t="s">
+        <v>61</v>
+      </c>
+      <c r="E44" t="s">
         <v>62</v>
       </c>
-      <c r="E44" t="s">
-        <v>47</v>
-      </c>
       <c r="F44" t="s">
+        <v>47</v>
+      </c>
+      <c r="G44" t="s">
         <v>39</v>
       </c>
-      <c r="G44" t="s">
+      <c r="H44" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>57</v>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C45" t="s">
+        <v>55</v>
+      </c>
+      <c r="D45" t="s">
         <v>59</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
         <v>65</v>
       </c>
-      <c r="E45" t="s">
-        <v>47</v>
-      </c>
       <c r="F45" t="s">
+        <v>47</v>
+      </c>
+      <c r="G45" t="s">
         <v>19</v>
       </c>
-      <c r="G45" t="s">
+      <c r="H45" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>57</v>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C46" t="s">
+        <v>55</v>
+      </c>
+      <c r="D46" t="s">
         <v>59</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>65</v>
       </c>
-      <c r="E46" t="s">
-        <v>47</v>
-      </c>
       <c r="F46" t="s">
+        <v>47</v>
+      </c>
+      <c r="G46" t="s">
         <v>19</v>
       </c>
-      <c r="G46" t="s">
+      <c r="H46" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>57</v>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C47" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D47" t="s">
+        <v>61</v>
+      </c>
+      <c r="E47" t="s">
         <v>62</v>
       </c>
-      <c r="E47" t="s">
-        <v>47</v>
-      </c>
       <c r="F47" t="s">
+        <v>47</v>
+      </c>
+      <c r="G47" t="s">
         <v>38</v>
       </c>
-      <c r="G47" t="s">
+      <c r="H47" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>57</v>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C48" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D48" t="s">
+        <v>61</v>
+      </c>
+      <c r="E48" t="s">
         <v>63</v>
       </c>
-      <c r="E48" t="s">
-        <v>47</v>
-      </c>
       <c r="F48" t="s">
+        <v>47</v>
+      </c>
+      <c r="G48" t="s">
         <v>15</v>
       </c>
-      <c r="G48" t="s">
+      <c r="H48" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>57</v>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C49" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D49" t="s">
+        <v>61</v>
+      </c>
+      <c r="E49" t="s">
         <v>64</v>
       </c>
-      <c r="E49" t="s">
-        <v>47</v>
-      </c>
       <c r="F49" t="s">
+        <v>47</v>
+      </c>
+      <c r="G49" t="s">
         <v>29</v>
       </c>
-      <c r="G49" t="s">
+      <c r="H49" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>57</v>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C50" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D50" t="s">
+        <v>61</v>
+      </c>
+      <c r="E50" t="s">
         <v>64</v>
       </c>
-      <c r="E50" t="s">
-        <v>47</v>
-      </c>
       <c r="F50" t="s">
+        <v>47</v>
+      </c>
+      <c r="G50" t="s">
         <v>36</v>
       </c>
-      <c r="G50" t="s">
+      <c r="H50" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>57</v>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C51" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D51" t="s">
+        <v>61</v>
+      </c>
+      <c r="E51" t="s">
         <v>62</v>
       </c>
-      <c r="E51" t="s">
-        <v>47</v>
-      </c>
       <c r="F51" t="s">
+        <v>47</v>
+      </c>
+      <c r="G51" t="s">
         <v>35</v>
       </c>
-      <c r="G51" t="s">
+      <c r="H51" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>57</v>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C52" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D52" t="s">
+        <v>61</v>
+      </c>
+      <c r="E52" t="s">
         <v>64</v>
       </c>
-      <c r="E52" t="s">
-        <v>47</v>
-      </c>
       <c r="F52" t="s">
+        <v>47</v>
+      </c>
+      <c r="G52" t="s">
         <v>40</v>
       </c>
-      <c r="G52" t="s">
+      <c r="H52" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>57</v>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C53" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D53" t="s">
+        <v>61</v>
+      </c>
+      <c r="E53" t="s">
         <v>64</v>
       </c>
-      <c r="E53" t="s">
-        <v>47</v>
-      </c>
       <c r="F53" t="s">
+        <v>47</v>
+      </c>
+      <c r="G53" t="s">
         <v>140</v>
       </c>
-      <c r="G53" t="s">
+      <c r="H53" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>57</v>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C54" t="s">
+        <v>55</v>
+      </c>
+      <c r="D54" t="s">
         <v>59</v>
       </c>
-      <c r="D54" t="s">
+      <c r="E54" t="s">
         <v>65</v>
       </c>
-      <c r="E54" t="s">
-        <v>47</v>
-      </c>
       <c r="F54" t="s">
+        <v>47</v>
+      </c>
+      <c r="G54" t="s">
         <v>6</v>
       </c>
-      <c r="G54" t="s">
+      <c r="H54" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>57</v>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C55" t="s">
+        <v>55</v>
+      </c>
+      <c r="D55" t="s">
         <v>59</v>
       </c>
-      <c r="D55" t="s">
+      <c r="E55" t="s">
         <v>65</v>
       </c>
-      <c r="E55" t="s">
-        <v>47</v>
-      </c>
       <c r="F55" t="s">
+        <v>47</v>
+      </c>
+      <c r="G55" t="s">
         <v>32</v>
       </c>
-      <c r="G55" t="s">
+      <c r="H55" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>57</v>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C56" t="s">
+        <v>55</v>
+      </c>
+      <c r="D56" t="s">
         <v>59</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
         <v>65</v>
       </c>
-      <c r="E56" t="s">
-        <v>47</v>
-      </c>
       <c r="F56" t="s">
+        <v>47</v>
+      </c>
+      <c r="G56" t="s">
         <v>33</v>
       </c>
-      <c r="G56" t="s">
+      <c r="H56" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>57</v>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C57" t="s">
+        <v>55</v>
+      </c>
+      <c r="D57" t="s">
         <v>59</v>
       </c>
-      <c r="D57" t="s">
+      <c r="E57" t="s">
         <v>65</v>
       </c>
-      <c r="E57" t="s">
-        <v>47</v>
-      </c>
       <c r="F57" t="s">
+        <v>47</v>
+      </c>
+      <c r="G57" t="s">
         <v>5</v>
       </c>
-      <c r="G57" t="s">
+      <c r="H57" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C58" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D58" t="s">
+        <v>61</v>
+      </c>
+      <c r="E58" t="s">
         <v>64</v>
       </c>
-      <c r="E58" t="s">
-        <v>47</v>
-      </c>
       <c r="F58" t="s">
+        <v>47</v>
+      </c>
+      <c r="G58" t="s">
         <v>34</v>
       </c>
-      <c r="G58" t="s">
+      <c r="H58" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>57</v>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C59" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D59" t="s">
+        <v>61</v>
+      </c>
+      <c r="E59" t="s">
         <v>62</v>
       </c>
-      <c r="E59" t="s">
-        <v>47</v>
-      </c>
       <c r="F59" t="s">
+        <v>47</v>
+      </c>
+      <c r="G59" t="s">
         <v>7</v>
       </c>
-      <c r="G59" t="s">
+      <c r="H59" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>57</v>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C60" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D60" t="s">
+        <v>61</v>
+      </c>
+      <c r="E60" t="s">
         <v>62</v>
       </c>
-      <c r="E60" t="s">
-        <v>47</v>
-      </c>
       <c r="F60" t="s">
+        <v>47</v>
+      </c>
+      <c r="G60" t="s">
         <v>8</v>
       </c>
-      <c r="G60" t="s">
+      <c r="H60" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>57</v>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C61" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D61" t="s">
+        <v>61</v>
+      </c>
+      <c r="E61" t="s">
         <v>64</v>
       </c>
-      <c r="E61" t="s">
-        <v>47</v>
-      </c>
       <c r="F61" t="s">
+        <v>47</v>
+      </c>
+      <c r="G61" t="s">
         <v>2</v>
       </c>
-      <c r="G61" t="s">
+      <c r="H61" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>57</v>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C62" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D62" t="s">
+        <v>61</v>
+      </c>
+      <c r="E62" t="s">
         <v>64</v>
       </c>
-      <c r="E62" t="s">
-        <v>47</v>
-      </c>
       <c r="F62" t="s">
+        <v>47</v>
+      </c>
+      <c r="G62" t="s">
         <v>0</v>
       </c>
-      <c r="G62" t="s">
+      <c r="H62" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>57</v>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C63" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D63" t="s">
+        <v>61</v>
+      </c>
+      <c r="E63" t="s">
         <v>64</v>
       </c>
-      <c r="E63" t="s">
-        <v>47</v>
-      </c>
       <c r="F63" t="s">
+        <v>47</v>
+      </c>
+      <c r="G63" t="s">
         <v>1</v>
       </c>
-      <c r="G63" t="s">
+      <c r="H63" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>57</v>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C64" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D64" t="s">
+        <v>61</v>
+      </c>
+      <c r="E64" t="s">
         <v>62</v>
       </c>
-      <c r="E64" t="s">
-        <v>47</v>
-      </c>
       <c r="F64" t="s">
+        <v>47</v>
+      </c>
+      <c r="G64" t="s">
         <v>37</v>
       </c>
-      <c r="G64" t="s">
+      <c r="H64" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>57</v>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C65" t="s">
+        <v>55</v>
+      </c>
+      <c r="D65" t="s">
         <v>59</v>
       </c>
-      <c r="D65" t="s">
+      <c r="E65" t="s">
         <v>65</v>
       </c>
-      <c r="E65" t="s">
-        <v>47</v>
-      </c>
       <c r="F65" t="s">
+        <v>47</v>
+      </c>
+      <c r="G65" t="s">
         <v>16</v>
       </c>
-      <c r="G65" t="s">
+      <c r="H65" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>57</v>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C66" t="s">
+        <v>55</v>
+      </c>
+      <c r="D66" t="s">
         <v>59</v>
       </c>
-      <c r="D66" t="s">
+      <c r="E66" t="s">
         <v>65</v>
       </c>
-      <c r="E66" t="s">
-        <v>47</v>
-      </c>
       <c r="F66" t="s">
+        <v>47</v>
+      </c>
+      <c r="G66" t="s">
         <v>17</v>
       </c>
-      <c r="G66" t="s">
+      <c r="H66" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>57</v>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C67" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D67" t="s">
+        <v>61</v>
+      </c>
+      <c r="E67" t="s">
         <v>62</v>
       </c>
-      <c r="E67" t="s">
-        <v>47</v>
-      </c>
       <c r="F67" t="s">
+        <v>47</v>
+      </c>
+      <c r="G67" t="s">
         <v>31</v>
       </c>
-      <c r="G67" t="s">
+      <c r="H67" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>57</v>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C68" t="s">
+        <v>55</v>
+      </c>
+      <c r="D68" t="s">
         <v>59</v>
       </c>
-      <c r="D68" t="s">
+      <c r="E68" t="s">
         <v>65</v>
       </c>
-      <c r="E68" t="s">
-        <v>47</v>
-      </c>
       <c r="F68" t="s">
+        <v>47</v>
+      </c>
+      <c r="G68" t="s">
         <v>41</v>
       </c>
-      <c r="G68" t="s">
+      <c r="H68" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>57</v>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C69" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D69" t="s">
+        <v>61</v>
+      </c>
+      <c r="E69" t="s">
         <v>63</v>
       </c>
-      <c r="E69" t="s">
-        <v>47</v>
-      </c>
       <c r="F69" t="s">
+        <v>47</v>
+      </c>
+      <c r="G69" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>57</v>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C70" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D70" t="s">
+        <v>61</v>
+      </c>
+      <c r="E70" t="s">
         <v>62</v>
       </c>
-      <c r="E70" t="s">
-        <v>47</v>
-      </c>
       <c r="F70" t="s">
+        <v>47</v>
+      </c>
+      <c r="G70" t="s">
         <v>30</v>
       </c>
-      <c r="G70" t="s">
+      <c r="H70" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>56</v>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>70</v>
       </c>
       <c r="B71" t="s">
+        <v>56</v>
+      </c>
+      <c r="C71" t="s">
         <v>58</v>
       </c>
-      <c r="C71" t="s">
-        <v>61</v>
-      </c>
       <c r="D71" t="s">
+        <v>61</v>
+      </c>
+      <c r="E71" t="s">
         <v>64</v>
       </c>
-      <c r="E71" t="s">
-        <v>47</v>
-      </c>
       <c r="F71" t="s">
+        <v>47</v>
+      </c>
+      <c r="G71" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>56</v>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>71</v>
       </c>
       <c r="B72" t="s">
+        <v>56</v>
+      </c>
+      <c r="C72" t="s">
         <v>58</v>
       </c>
-      <c r="C72" t="s">
-        <v>61</v>
-      </c>
       <c r="D72" t="s">
+        <v>61</v>
+      </c>
+      <c r="E72" t="s">
         <v>64</v>
       </c>
-      <c r="E72" t="s">
-        <v>47</v>
-      </c>
       <c r="F72" t="s">
+        <v>47</v>
+      </c>
+      <c r="G72" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>56</v>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>72</v>
       </c>
       <c r="B73" t="s">
+        <v>56</v>
+      </c>
+      <c r="C73" t="s">
         <v>58</v>
       </c>
-      <c r="C73" t="s">
-        <v>61</v>
-      </c>
       <c r="D73" t="s">
+        <v>61</v>
+      </c>
+      <c r="E73" t="s">
         <v>64</v>
       </c>
-      <c r="E73" t="s">
-        <v>47</v>
-      </c>
       <c r="F73" t="s">
+        <v>47</v>
+      </c>
+      <c r="G73" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>56</v>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>73</v>
       </c>
       <c r="B74" t="s">
+        <v>56</v>
+      </c>
+      <c r="C74" t="s">
         <v>58</v>
       </c>
-      <c r="C74" t="s">
-        <v>61</v>
-      </c>
       <c r="D74" t="s">
+        <v>61</v>
+      </c>
+      <c r="E74" t="s">
         <v>64</v>
       </c>
-      <c r="E74" t="s">
-        <v>47</v>
-      </c>
       <c r="F74" t="s">
+        <v>47</v>
+      </c>
+      <c r="G74" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>56</v>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>74</v>
       </c>
       <c r="B75" t="s">
+        <v>56</v>
+      </c>
+      <c r="C75" t="s">
         <v>58</v>
       </c>
-      <c r="C75" t="s">
-        <v>61</v>
-      </c>
       <c r="D75" t="s">
+        <v>61</v>
+      </c>
+      <c r="E75" t="s">
         <v>64</v>
       </c>
-      <c r="E75" t="s">
-        <v>47</v>
-      </c>
       <c r="F75" t="s">
+        <v>47</v>
+      </c>
+      <c r="G75" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>56</v>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>75</v>
       </c>
       <c r="B76" t="s">
+        <v>56</v>
+      </c>
+      <c r="C76" t="s">
         <v>58</v>
       </c>
-      <c r="C76" t="s">
-        <v>61</v>
-      </c>
       <c r="D76" t="s">
+        <v>61</v>
+      </c>
+      <c r="E76" t="s">
         <v>64</v>
       </c>
-      <c r="E76" t="s">
-        <v>47</v>
-      </c>
       <c r="F76" t="s">
+        <v>47</v>
+      </c>
+      <c r="G76" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>57</v>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>76</v>
       </c>
       <c r="B77" t="s">
+        <v>57</v>
+      </c>
+      <c r="C77" t="s">
         <v>58</v>
       </c>
-      <c r="C77" t="s">
+      <c r="D77" t="s">
         <v>60</v>
       </c>
-      <c r="D77" t="s">
+      <c r="E77" t="s">
         <v>62</v>
       </c>
-      <c r="E77" t="s">
-        <v>47</v>
-      </c>
       <c r="F77" t="s">
+        <v>47</v>
+      </c>
+      <c r="G77" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>57</v>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>77</v>
       </c>
       <c r="B78" t="s">
+        <v>57</v>
+      </c>
+      <c r="C78" t="s">
         <v>58</v>
       </c>
-      <c r="C78" t="s">
+      <c r="D78" t="s">
         <v>60</v>
       </c>
-      <c r="D78" t="s">
+      <c r="E78" t="s">
         <v>62</v>
       </c>
-      <c r="E78" t="s">
-        <v>47</v>
-      </c>
       <c r="F78" t="s">
+        <v>47</v>
+      </c>
+      <c r="G78" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>57</v>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>78</v>
       </c>
       <c r="B79" t="s">
+        <v>57</v>
+      </c>
+      <c r="C79" t="s">
         <v>58</v>
       </c>
-      <c r="C79" t="s">
+      <c r="D79" t="s">
         <v>60</v>
       </c>
-      <c r="D79" t="s">
+      <c r="E79" t="s">
         <v>62</v>
       </c>
-      <c r="E79" t="s">
-        <v>47</v>
-      </c>
       <c r="F79" t="s">
+        <v>47</v>
+      </c>
+      <c r="G79" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>57</v>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>79</v>
       </c>
       <c r="B80" t="s">
+        <v>57</v>
+      </c>
+      <c r="C80" t="s">
         <v>58</v>
       </c>
-      <c r="C80" t="s">
-        <v>61</v>
-      </c>
       <c r="D80" t="s">
+        <v>61</v>
+      </c>
+      <c r="E80" t="s">
         <v>64</v>
       </c>
-      <c r="E80" t="s">
-        <v>47</v>
-      </c>
       <c r="F80" t="s">
+        <v>47</v>
+      </c>
+      <c r="G80" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>57</v>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>80</v>
       </c>
       <c r="B81" t="s">
+        <v>57</v>
+      </c>
+      <c r="C81" t="s">
         <v>58</v>
       </c>
-      <c r="C81" t="s">
-        <v>61</v>
-      </c>
       <c r="D81" t="s">
+        <v>61</v>
+      </c>
+      <c r="E81" t="s">
         <v>62</v>
       </c>
-      <c r="E81" t="s">
-        <v>47</v>
-      </c>
       <c r="F81" t="s">
+        <v>47</v>
+      </c>
+      <c r="G81" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>57</v>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>81</v>
       </c>
       <c r="B82" t="s">
+        <v>57</v>
+      </c>
+      <c r="C82" t="s">
         <v>58</v>
       </c>
-      <c r="C82" t="s">
-        <v>61</v>
-      </c>
       <c r="D82" t="s">
+        <v>61</v>
+      </c>
+      <c r="E82" t="s">
         <v>64</v>
       </c>
-      <c r="E82" t="s">
-        <v>47</v>
-      </c>
       <c r="F82" t="s">
+        <v>47</v>
+      </c>
+      <c r="G82" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>57</v>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>82</v>
       </c>
       <c r="B83" t="s">
+        <v>57</v>
+      </c>
+      <c r="C83" t="s">
         <v>58</v>
       </c>
-      <c r="C83" t="s">
-        <v>61</v>
-      </c>
       <c r="D83" t="s">
+        <v>61</v>
+      </c>
+      <c r="E83" t="s">
         <v>62</v>
       </c>
-      <c r="E83" t="s">
-        <v>47</v>
-      </c>
       <c r="F83" t="s">
+        <v>47</v>
+      </c>
+      <c r="G83" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>57</v>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>83</v>
       </c>
       <c r="B84" t="s">
+        <v>57</v>
+      </c>
+      <c r="C84" t="s">
         <v>58</v>
       </c>
-      <c r="C84" t="s">
-        <v>61</v>
-      </c>
       <c r="D84" t="s">
+        <v>61</v>
+      </c>
+      <c r="E84" t="s">
         <v>62</v>
       </c>
-      <c r="E84" t="s">
-        <v>47</v>
-      </c>
       <c r="F84" t="s">
+        <v>47</v>
+      </c>
+      <c r="G84" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>57</v>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>84</v>
       </c>
       <c r="B85" t="s">
+        <v>57</v>
+      </c>
+      <c r="C85" t="s">
         <v>58</v>
       </c>
-      <c r="C85" t="s">
-        <v>61</v>
-      </c>
       <c r="D85" t="s">
+        <v>61</v>
+      </c>
+      <c r="E85" t="s">
         <v>64</v>
       </c>
-      <c r="E85" t="s">
-        <v>47</v>
-      </c>
       <c r="F85" t="s">
+        <v>47</v>
+      </c>
+      <c r="G85" t="s">
         <v>44</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E75" xr:uid="{1B50ED21-1FB3-1647-9374-5C9653EBF4CC}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E75">
-      <sortCondition ref="D2:D75"/>
+  <autoFilter ref="B1:F75" xr:uid="{1B50ED21-1FB3-1647-9374-5C9653EBF4CC}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:F75">
+      <sortCondition ref="E2:E75"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H76">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:I76">
+    <sortCondition ref="C2:C76"/>
     <sortCondition ref="B2:B76"/>
-    <sortCondition ref="A2:A76"/>
-    <sortCondition ref="F2:F76"/>
+    <sortCondition ref="G2:G76"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
generate dates and saves to settings
</commit_message>
<xml_diff>
--- a/data/AlertsToSimulate.xlsx
+++ b/data/AlertsToSimulate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brice/Developer/public/alertsimulator/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A545592-B042-A24F-9844-EC99D0C23908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31CE9CF8-03A4-7C40-9B76-6297B374CDDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="800" windowWidth="30240" windowHeight="18800" xr2:uid="{11BBE7C0-3DF5-4C46-A363-C7759B687477}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="144">
   <si>
     <t>OIL PRESS</t>
   </si>
@@ -193,9 +193,6 @@
   </si>
   <si>
     <t>message</t>
-  </si>
-  <si>
-    <t>description</t>
   </si>
   <si>
     <t>action</t>
@@ -853,20 +850,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B50ED21-1FB3-1647-9374-5C9653EBF4CC}">
-  <dimension ref="A1:I85"/>
+  <dimension ref="A1:H85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="7" max="7" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" customWidth="1"/>
-    <col min="9" max="9" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="180" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B1" t="s">
         <v>48</v>
@@ -875,39 +873,36 @@
         <v>49</v>
       </c>
       <c r="D1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" t="s">
         <v>52</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>53</v>
-      </c>
-      <c r="F1" t="s">
-        <v>54</v>
       </c>
       <c r="G1" t="s">
         <v>50</v>
       </c>
       <c r="H1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F2" t="s">
         <v>47</v>
@@ -916,24 +911,24 @@
         <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F3" t="s">
         <v>47</v>
@@ -942,24 +937,24 @@
         <v>11</v>
       </c>
       <c r="H3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F4" t="s">
         <v>47</v>
@@ -968,24 +963,24 @@
         <v>4</v>
       </c>
       <c r="H4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F5" t="s">
         <v>47</v>
@@ -994,24 +989,24 @@
         <v>22</v>
       </c>
       <c r="H5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F6" t="s">
         <v>47</v>
@@ -1020,24 +1015,24 @@
         <v>23</v>
       </c>
       <c r="H6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F7" t="s">
         <v>47</v>
@@ -1046,24 +1041,24 @@
         <v>20</v>
       </c>
       <c r="H7" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F8" t="s">
         <v>47</v>
@@ -1072,24 +1067,24 @@
         <v>20</v>
       </c>
       <c r="H8" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F9" t="s">
         <v>47</v>
@@ -1098,24 +1093,24 @@
         <v>19</v>
       </c>
       <c r="H9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F10" t="s">
         <v>47</v>
@@ -1124,24 +1119,24 @@
         <v>19</v>
       </c>
       <c r="H10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F11" t="s">
         <v>47</v>
@@ -1150,24 +1145,24 @@
         <v>21</v>
       </c>
       <c r="H11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F12" t="s">
         <v>47</v>
@@ -1176,24 +1171,24 @@
         <v>21</v>
       </c>
       <c r="H12" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F13" t="s">
         <v>47</v>
@@ -1202,24 +1197,24 @@
         <v>18</v>
       </c>
       <c r="H13" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F14" t="s">
         <v>47</v>
@@ -1228,59 +1223,59 @@
         <v>24</v>
       </c>
       <c r="H14" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F15" t="s">
         <v>47</v>
       </c>
       <c r="G15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H15" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F16" t="s">
         <v>47</v>
       </c>
       <c r="G16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -1288,25 +1283,25 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F17" t="s">
         <v>47</v>
       </c>
       <c r="G17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -1314,25 +1309,25 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F18" t="s">
         <v>47</v>
       </c>
       <c r="G18" t="s">
+        <v>115</v>
+      </c>
+      <c r="H18" t="s">
         <v>116</v>
-      </c>
-      <c r="H18" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -1340,16 +1335,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F19" t="s">
         <v>47</v>
@@ -1358,7 +1353,7 @@
         <v>9</v>
       </c>
       <c r="H19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -1366,16 +1361,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F20" t="s">
         <v>47</v>
@@ -1384,7 +1379,7 @@
         <v>15</v>
       </c>
       <c r="H20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -1392,25 +1387,25 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F21" t="s">
         <v>47</v>
       </c>
       <c r="G21" t="s">
+        <v>78</v>
+      </c>
+      <c r="H21" t="s">
         <v>79</v>
-      </c>
-      <c r="H21" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -1418,25 +1413,25 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F22" t="s">
         <v>47</v>
       </c>
       <c r="G22" t="s">
+        <v>118</v>
+      </c>
+      <c r="H22" t="s">
         <v>119</v>
-      </c>
-      <c r="H22" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -1444,16 +1439,16 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F23" t="s">
         <v>47</v>
@@ -1462,7 +1457,7 @@
         <v>6</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -1470,16 +1465,16 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F24" t="s">
         <v>47</v>
@@ -1488,7 +1483,7 @@
         <v>5</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -1496,25 +1491,25 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F25" t="s">
         <v>47</v>
       </c>
       <c r="G25" t="s">
+        <v>121</v>
+      </c>
+      <c r="H25" t="s">
         <v>122</v>
-      </c>
-      <c r="H25" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -1522,25 +1517,25 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F26" t="s">
         <v>47</v>
       </c>
       <c r="G26" t="s">
+        <v>123</v>
+      </c>
+      <c r="H26" t="s">
         <v>124</v>
-      </c>
-      <c r="H26" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -1548,25 +1543,25 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F27" t="s">
         <v>47</v>
       </c>
       <c r="G27" t="s">
+        <v>125</v>
+      </c>
+      <c r="H27" t="s">
         <v>126</v>
-      </c>
-      <c r="H27" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -1574,16 +1569,16 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F28" t="s">
         <v>47</v>
@@ -1592,7 +1587,7 @@
         <v>7</v>
       </c>
       <c r="H28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -1600,16 +1595,16 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F29" t="s">
         <v>47</v>
@@ -1618,7 +1613,7 @@
         <v>8</v>
       </c>
       <c r="H29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -1626,16 +1621,16 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F30" t="s">
         <v>47</v>
@@ -1644,7 +1639,7 @@
         <v>2</v>
       </c>
       <c r="H30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -1652,25 +1647,25 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F31" t="s">
         <v>47</v>
       </c>
       <c r="G31" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -1678,25 +1673,25 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F32" t="s">
         <v>47</v>
       </c>
       <c r="G32" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H32" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -1704,16 +1699,16 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E33" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F33" t="s">
         <v>47</v>
@@ -1722,7 +1717,7 @@
         <v>0</v>
       </c>
       <c r="H33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -1730,16 +1725,16 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E34" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F34" t="s">
         <v>47</v>
@@ -1748,7 +1743,7 @@
         <v>1</v>
       </c>
       <c r="H34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -1756,16 +1751,16 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D35" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F35" t="s">
         <v>47</v>
@@ -1774,7 +1769,7 @@
         <v>16</v>
       </c>
       <c r="H35" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
@@ -1782,16 +1777,16 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C36" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F36" t="s">
         <v>47</v>
@@ -1800,7 +1795,7 @@
         <v>17</v>
       </c>
       <c r="H36" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
@@ -1808,16 +1803,16 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D37" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E37" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F37" t="s">
         <v>47</v>
@@ -1826,7 +1821,7 @@
         <v>25</v>
       </c>
       <c r="H37" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -1834,16 +1829,16 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F38" t="s">
         <v>47</v>
@@ -1852,7 +1847,7 @@
         <v>12</v>
       </c>
       <c r="H38" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
@@ -1860,16 +1855,16 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E39" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F39" t="s">
         <v>47</v>
@@ -1878,7 +1873,7 @@
         <v>13</v>
       </c>
       <c r="H39" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
@@ -1886,25 +1881,25 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C40" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E40" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F40" t="s">
         <v>47</v>
       </c>
       <c r="G40" t="s">
+        <v>132</v>
+      </c>
+      <c r="H40" t="s">
         <v>133</v>
-      </c>
-      <c r="H40" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
@@ -1912,25 +1907,25 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D41" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E41" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F41" t="s">
         <v>47</v>
       </c>
       <c r="G41" t="s">
+        <v>134</v>
+      </c>
+      <c r="H41" t="s">
         <v>135</v>
-      </c>
-      <c r="H41" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
@@ -1938,16 +1933,16 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C42" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E42" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F42" t="s">
         <v>47</v>
@@ -1956,7 +1951,7 @@
         <v>3</v>
       </c>
       <c r="H42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
@@ -1964,16 +1959,16 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C43" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D43" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E43" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F43" t="s">
         <v>47</v>
@@ -1982,7 +1977,7 @@
         <v>14</v>
       </c>
       <c r="H43" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
@@ -1990,16 +1985,16 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D44" t="s">
+        <v>60</v>
+      </c>
+      <c r="E44" t="s">
         <v>61</v>
-      </c>
-      <c r="E44" t="s">
-        <v>62</v>
       </c>
       <c r="F44" t="s">
         <v>47</v>
@@ -2008,7 +2003,7 @@
         <v>39</v>
       </c>
       <c r="H44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
@@ -2016,16 +2011,16 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C45" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D45" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E45" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F45" t="s">
         <v>47</v>
@@ -2034,7 +2029,7 @@
         <v>19</v>
       </c>
       <c r="H45" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
@@ -2042,16 +2037,16 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C46" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E46" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F46" t="s">
         <v>47</v>
@@ -2060,7 +2055,7 @@
         <v>19</v>
       </c>
       <c r="H46" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
@@ -2068,16 +2063,16 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C47" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D47" t="s">
+        <v>60</v>
+      </c>
+      <c r="E47" t="s">
         <v>61</v>
-      </c>
-      <c r="E47" t="s">
-        <v>62</v>
       </c>
       <c r="F47" t="s">
         <v>47</v>
@@ -2086,7 +2081,7 @@
         <v>38</v>
       </c>
       <c r="H47" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
@@ -2094,16 +2089,16 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C48" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D48" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E48" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F48" t="s">
         <v>47</v>
@@ -2112,7 +2107,7 @@
         <v>15</v>
       </c>
       <c r="H48" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
@@ -2120,16 +2115,16 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C49" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E49" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F49" t="s">
         <v>47</v>
@@ -2138,7 +2133,7 @@
         <v>29</v>
       </c>
       <c r="H49" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
@@ -2146,16 +2141,16 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C50" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E50" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F50" t="s">
         <v>47</v>
@@ -2164,7 +2159,7 @@
         <v>36</v>
       </c>
       <c r="H50" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
@@ -2172,16 +2167,16 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C51" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D51" t="s">
+        <v>60</v>
+      </c>
+      <c r="E51" t="s">
         <v>61</v>
-      </c>
-      <c r="E51" t="s">
-        <v>62</v>
       </c>
       <c r="F51" t="s">
         <v>47</v>
@@ -2190,7 +2185,7 @@
         <v>35</v>
       </c>
       <c r="H51" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
@@ -2198,16 +2193,16 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C52" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D52" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E52" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F52" t="s">
         <v>47</v>
@@ -2216,7 +2211,7 @@
         <v>40</v>
       </c>
       <c r="H52" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
@@ -2224,25 +2219,25 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C53" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D53" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E53" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F53" t="s">
         <v>47</v>
       </c>
       <c r="G53" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H53" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
@@ -2250,16 +2245,16 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C54" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D54" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E54" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F54" t="s">
         <v>47</v>
@@ -2268,7 +2263,7 @@
         <v>6</v>
       </c>
       <c r="H54" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
@@ -2276,16 +2271,16 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C55" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D55" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E55" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F55" t="s">
         <v>47</v>
@@ -2294,7 +2289,7 @@
         <v>32</v>
       </c>
       <c r="H55" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
@@ -2302,16 +2297,16 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C56" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D56" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E56" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F56" t="s">
         <v>47</v>
@@ -2320,7 +2315,7 @@
         <v>33</v>
       </c>
       <c r="H56" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
@@ -2328,16 +2323,16 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C57" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D57" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E57" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F57" t="s">
         <v>47</v>
@@ -2346,7 +2341,7 @@
         <v>5</v>
       </c>
       <c r="H57" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
@@ -2354,16 +2349,16 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C58" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D58" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E58" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F58" t="s">
         <v>47</v>
@@ -2372,7 +2367,7 @@
         <v>34</v>
       </c>
       <c r="H58" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
@@ -2380,16 +2375,16 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C59" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D59" t="s">
+        <v>60</v>
+      </c>
+      <c r="E59" t="s">
         <v>61</v>
-      </c>
-      <c r="E59" t="s">
-        <v>62</v>
       </c>
       <c r="F59" t="s">
         <v>47</v>
@@ -2398,7 +2393,7 @@
         <v>7</v>
       </c>
       <c r="H59" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
@@ -2406,16 +2401,16 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C60" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D60" t="s">
+        <v>60</v>
+      </c>
+      <c r="E60" t="s">
         <v>61</v>
-      </c>
-      <c r="E60" t="s">
-        <v>62</v>
       </c>
       <c r="F60" t="s">
         <v>47</v>
@@ -2424,7 +2419,7 @@
         <v>8</v>
       </c>
       <c r="H60" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
@@ -2432,16 +2427,16 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C61" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D61" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E61" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F61" t="s">
         <v>47</v>
@@ -2450,7 +2445,7 @@
         <v>2</v>
       </c>
       <c r="H61" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
@@ -2458,16 +2453,16 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C62" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E62" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F62" t="s">
         <v>47</v>
@@ -2476,7 +2471,7 @@
         <v>0</v>
       </c>
       <c r="H62" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
@@ -2484,16 +2479,16 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C63" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D63" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E63" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F63" t="s">
         <v>47</v>
@@ -2502,7 +2497,7 @@
         <v>1</v>
       </c>
       <c r="H63" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
@@ -2510,16 +2505,16 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C64" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D64" t="s">
+        <v>60</v>
+      </c>
+      <c r="E64" t="s">
         <v>61</v>
-      </c>
-      <c r="E64" t="s">
-        <v>62</v>
       </c>
       <c r="F64" t="s">
         <v>47</v>
@@ -2528,7 +2523,7 @@
         <v>37</v>
       </c>
       <c r="H64" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
@@ -2536,16 +2531,16 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C65" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D65" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E65" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F65" t="s">
         <v>47</v>
@@ -2554,7 +2549,7 @@
         <v>16</v>
       </c>
       <c r="H65" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
@@ -2562,16 +2557,16 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C66" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D66" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E66" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F66" t="s">
         <v>47</v>
@@ -2580,7 +2575,7 @@
         <v>17</v>
       </c>
       <c r="H66" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
@@ -2588,16 +2583,16 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C67" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D67" t="s">
+        <v>60</v>
+      </c>
+      <c r="E67" t="s">
         <v>61</v>
-      </c>
-      <c r="E67" t="s">
-        <v>62</v>
       </c>
       <c r="F67" t="s">
         <v>47</v>
@@ -2606,7 +2601,7 @@
         <v>31</v>
       </c>
       <c r="H67" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
@@ -2614,16 +2609,16 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C68" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D68" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E68" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F68" t="s">
         <v>47</v>
@@ -2632,7 +2627,7 @@
         <v>41</v>
       </c>
       <c r="H68" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
@@ -2640,16 +2635,16 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C69" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D69" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E69" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F69" t="s">
         <v>47</v>
@@ -2663,16 +2658,16 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C70" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D70" t="s">
+        <v>60</v>
+      </c>
+      <c r="E70" t="s">
         <v>61</v>
-      </c>
-      <c r="E70" t="s">
-        <v>62</v>
       </c>
       <c r="F70" t="s">
         <v>47</v>
@@ -2681,7 +2676,7 @@
         <v>30</v>
       </c>
       <c r="H70" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
@@ -2689,22 +2684,22 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C71" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E71" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F71" t="s">
         <v>47</v>
       </c>
       <c r="G71" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
@@ -2712,22 +2707,22 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C72" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D72" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E72" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F72" t="s">
         <v>47</v>
       </c>
       <c r="G72" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
@@ -2735,22 +2730,22 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C73" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D73" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E73" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F73" t="s">
         <v>47</v>
       </c>
       <c r="G73" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
@@ -2758,16 +2753,16 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C74" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D74" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E74" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F74" t="s">
         <v>47</v>
@@ -2781,16 +2776,16 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C75" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D75" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E75" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F75" t="s">
         <v>47</v>
@@ -2804,16 +2799,16 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C76" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D76" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E76" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F76" t="s">
         <v>47</v>
@@ -2827,22 +2822,22 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
+        <v>56</v>
+      </c>
+      <c r="C77" t="s">
         <v>57</v>
       </c>
-      <c r="C77" t="s">
-        <v>58</v>
-      </c>
       <c r="D77" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E77" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F77" t="s">
         <v>47</v>
       </c>
       <c r="G77" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
@@ -2850,22 +2845,22 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
+        <v>56</v>
+      </c>
+      <c r="C78" t="s">
         <v>57</v>
       </c>
-      <c r="C78" t="s">
-        <v>58</v>
-      </c>
       <c r="D78" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E78" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F78" t="s">
         <v>47</v>
       </c>
       <c r="G78" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
@@ -2873,22 +2868,22 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
+        <v>56</v>
+      </c>
+      <c r="C79" t="s">
         <v>57</v>
       </c>
-      <c r="C79" t="s">
-        <v>58</v>
-      </c>
       <c r="D79" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E79" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F79" t="s">
         <v>47</v>
       </c>
       <c r="G79" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
@@ -2896,16 +2891,16 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
+        <v>56</v>
+      </c>
+      <c r="C80" t="s">
         <v>57</v>
       </c>
-      <c r="C80" t="s">
-        <v>58</v>
-      </c>
       <c r="D80" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E80" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F80" t="s">
         <v>47</v>
@@ -2919,22 +2914,22 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
+        <v>56</v>
+      </c>
+      <c r="C81" t="s">
         <v>57</v>
       </c>
-      <c r="C81" t="s">
-        <v>58</v>
-      </c>
       <c r="D81" t="s">
+        <v>60</v>
+      </c>
+      <c r="E81" t="s">
         <v>61</v>
       </c>
-      <c r="E81" t="s">
-        <v>62</v>
-      </c>
       <c r="F81" t="s">
         <v>47</v>
       </c>
       <c r="G81" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
@@ -2942,16 +2937,16 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
+        <v>56</v>
+      </c>
+      <c r="C82" t="s">
         <v>57</v>
       </c>
-      <c r="C82" t="s">
-        <v>58</v>
-      </c>
       <c r="D82" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E82" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F82" t="s">
         <v>47</v>
@@ -2965,16 +2960,16 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
+        <v>56</v>
+      </c>
+      <c r="C83" t="s">
         <v>57</v>
       </c>
-      <c r="C83" t="s">
-        <v>58</v>
-      </c>
       <c r="D83" t="s">
+        <v>60</v>
+      </c>
+      <c r="E83" t="s">
         <v>61</v>
-      </c>
-      <c r="E83" t="s">
-        <v>62</v>
       </c>
       <c r="F83" t="s">
         <v>47</v>
@@ -2988,16 +2983,16 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
+        <v>56</v>
+      </c>
+      <c r="C84" t="s">
         <v>57</v>
       </c>
-      <c r="C84" t="s">
-        <v>58</v>
-      </c>
       <c r="D84" t="s">
+        <v>60</v>
+      </c>
+      <c r="E84" t="s">
         <v>61</v>
-      </c>
-      <c r="E84" t="s">
-        <v>62</v>
       </c>
       <c r="F84" t="s">
         <v>47</v>
@@ -3011,16 +3006,16 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
+        <v>56</v>
+      </c>
+      <c r="C85" t="s">
         <v>57</v>
       </c>
-      <c r="C85" t="s">
-        <v>58</v>
-      </c>
       <c r="D85" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E85" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F85" t="s">
         <v>47</v>
@@ -3035,7 +3030,7 @@
       <sortCondition ref="E2:E75"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:I76">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:H76">
     <sortCondition ref="C2:C76"/>
     <sortCondition ref="B2:B76"/>
     <sortCondition ref="G2:G76"/>

</xml_diff>

<commit_message>
added g7 alerts and ui to choose airplane
</commit_message>
<xml_diff>
--- a/data/AlertsToSimulate.xlsx
+++ b/data/AlertsToSimulate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brice/Developer/public/alertsimulator/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31CE9CF8-03A4-7C40-9B76-6297B374CDDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43162837-9B92-FA43-AF39-67462C6F4487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="800" windowWidth="30240" windowHeight="18800" xr2:uid="{11BBE7C0-3DF5-4C46-A363-C7759B687477}"/>
+    <workbookView xWindow="13820" yWindow="500" windowWidth="30240" windowHeight="18800" xr2:uid="{11BBE7C0-3DF5-4C46-A363-C7759B687477}"/>
   </bookViews>
   <sheets>
     <sheet name="Alerts" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1412" uniqueCount="289">
   <si>
     <t>OIL PRESS</t>
   </si>
@@ -472,6 +472,441 @@
   </si>
   <si>
     <t>uid</t>
+  </si>
+  <si>
+    <t>S22TG7</t>
+  </si>
+  <si>
+    <t>APPROACH SPEED </t>
+  </si>
+  <si>
+    <t>Approach Speed is too high. </t>
+  </si>
+  <si>
+    <t>AUTO DESCENT </t>
+  </si>
+  <si>
+    <t>Automatic descent to 14,000FT in 60 seconds. </t>
+  </si>
+  <si>
+    <t>Aircraft descending to 14,000FT. </t>
+  </si>
+  <si>
+    <t>Aircraft descending to 12,500FT. </t>
+  </si>
+  <si>
+    <t>Aircraft descended due to pilot incapacitation. </t>
+  </si>
+  <si>
+    <t>CO LVL HIGH </t>
+  </si>
+  <si>
+    <t>ESSENTIAL BUS VOLTS </t>
+  </si>
+  <si>
+    <t>Full flaps prohibited in icing conditions. </t>
+  </si>
+  <si>
+    <t>FUEL FLOW </t>
+  </si>
+  <si>
+    <t>FUEL IMBALANCE </t>
+  </si>
+  <si>
+    <t>FUEL LOW LEFT </t>
+  </si>
+  <si>
+    <t>Left fuel tank is nearly empty. </t>
+  </si>
+  <si>
+    <t>FUEL LOW RIGHT </t>
+  </si>
+  <si>
+    <t>Right fuel tank is nearly empty. </t>
+  </si>
+  <si>
+    <t>FUEL LOW TOTAL </t>
+  </si>
+  <si>
+    <t>IPS CONTROL FAIL </t>
+  </si>
+  <si>
+    <t>IPS valves cannot be closed. </t>
+  </si>
+  <si>
+    <t>IPS FLUID LOW </t>
+  </si>
+  <si>
+    <t>IPS fluid quantity is low. </t>
+  </si>
+  <si>
+    <t>IPS QUANTITY FAIL </t>
+  </si>
+  <si>
+    <t>Left and right IPS fluid quantities are unknown. </t>
+  </si>
+  <si>
+    <t>MAIN BUS 1 VOLTS </t>
+  </si>
+  <si>
+    <t>MAIN BUS 2 VOLTS </t>
+  </si>
+  <si>
+    <t>MANIFOLD PRESSURE </t>
+  </si>
+  <si>
+    <t>OIL PRESSURE </t>
+  </si>
+  <si>
+    <t>OIL TEMP </t>
+  </si>
+  <si>
+    <t>RPM </t>
+  </si>
+  <si>
+    <t>SPIN SPIN SPIN </t>
+  </si>
+  <si>
+    <t>STALL </t>
+  </si>
+  <si>
+    <t>Stall warning. </t>
+  </si>
+  <si>
+    <t>STALL WARNING FAIL </t>
+  </si>
+  <si>
+    <t>Stall warning is inoperative. </t>
+  </si>
+  <si>
+    <t>STARTER ENGAGED </t>
+  </si>
+  <si>
+    <t>Turbine inlet temperature is high. </t>
+  </si>
+  <si>
+    <t>AOA OVERHEAT2 </t>
+  </si>
+  <si>
+    <t>FLAPS ICE2 </t>
+  </si>
+  <si>
+    <t>OXYGEN FAULT1 </t>
+  </si>
+  <si>
+    <t>OXYGEN QTY LOW1 </t>
+  </si>
+  <si>
+    <t>OXYGEN REQUIRED1 </t>
+  </si>
+  <si>
+    <t>TIT3 </t>
+  </si>
+  <si>
+    <t>ALT AIR OPEN2 </t>
+  </si>
+  <si>
+    <t>ALTERNATOR 1 CURRENT </t>
+  </si>
+  <si>
+    <t>ALTERNATOR 2 CURRENT </t>
+  </si>
+  <si>
+    <t>AOA HEAT FAIL 3 </t>
+  </si>
+  <si>
+    <t>Autopilot is unavailable due to miscompare. </t>
+  </si>
+  <si>
+    <t>AP MISCOMPARE </t>
+  </si>
+  <si>
+    <t>AP/PFD DIF ADC </t>
+  </si>
+  <si>
+    <t>AP/PFD DIF AHRS </t>
+  </si>
+  <si>
+    <t>BATTERY 1 CURRENT </t>
+  </si>
+  <si>
+    <t>BATTERY 1 FAIL </t>
+  </si>
+  <si>
+    <t>Battery 1 service is required. </t>
+  </si>
+  <si>
+    <t>BATTERY 1 FAULT </t>
+  </si>
+  <si>
+    <t>Battery 1 fault detected. </t>
+  </si>
+  <si>
+    <t>BATTERY 1 LOW </t>
+  </si>
+  <si>
+    <t>Battery 1 state of charge is low. </t>
+  </si>
+  <si>
+    <t>FLAPS AIRSPEED INHIBIT </t>
+  </si>
+  <si>
+    <t>Flaps motion inhibited. </t>
+  </si>
+  <si>
+    <t>FLAPS DISAGREE </t>
+  </si>
+  <si>
+    <t>Flaps not in commanded position. </t>
+  </si>
+  <si>
+    <t>FLAPS FAIL </t>
+  </si>
+  <si>
+    <t>FLAPS SELECTOR FAIL </t>
+  </si>
+  <si>
+    <t>FUEL PUMP OFF </t>
+  </si>
+  <si>
+    <t>Fuel pump is turned off. </t>
+  </si>
+  <si>
+    <t>FUEL QTY MISCOMP </t>
+  </si>
+  <si>
+    <t>Sensed and totalized fuel quantity disagreement. </t>
+  </si>
+  <si>
+    <t>FUEL VALVE AUTO FAIL </t>
+  </si>
+  <si>
+    <t>Automatic fuel tank selection is unavailable. </t>
+  </si>
+  <si>
+    <t>HYPOXIA ALERT </t>
+  </si>
+  <si>
+    <t>Hypoxia caution alert. </t>
+  </si>
+  <si>
+    <t>IPS FLUID LOW3 </t>
+  </si>
+  <si>
+    <t>IPS IMBALANCE3 </t>
+  </si>
+  <si>
+    <t>IPS fluid quantity imbalance has been detected. </t>
+  </si>
+  <si>
+    <t>IPS PRESSURE HIGH3 </t>
+  </si>
+  <si>
+    <t>IPS pressure is high. </t>
+  </si>
+  <si>
+    <t>IPS PRESSURE LOW 3 </t>
+  </si>
+  <si>
+    <t>IPS tail pressure is low. </t>
+  </si>
+  <si>
+    <t>IPS QUANTITY FAIL 3 </t>
+  </si>
+  <si>
+    <t>Left IPS fluid quantity is unreliable. </t>
+  </si>
+  <si>
+    <t>Right IPS fluid quantity is unreliable. </t>
+  </si>
+  <si>
+    <t>IPS SPEED HIGH 3 </t>
+  </si>
+  <si>
+    <t>Airspeed is too high for ice protection. </t>
+  </si>
+  <si>
+    <t>IPS SPEED LOW 3 </t>
+  </si>
+  <si>
+    <t>Airspeed is too low for ice protection. </t>
+  </si>
+  <si>
+    <t>IPS TEMP LOW 3 </t>
+  </si>
+  <si>
+    <t>Temperature is too low for ice protection. </t>
+  </si>
+  <si>
+    <t>NO ADC MODES </t>
+  </si>
+  <si>
+    <t>NO VERT MODES </t>
+  </si>
+  <si>
+    <t>PARK BRAKE </t>
+  </si>
+  <si>
+    <t>PITOT HEAT FAIL </t>
+  </si>
+  <si>
+    <t>PROBE HEAT OFF </t>
+  </si>
+  <si>
+    <t>Probe heat is required. </t>
+  </si>
+  <si>
+    <t>SFD ALT MISCOMPARE </t>
+  </si>
+  <si>
+    <t>SFD altitude miscompare. </t>
+  </si>
+  <si>
+    <t>SFD IAS MISCOMPARE </t>
+  </si>
+  <si>
+    <t>SFD airspeed miscompare. </t>
+  </si>
+  <si>
+    <t>SFD PITCH MISCOMPARE </t>
+  </si>
+  <si>
+    <t>SFD pitch miscompare. </t>
+  </si>
+  <si>
+    <t>SFD ROLL MISCOMPARE </t>
+  </si>
+  <si>
+    <t>SFD roll miscompare. </t>
+  </si>
+  <si>
+    <t>AOA/stall warning input invalid. </t>
+  </si>
+  <si>
+    <t>TAKEOFF FLAPS </t>
+  </si>
+  <si>
+    <t>ALTITUDE SEL </t>
+  </si>
+  <si>
+    <t>Climbing away from selected altitude. </t>
+  </si>
+  <si>
+    <t>Descending away from selected altitude. </t>
+  </si>
+  <si>
+    <t>AOA FAIL2 </t>
+  </si>
+  <si>
+    <t>Dynamic stall speed band is unavailable. </t>
+  </si>
+  <si>
+    <t>ARE YOU ALERT? </t>
+  </si>
+  <si>
+    <t>Are you alert? </t>
+  </si>
+  <si>
+    <t>CHECK OXYGEN1 </t>
+  </si>
+  <si>
+    <t>Check oxygen system status. </t>
+  </si>
+  <si>
+    <t>COURSE SELECT1 </t>
+  </si>
+  <si>
+    <t>Current track will not intercept selected course. </t>
+  </si>
+  <si>
+    <t>ECS RECIRC ON </t>
+  </si>
+  <si>
+    <t>ECS recirculation mode is prohibited in flight. </t>
+  </si>
+  <si>
+    <t>ESP CONFIG </t>
+  </si>
+  <si>
+    <t>ESP config error. Config service req'd. </t>
+  </si>
+  <si>
+    <t>EXIT ICING2 1 </t>
+  </si>
+  <si>
+    <t>Exit icing conditions. </t>
+  </si>
+  <si>
+    <t>FAILED PATH </t>
+  </si>
+  <si>
+    <t>An autopilot servo data path has failed. </t>
+  </si>
+  <si>
+    <t>FLAPS CLIMB </t>
+  </si>
+  <si>
+    <t>Flaps not set for enroute climb. </t>
+  </si>
+  <si>
+    <t>FUEL VALVE OFF </t>
+  </si>
+  <si>
+    <t>Fuel valve is in the off position. </t>
+  </si>
+  <si>
+    <t>IPS FLUID LOW2 </t>
+  </si>
+  <si>
+    <t>IPS PUMP BACKUP3 </t>
+  </si>
+  <si>
+    <t>IPS backup pump mode has been selected. </t>
+  </si>
+  <si>
+    <t>OXYGEN ON1 </t>
+  </si>
+  <si>
+    <t>Oxygen system is left on after shutdown. </t>
+  </si>
+  <si>
+    <t>ROL MODE </t>
+  </si>
+  <si>
+    <t>Roll mode is active. </t>
+  </si>
+  <si>
+    <t>SFC WATCH FAIL </t>
+  </si>
+  <si>
+    <t>SurfaceWatch failed. </t>
+  </si>
+  <si>
+    <t>SFC WATCH INHIB </t>
+  </si>
+  <si>
+    <t>SurfaceWatch inhibited. </t>
+  </si>
+  <si>
+    <t>SFD NO COMPARE </t>
+  </si>
+  <si>
+    <t>SFD comparison data missing. </t>
+  </si>
+  <si>
+    <t>VNAV ALT SEL </t>
+  </si>
+  <si>
+    <t>VNAV needs lower ALT SEL to capture VPATH. </t>
+  </si>
+  <si>
+    <t>VNAV NOT ARMED </t>
+  </si>
+  <si>
+    <t>Press VNV to arm VPATH capture. </t>
+  </si>
+  <si>
+    <t>normal</t>
   </si>
 </sst>
 </file>
@@ -850,10 +1285,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B50ED21-1FB3-1647-9374-5C9653EBF4CC}">
-  <dimension ref="A1:H85"/>
+  <dimension ref="A1:H206"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A177" workbookViewId="0">
+      <selection activeCell="D169" sqref="D169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2909,7 +3344,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>80</v>
       </c>
@@ -2932,7 +3367,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
@@ -2955,7 +3390,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>82</v>
       </c>
@@ -2978,7 +3413,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>83</v>
       </c>
@@ -3001,7 +3436,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>84</v>
       </c>
@@ -3021,6 +3456,3122 @@
         <v>47</v>
       </c>
       <c r="G85" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>100</v>
+      </c>
+      <c r="B86" t="s">
+        <v>56</v>
+      </c>
+      <c r="C86" t="s">
+        <v>54</v>
+      </c>
+      <c r="D86" t="s">
+        <v>60</v>
+      </c>
+      <c r="E86" t="s">
+        <v>61</v>
+      </c>
+      <c r="F86" t="s">
+        <v>144</v>
+      </c>
+      <c r="G86" t="s">
+        <v>181</v>
+      </c>
+      <c r="H86" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>101</v>
+      </c>
+      <c r="B87" t="s">
+        <v>56</v>
+      </c>
+      <c r="C87" t="s">
+        <v>54</v>
+      </c>
+      <c r="D87" t="s">
+        <v>60</v>
+      </c>
+      <c r="E87" t="s">
+        <v>61</v>
+      </c>
+      <c r="F87" t="s">
+        <v>144</v>
+      </c>
+      <c r="G87" t="s">
+        <v>145</v>
+      </c>
+      <c r="H87" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>102</v>
+      </c>
+      <c r="B88" t="s">
+        <v>56</v>
+      </c>
+      <c r="C88" t="s">
+        <v>54</v>
+      </c>
+      <c r="D88" t="s">
+        <v>60</v>
+      </c>
+      <c r="E88" t="s">
+        <v>61</v>
+      </c>
+      <c r="F88" t="s">
+        <v>144</v>
+      </c>
+      <c r="G88" t="s">
+        <v>147</v>
+      </c>
+      <c r="H88" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>103</v>
+      </c>
+      <c r="B89" t="s">
+        <v>56</v>
+      </c>
+      <c r="C89" t="s">
+        <v>54</v>
+      </c>
+      <c r="D89" t="s">
+        <v>60</v>
+      </c>
+      <c r="E89" t="s">
+        <v>61</v>
+      </c>
+      <c r="F89" t="s">
+        <v>144</v>
+      </c>
+      <c r="G89" t="s">
+        <v>147</v>
+      </c>
+      <c r="H89" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>104</v>
+      </c>
+      <c r="B90" t="s">
+        <v>56</v>
+      </c>
+      <c r="C90" t="s">
+        <v>54</v>
+      </c>
+      <c r="D90" t="s">
+        <v>60</v>
+      </c>
+      <c r="E90" t="s">
+        <v>61</v>
+      </c>
+      <c r="F90" t="s">
+        <v>144</v>
+      </c>
+      <c r="G90" t="s">
+        <v>147</v>
+      </c>
+      <c r="H90" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>105</v>
+      </c>
+      <c r="B91" t="s">
+        <v>56</v>
+      </c>
+      <c r="C91" t="s">
+        <v>54</v>
+      </c>
+      <c r="D91" t="s">
+        <v>60</v>
+      </c>
+      <c r="E91" t="s">
+        <v>61</v>
+      </c>
+      <c r="F91" t="s">
+        <v>144</v>
+      </c>
+      <c r="G91" t="s">
+        <v>147</v>
+      </c>
+      <c r="H91" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>106</v>
+      </c>
+      <c r="B92" t="s">
+        <v>56</v>
+      </c>
+      <c r="C92" t="s">
+        <v>54</v>
+      </c>
+      <c r="D92" t="s">
+        <v>60</v>
+      </c>
+      <c r="E92" t="s">
+        <v>61</v>
+      </c>
+      <c r="F92" t="s">
+        <v>144</v>
+      </c>
+      <c r="G92" t="s">
+        <v>78</v>
+      </c>
+      <c r="H92" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>107</v>
+      </c>
+      <c r="B93" t="s">
+        <v>56</v>
+      </c>
+      <c r="C93" t="s">
+        <v>54</v>
+      </c>
+      <c r="D93" t="s">
+        <v>60</v>
+      </c>
+      <c r="E93" t="s">
+        <v>61</v>
+      </c>
+      <c r="F93" t="s">
+        <v>144</v>
+      </c>
+      <c r="G93" t="s">
+        <v>152</v>
+      </c>
+      <c r="H93" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>108</v>
+      </c>
+      <c r="B94" t="s">
+        <v>56</v>
+      </c>
+      <c r="C94" t="s">
+        <v>54</v>
+      </c>
+      <c r="D94" t="s">
+        <v>60</v>
+      </c>
+      <c r="E94" t="s">
+        <v>61</v>
+      </c>
+      <c r="F94" t="s">
+        <v>144</v>
+      </c>
+      <c r="G94" t="s">
+        <v>153</v>
+      </c>
+      <c r="H94" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>109</v>
+      </c>
+      <c r="B95" t="s">
+        <v>56</v>
+      </c>
+      <c r="C95" t="s">
+        <v>54</v>
+      </c>
+      <c r="D95" t="s">
+        <v>60</v>
+      </c>
+      <c r="E95" t="s">
+        <v>61</v>
+      </c>
+      <c r="F95" t="s">
+        <v>144</v>
+      </c>
+      <c r="G95" t="s">
+        <v>182</v>
+      </c>
+      <c r="H95" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>110</v>
+      </c>
+      <c r="B96" t="s">
+        <v>56</v>
+      </c>
+      <c r="C96" t="s">
+        <v>54</v>
+      </c>
+      <c r="D96" t="s">
+        <v>60</v>
+      </c>
+      <c r="E96" t="s">
+        <v>61</v>
+      </c>
+      <c r="F96" t="s">
+        <v>144</v>
+      </c>
+      <c r="G96" t="s">
+        <v>155</v>
+      </c>
+      <c r="H96" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>111</v>
+      </c>
+      <c r="B97" t="s">
+        <v>56</v>
+      </c>
+      <c r="C97" t="s">
+        <v>54</v>
+      </c>
+      <c r="D97" t="s">
+        <v>60</v>
+      </c>
+      <c r="E97" t="s">
+        <v>61</v>
+      </c>
+      <c r="F97" t="s">
+        <v>144</v>
+      </c>
+      <c r="G97" t="s">
+        <v>156</v>
+      </c>
+      <c r="H97" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>112</v>
+      </c>
+      <c r="B98" t="s">
+        <v>56</v>
+      </c>
+      <c r="C98" t="s">
+        <v>54</v>
+      </c>
+      <c r="D98" t="s">
+        <v>60</v>
+      </c>
+      <c r="E98" t="s">
+        <v>61</v>
+      </c>
+      <c r="F98" t="s">
+        <v>144</v>
+      </c>
+      <c r="G98" t="s">
+        <v>157</v>
+      </c>
+      <c r="H98" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>113</v>
+      </c>
+      <c r="B99" t="s">
+        <v>56</v>
+      </c>
+      <c r="C99" t="s">
+        <v>54</v>
+      </c>
+      <c r="D99" t="s">
+        <v>60</v>
+      </c>
+      <c r="E99" t="s">
+        <v>61</v>
+      </c>
+      <c r="F99" t="s">
+        <v>144</v>
+      </c>
+      <c r="G99" t="s">
+        <v>159</v>
+      </c>
+      <c r="H99" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>114</v>
+      </c>
+      <c r="B100" t="s">
+        <v>56</v>
+      </c>
+      <c r="C100" t="s">
+        <v>54</v>
+      </c>
+      <c r="D100" t="s">
+        <v>60</v>
+      </c>
+      <c r="E100" t="s">
+        <v>61</v>
+      </c>
+      <c r="F100" t="s">
+        <v>144</v>
+      </c>
+      <c r="G100" t="s">
+        <v>161</v>
+      </c>
+      <c r="H100" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>115</v>
+      </c>
+      <c r="B101" t="s">
+        <v>56</v>
+      </c>
+      <c r="C101" t="s">
+        <v>54</v>
+      </c>
+      <c r="D101" t="s">
+        <v>60</v>
+      </c>
+      <c r="E101" t="s">
+        <v>61</v>
+      </c>
+      <c r="F101" t="s">
+        <v>144</v>
+      </c>
+      <c r="G101" t="s">
+        <v>162</v>
+      </c>
+      <c r="H101" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>116</v>
+      </c>
+      <c r="B102" t="s">
+        <v>56</v>
+      </c>
+      <c r="C102" t="s">
+        <v>54</v>
+      </c>
+      <c r="D102" t="s">
+        <v>60</v>
+      </c>
+      <c r="E102" t="s">
+        <v>61</v>
+      </c>
+      <c r="F102" t="s">
+        <v>144</v>
+      </c>
+      <c r="G102" t="s">
+        <v>164</v>
+      </c>
+      <c r="H102" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>117</v>
+      </c>
+      <c r="B103" t="s">
+        <v>56</v>
+      </c>
+      <c r="C103" t="s">
+        <v>54</v>
+      </c>
+      <c r="D103" t="s">
+        <v>60</v>
+      </c>
+      <c r="E103" t="s">
+        <v>61</v>
+      </c>
+      <c r="F103" t="s">
+        <v>144</v>
+      </c>
+      <c r="G103" t="s">
+        <v>166</v>
+      </c>
+      <c r="H103" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>118</v>
+      </c>
+      <c r="B104" t="s">
+        <v>56</v>
+      </c>
+      <c r="C104" t="s">
+        <v>54</v>
+      </c>
+      <c r="D104" t="s">
+        <v>60</v>
+      </c>
+      <c r="E104" t="s">
+        <v>61</v>
+      </c>
+      <c r="F104" t="s">
+        <v>144</v>
+      </c>
+      <c r="G104" t="s">
+        <v>168</v>
+      </c>
+      <c r="H104" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>119</v>
+      </c>
+      <c r="B105" t="s">
+        <v>56</v>
+      </c>
+      <c r="C105" t="s">
+        <v>54</v>
+      </c>
+      <c r="D105" t="s">
+        <v>60</v>
+      </c>
+      <c r="E105" t="s">
+        <v>61</v>
+      </c>
+      <c r="F105" t="s">
+        <v>144</v>
+      </c>
+      <c r="G105" t="s">
+        <v>169</v>
+      </c>
+      <c r="H105" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>120</v>
+      </c>
+      <c r="B106" t="s">
+        <v>56</v>
+      </c>
+      <c r="C106" t="s">
+        <v>54</v>
+      </c>
+      <c r="D106" t="s">
+        <v>60</v>
+      </c>
+      <c r="E106" t="s">
+        <v>61</v>
+      </c>
+      <c r="F106" t="s">
+        <v>144</v>
+      </c>
+      <c r="G106" t="s">
+        <v>170</v>
+      </c>
+      <c r="H106" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>121</v>
+      </c>
+      <c r="B107" t="s">
+        <v>56</v>
+      </c>
+      <c r="C107" t="s">
+        <v>54</v>
+      </c>
+      <c r="D107" t="s">
+        <v>60</v>
+      </c>
+      <c r="E107" t="s">
+        <v>61</v>
+      </c>
+      <c r="F107" t="s">
+        <v>144</v>
+      </c>
+      <c r="G107" t="s">
+        <v>171</v>
+      </c>
+      <c r="H107" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>122</v>
+      </c>
+      <c r="B108" t="s">
+        <v>56</v>
+      </c>
+      <c r="C108" t="s">
+        <v>54</v>
+      </c>
+      <c r="D108" t="s">
+        <v>60</v>
+      </c>
+      <c r="E108" t="s">
+        <v>61</v>
+      </c>
+      <c r="F108" t="s">
+        <v>144</v>
+      </c>
+      <c r="G108" t="s">
+        <v>172</v>
+      </c>
+      <c r="H108" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>123</v>
+      </c>
+      <c r="B109" t="s">
+        <v>56</v>
+      </c>
+      <c r="C109" t="s">
+        <v>54</v>
+      </c>
+      <c r="D109" t="s">
+        <v>60</v>
+      </c>
+      <c r="E109" t="s">
+        <v>61</v>
+      </c>
+      <c r="F109" t="s">
+        <v>144</v>
+      </c>
+      <c r="G109" t="s">
+        <v>183</v>
+      </c>
+      <c r="H109" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>124</v>
+      </c>
+      <c r="B110" t="s">
+        <v>56</v>
+      </c>
+      <c r="C110" t="s">
+        <v>54</v>
+      </c>
+      <c r="D110" t="s">
+        <v>60</v>
+      </c>
+      <c r="E110" t="s">
+        <v>61</v>
+      </c>
+      <c r="F110" t="s">
+        <v>144</v>
+      </c>
+      <c r="G110" t="s">
+        <v>184</v>
+      </c>
+      <c r="H110" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>125</v>
+      </c>
+      <c r="B111" t="s">
+        <v>56</v>
+      </c>
+      <c r="C111" t="s">
+        <v>54</v>
+      </c>
+      <c r="D111" t="s">
+        <v>60</v>
+      </c>
+      <c r="E111" t="s">
+        <v>61</v>
+      </c>
+      <c r="F111" t="s">
+        <v>144</v>
+      </c>
+      <c r="G111" t="s">
+        <v>185</v>
+      </c>
+      <c r="H111" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>126</v>
+      </c>
+      <c r="B112" t="s">
+        <v>56</v>
+      </c>
+      <c r="C112" t="s">
+        <v>54</v>
+      </c>
+      <c r="D112" t="s">
+        <v>60</v>
+      </c>
+      <c r="E112" t="s">
+        <v>61</v>
+      </c>
+      <c r="F112" t="s">
+        <v>144</v>
+      </c>
+      <c r="G112" t="s">
+        <v>173</v>
+      </c>
+      <c r="H112" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>127</v>
+      </c>
+      <c r="B113" t="s">
+        <v>56</v>
+      </c>
+      <c r="C113" t="s">
+        <v>54</v>
+      </c>
+      <c r="D113" t="s">
+        <v>60</v>
+      </c>
+      <c r="E113" t="s">
+        <v>61</v>
+      </c>
+      <c r="F113" t="s">
+        <v>144</v>
+      </c>
+      <c r="G113" t="s">
+        <v>174</v>
+      </c>
+      <c r="H113" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>128</v>
+      </c>
+      <c r="B114" t="s">
+        <v>56</v>
+      </c>
+      <c r="C114" t="s">
+        <v>54</v>
+      </c>
+      <c r="D114" t="s">
+        <v>60</v>
+      </c>
+      <c r="E114" t="s">
+        <v>61</v>
+      </c>
+      <c r="F114" t="s">
+        <v>144</v>
+      </c>
+      <c r="G114" t="s">
+        <v>175</v>
+      </c>
+      <c r="H114" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>129</v>
+      </c>
+      <c r="B115" t="s">
+        <v>56</v>
+      </c>
+      <c r="C115" t="s">
+        <v>54</v>
+      </c>
+      <c r="D115" t="s">
+        <v>60</v>
+      </c>
+      <c r="E115" t="s">
+        <v>61</v>
+      </c>
+      <c r="F115" t="s">
+        <v>144</v>
+      </c>
+      <c r="G115" t="s">
+        <v>177</v>
+      </c>
+      <c r="H115" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>130</v>
+      </c>
+      <c r="B116" t="s">
+        <v>56</v>
+      </c>
+      <c r="C116" t="s">
+        <v>54</v>
+      </c>
+      <c r="D116" t="s">
+        <v>60</v>
+      </c>
+      <c r="E116" t="s">
+        <v>61</v>
+      </c>
+      <c r="F116" t="s">
+        <v>144</v>
+      </c>
+      <c r="G116" t="s">
+        <v>179</v>
+      </c>
+      <c r="H116" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>131</v>
+      </c>
+      <c r="B117" t="s">
+        <v>56</v>
+      </c>
+      <c r="C117" t="s">
+        <v>54</v>
+      </c>
+      <c r="D117" t="s">
+        <v>60</v>
+      </c>
+      <c r="E117" t="s">
+        <v>61</v>
+      </c>
+      <c r="F117" t="s">
+        <v>144</v>
+      </c>
+      <c r="G117" t="s">
+        <v>186</v>
+      </c>
+      <c r="H117" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>132</v>
+      </c>
+      <c r="B118" t="s">
+        <v>55</v>
+      </c>
+      <c r="C118" t="s">
+        <v>54</v>
+      </c>
+      <c r="D118" t="s">
+        <v>60</v>
+      </c>
+      <c r="E118" t="s">
+        <v>63</v>
+      </c>
+      <c r="F118" t="s">
+        <v>144</v>
+      </c>
+      <c r="G118" t="s">
+        <v>187</v>
+      </c>
+      <c r="H118" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>133</v>
+      </c>
+      <c r="B119" t="s">
+        <v>55</v>
+      </c>
+      <c r="C119" t="s">
+        <v>54</v>
+      </c>
+      <c r="D119" t="s">
+        <v>60</v>
+      </c>
+      <c r="E119" t="s">
+        <v>63</v>
+      </c>
+      <c r="F119" t="s">
+        <v>144</v>
+      </c>
+      <c r="G119" t="s">
+        <v>188</v>
+      </c>
+      <c r="H119" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>134</v>
+      </c>
+      <c r="B120" t="s">
+        <v>55</v>
+      </c>
+      <c r="C120" t="s">
+        <v>54</v>
+      </c>
+      <c r="D120" t="s">
+        <v>60</v>
+      </c>
+      <c r="E120" t="s">
+        <v>63</v>
+      </c>
+      <c r="F120" t="s">
+        <v>144</v>
+      </c>
+      <c r="G120" t="s">
+        <v>189</v>
+      </c>
+      <c r="H120" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>135</v>
+      </c>
+      <c r="B121" t="s">
+        <v>55</v>
+      </c>
+      <c r="C121" t="s">
+        <v>54</v>
+      </c>
+      <c r="D121" t="s">
+        <v>60</v>
+      </c>
+      <c r="E121" t="s">
+        <v>63</v>
+      </c>
+      <c r="F121" t="s">
+        <v>144</v>
+      </c>
+      <c r="G121" t="s">
+        <v>190</v>
+      </c>
+      <c r="H121" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>136</v>
+      </c>
+      <c r="B122" t="s">
+        <v>55</v>
+      </c>
+      <c r="C122" t="s">
+        <v>54</v>
+      </c>
+      <c r="D122" t="s">
+        <v>60</v>
+      </c>
+      <c r="E122" t="s">
+        <v>63</v>
+      </c>
+      <c r="F122" t="s">
+        <v>144</v>
+      </c>
+      <c r="G122" t="s">
+        <v>192</v>
+      </c>
+      <c r="H122" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>137</v>
+      </c>
+      <c r="B123" t="s">
+        <v>55</v>
+      </c>
+      <c r="C123" t="s">
+        <v>54</v>
+      </c>
+      <c r="D123" t="s">
+        <v>60</v>
+      </c>
+      <c r="E123" t="s">
+        <v>63</v>
+      </c>
+      <c r="F123" t="s">
+        <v>144</v>
+      </c>
+      <c r="G123" t="s">
+        <v>193</v>
+      </c>
+      <c r="H123" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>138</v>
+      </c>
+      <c r="B124" t="s">
+        <v>55</v>
+      </c>
+      <c r="C124" t="s">
+        <v>54</v>
+      </c>
+      <c r="D124" t="s">
+        <v>60</v>
+      </c>
+      <c r="E124" t="s">
+        <v>63</v>
+      </c>
+      <c r="F124" t="s">
+        <v>144</v>
+      </c>
+      <c r="G124" t="s">
+        <v>194</v>
+      </c>
+      <c r="H124" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>139</v>
+      </c>
+      <c r="B125" t="s">
+        <v>55</v>
+      </c>
+      <c r="C125" t="s">
+        <v>54</v>
+      </c>
+      <c r="D125" t="s">
+        <v>60</v>
+      </c>
+      <c r="E125" t="s">
+        <v>63</v>
+      </c>
+      <c r="F125" t="s">
+        <v>144</v>
+      </c>
+      <c r="G125" t="s">
+        <v>195</v>
+      </c>
+      <c r="H125" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>140</v>
+      </c>
+      <c r="B126" t="s">
+        <v>55</v>
+      </c>
+      <c r="C126" t="s">
+        <v>54</v>
+      </c>
+      <c r="D126" t="s">
+        <v>60</v>
+      </c>
+      <c r="E126" t="s">
+        <v>63</v>
+      </c>
+      <c r="F126" t="s">
+        <v>144</v>
+      </c>
+      <c r="G126" t="s">
+        <v>196</v>
+      </c>
+      <c r="H126" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>141</v>
+      </c>
+      <c r="B127" t="s">
+        <v>55</v>
+      </c>
+      <c r="C127" t="s">
+        <v>54</v>
+      </c>
+      <c r="D127" t="s">
+        <v>60</v>
+      </c>
+      <c r="E127" t="s">
+        <v>63</v>
+      </c>
+      <c r="F127" t="s">
+        <v>144</v>
+      </c>
+      <c r="G127" t="s">
+        <v>198</v>
+      </c>
+      <c r="H127" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>142</v>
+      </c>
+      <c r="B128" t="s">
+        <v>55</v>
+      </c>
+      <c r="C128" t="s">
+        <v>54</v>
+      </c>
+      <c r="D128" t="s">
+        <v>60</v>
+      </c>
+      <c r="E128" t="s">
+        <v>63</v>
+      </c>
+      <c r="F128" t="s">
+        <v>144</v>
+      </c>
+      <c r="G128" t="s">
+        <v>200</v>
+      </c>
+      <c r="H128" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>143</v>
+      </c>
+      <c r="B129" t="s">
+        <v>55</v>
+      </c>
+      <c r="C129" t="s">
+        <v>54</v>
+      </c>
+      <c r="D129" t="s">
+        <v>60</v>
+      </c>
+      <c r="E129" t="s">
+        <v>63</v>
+      </c>
+      <c r="F129" t="s">
+        <v>144</v>
+      </c>
+      <c r="G129" t="s">
+        <v>78</v>
+      </c>
+      <c r="H129" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>144</v>
+      </c>
+      <c r="B130" t="s">
+        <v>55</v>
+      </c>
+      <c r="C130" t="s">
+        <v>54</v>
+      </c>
+      <c r="D130" t="s">
+        <v>60</v>
+      </c>
+      <c r="E130" t="s">
+        <v>63</v>
+      </c>
+      <c r="F130" t="s">
+        <v>144</v>
+      </c>
+      <c r="G130" t="s">
+        <v>202</v>
+      </c>
+      <c r="H130" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>145</v>
+      </c>
+      <c r="B131" t="s">
+        <v>55</v>
+      </c>
+      <c r="C131" t="s">
+        <v>54</v>
+      </c>
+      <c r="D131" t="s">
+        <v>60</v>
+      </c>
+      <c r="E131" t="s">
+        <v>63</v>
+      </c>
+      <c r="F131" t="s">
+        <v>144</v>
+      </c>
+      <c r="G131" t="s">
+        <v>204</v>
+      </c>
+      <c r="H131" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>146</v>
+      </c>
+      <c r="B132" t="s">
+        <v>55</v>
+      </c>
+      <c r="C132" t="s">
+        <v>54</v>
+      </c>
+      <c r="D132" t="s">
+        <v>60</v>
+      </c>
+      <c r="E132" t="s">
+        <v>63</v>
+      </c>
+      <c r="F132" t="s">
+        <v>144</v>
+      </c>
+      <c r="G132" t="s">
+        <v>206</v>
+      </c>
+      <c r="H132" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>147</v>
+      </c>
+      <c r="B133" t="s">
+        <v>55</v>
+      </c>
+      <c r="C133" t="s">
+        <v>54</v>
+      </c>
+      <c r="D133" t="s">
+        <v>60</v>
+      </c>
+      <c r="E133" t="s">
+        <v>63</v>
+      </c>
+      <c r="F133" t="s">
+        <v>144</v>
+      </c>
+      <c r="G133" t="s">
+        <v>207</v>
+      </c>
+      <c r="H133" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>148</v>
+      </c>
+      <c r="B134" t="s">
+        <v>55</v>
+      </c>
+      <c r="C134" t="s">
+        <v>54</v>
+      </c>
+      <c r="D134" t="s">
+        <v>60</v>
+      </c>
+      <c r="E134" t="s">
+        <v>63</v>
+      </c>
+      <c r="F134" t="s">
+        <v>144</v>
+      </c>
+      <c r="G134" t="s">
+        <v>156</v>
+      </c>
+      <c r="H134" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>149</v>
+      </c>
+      <c r="B135" t="s">
+        <v>55</v>
+      </c>
+      <c r="C135" t="s">
+        <v>54</v>
+      </c>
+      <c r="D135" t="s">
+        <v>60</v>
+      </c>
+      <c r="E135" t="s">
+        <v>63</v>
+      </c>
+      <c r="F135" t="s">
+        <v>144</v>
+      </c>
+      <c r="G135" t="s">
+        <v>161</v>
+      </c>
+      <c r="H135" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>150</v>
+      </c>
+      <c r="B136" t="s">
+        <v>55</v>
+      </c>
+      <c r="C136" t="s">
+        <v>54</v>
+      </c>
+      <c r="D136" t="s">
+        <v>60</v>
+      </c>
+      <c r="E136" t="s">
+        <v>63</v>
+      </c>
+      <c r="F136" t="s">
+        <v>144</v>
+      </c>
+      <c r="G136" t="s">
+        <v>208</v>
+      </c>
+      <c r="H136" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>151</v>
+      </c>
+      <c r="B137" t="s">
+        <v>55</v>
+      </c>
+      <c r="C137" t="s">
+        <v>54</v>
+      </c>
+      <c r="D137" t="s">
+        <v>60</v>
+      </c>
+      <c r="E137" t="s">
+        <v>63</v>
+      </c>
+      <c r="F137" t="s">
+        <v>144</v>
+      </c>
+      <c r="G137" t="s">
+        <v>210</v>
+      </c>
+      <c r="H137" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>152</v>
+      </c>
+      <c r="B138" t="s">
+        <v>55</v>
+      </c>
+      <c r="C138" t="s">
+        <v>54</v>
+      </c>
+      <c r="D138" t="s">
+        <v>60</v>
+      </c>
+      <c r="E138" t="s">
+        <v>63</v>
+      </c>
+      <c r="F138" t="s">
+        <v>144</v>
+      </c>
+      <c r="G138" t="s">
+        <v>212</v>
+      </c>
+      <c r="H138" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>153</v>
+      </c>
+      <c r="B139" t="s">
+        <v>55</v>
+      </c>
+      <c r="C139" t="s">
+        <v>54</v>
+      </c>
+      <c r="D139" t="s">
+        <v>60</v>
+      </c>
+      <c r="E139" t="s">
+        <v>63</v>
+      </c>
+      <c r="F139" t="s">
+        <v>144</v>
+      </c>
+      <c r="G139" t="s">
+        <v>214</v>
+      </c>
+      <c r="H139" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>154</v>
+      </c>
+      <c r="B140" t="s">
+        <v>55</v>
+      </c>
+      <c r="C140" t="s">
+        <v>54</v>
+      </c>
+      <c r="D140" t="s">
+        <v>60</v>
+      </c>
+      <c r="E140" t="s">
+        <v>63</v>
+      </c>
+      <c r="F140" t="s">
+        <v>144</v>
+      </c>
+      <c r="G140" t="s">
+        <v>216</v>
+      </c>
+      <c r="H140" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>155</v>
+      </c>
+      <c r="B141" t="s">
+        <v>55</v>
+      </c>
+      <c r="C141" t="s">
+        <v>54</v>
+      </c>
+      <c r="D141" t="s">
+        <v>60</v>
+      </c>
+      <c r="E141" t="s">
+        <v>63</v>
+      </c>
+      <c r="F141" t="s">
+        <v>144</v>
+      </c>
+      <c r="G141" t="s">
+        <v>217</v>
+      </c>
+      <c r="H141" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>156</v>
+      </c>
+      <c r="B142" t="s">
+        <v>55</v>
+      </c>
+      <c r="C142" t="s">
+        <v>54</v>
+      </c>
+      <c r="D142" t="s">
+        <v>60</v>
+      </c>
+      <c r="E142" t="s">
+        <v>63</v>
+      </c>
+      <c r="F142" t="s">
+        <v>144</v>
+      </c>
+      <c r="G142" t="s">
+        <v>219</v>
+      </c>
+      <c r="H142" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>157</v>
+      </c>
+      <c r="B143" t="s">
+        <v>55</v>
+      </c>
+      <c r="C143" t="s">
+        <v>54</v>
+      </c>
+      <c r="D143" t="s">
+        <v>60</v>
+      </c>
+      <c r="E143" t="s">
+        <v>63</v>
+      </c>
+      <c r="F143" t="s">
+        <v>144</v>
+      </c>
+      <c r="G143" t="s">
+        <v>221</v>
+      </c>
+      <c r="H143" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>158</v>
+      </c>
+      <c r="B144" t="s">
+        <v>55</v>
+      </c>
+      <c r="C144" t="s">
+        <v>54</v>
+      </c>
+      <c r="D144" t="s">
+        <v>60</v>
+      </c>
+      <c r="E144" t="s">
+        <v>63</v>
+      </c>
+      <c r="F144" t="s">
+        <v>144</v>
+      </c>
+      <c r="G144" t="s">
+        <v>223</v>
+      </c>
+      <c r="H144" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>159</v>
+      </c>
+      <c r="B145" t="s">
+        <v>55</v>
+      </c>
+      <c r="C145" t="s">
+        <v>54</v>
+      </c>
+      <c r="D145" t="s">
+        <v>60</v>
+      </c>
+      <c r="E145" t="s">
+        <v>63</v>
+      </c>
+      <c r="F145" t="s">
+        <v>144</v>
+      </c>
+      <c r="G145" t="s">
+        <v>223</v>
+      </c>
+      <c r="H145" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A146">
+        <v>160</v>
+      </c>
+      <c r="B146" t="s">
+        <v>55</v>
+      </c>
+      <c r="C146" t="s">
+        <v>54</v>
+      </c>
+      <c r="D146" t="s">
+        <v>60</v>
+      </c>
+      <c r="E146" t="s">
+        <v>63</v>
+      </c>
+      <c r="F146" t="s">
+        <v>144</v>
+      </c>
+      <c r="G146" t="s">
+        <v>226</v>
+      </c>
+      <c r="H146" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <v>161</v>
+      </c>
+      <c r="B147" t="s">
+        <v>55</v>
+      </c>
+      <c r="C147" t="s">
+        <v>54</v>
+      </c>
+      <c r="D147" t="s">
+        <v>60</v>
+      </c>
+      <c r="E147" t="s">
+        <v>63</v>
+      </c>
+      <c r="F147" t="s">
+        <v>144</v>
+      </c>
+      <c r="G147" t="s">
+        <v>228</v>
+      </c>
+      <c r="H147" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A148">
+        <v>162</v>
+      </c>
+      <c r="B148" t="s">
+        <v>55</v>
+      </c>
+      <c r="C148" t="s">
+        <v>54</v>
+      </c>
+      <c r="D148" t="s">
+        <v>60</v>
+      </c>
+      <c r="E148" t="s">
+        <v>63</v>
+      </c>
+      <c r="F148" t="s">
+        <v>144</v>
+      </c>
+      <c r="G148" t="s">
+        <v>230</v>
+      </c>
+      <c r="H148" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A149">
+        <v>163</v>
+      </c>
+      <c r="B149" t="s">
+        <v>55</v>
+      </c>
+      <c r="C149" t="s">
+        <v>54</v>
+      </c>
+      <c r="D149" t="s">
+        <v>60</v>
+      </c>
+      <c r="E149" t="s">
+        <v>63</v>
+      </c>
+      <c r="F149" t="s">
+        <v>144</v>
+      </c>
+      <c r="G149" t="s">
+        <v>168</v>
+      </c>
+      <c r="H149" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A150">
+        <v>164</v>
+      </c>
+      <c r="B150" t="s">
+        <v>55</v>
+      </c>
+      <c r="C150" t="s">
+        <v>54</v>
+      </c>
+      <c r="D150" t="s">
+        <v>60</v>
+      </c>
+      <c r="E150" t="s">
+        <v>63</v>
+      </c>
+      <c r="F150" t="s">
+        <v>144</v>
+      </c>
+      <c r="G150" t="s">
+        <v>169</v>
+      </c>
+      <c r="H150" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A151">
+        <v>165</v>
+      </c>
+      <c r="B151" t="s">
+        <v>55</v>
+      </c>
+      <c r="C151" t="s">
+        <v>54</v>
+      </c>
+      <c r="D151" t="s">
+        <v>60</v>
+      </c>
+      <c r="E151" t="s">
+        <v>63</v>
+      </c>
+      <c r="F151" t="s">
+        <v>144</v>
+      </c>
+      <c r="G151" t="s">
+        <v>170</v>
+      </c>
+      <c r="H151" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A152">
+        <v>166</v>
+      </c>
+      <c r="B152" t="s">
+        <v>55</v>
+      </c>
+      <c r="C152" t="s">
+        <v>54</v>
+      </c>
+      <c r="D152" t="s">
+        <v>60</v>
+      </c>
+      <c r="E152" t="s">
+        <v>63</v>
+      </c>
+      <c r="F152" t="s">
+        <v>144</v>
+      </c>
+      <c r="G152" t="s">
+        <v>232</v>
+      </c>
+      <c r="H152" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A153">
+        <v>167</v>
+      </c>
+      <c r="B153" t="s">
+        <v>55</v>
+      </c>
+      <c r="C153" t="s">
+        <v>54</v>
+      </c>
+      <c r="D153" t="s">
+        <v>60</v>
+      </c>
+      <c r="E153" t="s">
+        <v>63</v>
+      </c>
+      <c r="F153" t="s">
+        <v>144</v>
+      </c>
+      <c r="G153" t="s">
+        <v>233</v>
+      </c>
+      <c r="H153" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A154">
+        <v>168</v>
+      </c>
+      <c r="B154" t="s">
+        <v>55</v>
+      </c>
+      <c r="C154" t="s">
+        <v>54</v>
+      </c>
+      <c r="D154" t="s">
+        <v>60</v>
+      </c>
+      <c r="E154" t="s">
+        <v>63</v>
+      </c>
+      <c r="F154" t="s">
+        <v>144</v>
+      </c>
+      <c r="G154" t="s">
+        <v>171</v>
+      </c>
+      <c r="H154" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A155">
+        <v>169</v>
+      </c>
+      <c r="B155" t="s">
+        <v>55</v>
+      </c>
+      <c r="C155" t="s">
+        <v>54</v>
+      </c>
+      <c r="D155" t="s">
+        <v>60</v>
+      </c>
+      <c r="E155" t="s">
+        <v>63</v>
+      </c>
+      <c r="F155" t="s">
+        <v>144</v>
+      </c>
+      <c r="G155" t="s">
+        <v>172</v>
+      </c>
+      <c r="H155" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A156">
+        <v>170</v>
+      </c>
+      <c r="B156" t="s">
+        <v>55</v>
+      </c>
+      <c r="C156" t="s">
+        <v>54</v>
+      </c>
+      <c r="D156" t="s">
+        <v>60</v>
+      </c>
+      <c r="E156" t="s">
+        <v>63</v>
+      </c>
+      <c r="F156" t="s">
+        <v>144</v>
+      </c>
+      <c r="G156" t="s">
+        <v>184</v>
+      </c>
+      <c r="H156" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A157">
+        <v>171</v>
+      </c>
+      <c r="B157" t="s">
+        <v>55</v>
+      </c>
+      <c r="C157" t="s">
+        <v>54</v>
+      </c>
+      <c r="D157" t="s">
+        <v>60</v>
+      </c>
+      <c r="E157" t="s">
+        <v>63</v>
+      </c>
+      <c r="F157" t="s">
+        <v>144</v>
+      </c>
+      <c r="G157" t="s">
+        <v>185</v>
+      </c>
+      <c r="H157" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A158">
+        <v>172</v>
+      </c>
+      <c r="B158" t="s">
+        <v>55</v>
+      </c>
+      <c r="C158" t="s">
+        <v>54</v>
+      </c>
+      <c r="D158" t="s">
+        <v>60</v>
+      </c>
+      <c r="E158" t="s">
+        <v>63</v>
+      </c>
+      <c r="F158" t="s">
+        <v>144</v>
+      </c>
+      <c r="G158" t="s">
+        <v>234</v>
+      </c>
+      <c r="H158" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A159">
+        <v>173</v>
+      </c>
+      <c r="B159" t="s">
+        <v>55</v>
+      </c>
+      <c r="C159" t="s">
+        <v>54</v>
+      </c>
+      <c r="D159" t="s">
+        <v>60</v>
+      </c>
+      <c r="E159" t="s">
+        <v>63</v>
+      </c>
+      <c r="F159" t="s">
+        <v>144</v>
+      </c>
+      <c r="G159" t="s">
+        <v>235</v>
+      </c>
+      <c r="H159" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A160">
+        <v>174</v>
+      </c>
+      <c r="B160" t="s">
+        <v>55</v>
+      </c>
+      <c r="C160" t="s">
+        <v>54</v>
+      </c>
+      <c r="D160" t="s">
+        <v>60</v>
+      </c>
+      <c r="E160" t="s">
+        <v>63</v>
+      </c>
+      <c r="F160" t="s">
+        <v>144</v>
+      </c>
+      <c r="G160" t="s">
+        <v>236</v>
+      </c>
+      <c r="H160" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A161">
+        <v>175</v>
+      </c>
+      <c r="B161" t="s">
+        <v>55</v>
+      </c>
+      <c r="C161" t="s">
+        <v>54</v>
+      </c>
+      <c r="D161" t="s">
+        <v>60</v>
+      </c>
+      <c r="E161" t="s">
+        <v>63</v>
+      </c>
+      <c r="F161" t="s">
+        <v>144</v>
+      </c>
+      <c r="G161" t="s">
+        <v>238</v>
+      </c>
+      <c r="H161" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A162">
+        <v>176</v>
+      </c>
+      <c r="B162" t="s">
+        <v>55</v>
+      </c>
+      <c r="C162" t="s">
+        <v>54</v>
+      </c>
+      <c r="D162" t="s">
+        <v>60</v>
+      </c>
+      <c r="E162" t="s">
+        <v>63</v>
+      </c>
+      <c r="F162" t="s">
+        <v>144</v>
+      </c>
+      <c r="G162" t="s">
+        <v>240</v>
+      </c>
+      <c r="H162" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A163">
+        <v>177</v>
+      </c>
+      <c r="B163" t="s">
+        <v>55</v>
+      </c>
+      <c r="C163" t="s">
+        <v>54</v>
+      </c>
+      <c r="D163" t="s">
+        <v>60</v>
+      </c>
+      <c r="E163" t="s">
+        <v>63</v>
+      </c>
+      <c r="F163" t="s">
+        <v>144</v>
+      </c>
+      <c r="G163" t="s">
+        <v>242</v>
+      </c>
+      <c r="H163" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A164">
+        <v>178</v>
+      </c>
+      <c r="B164" t="s">
+        <v>55</v>
+      </c>
+      <c r="C164" t="s">
+        <v>54</v>
+      </c>
+      <c r="D164" t="s">
+        <v>60</v>
+      </c>
+      <c r="E164" t="s">
+        <v>63</v>
+      </c>
+      <c r="F164" t="s">
+        <v>144</v>
+      </c>
+      <c r="G164" t="s">
+        <v>244</v>
+      </c>
+      <c r="H164" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A165">
+        <v>179</v>
+      </c>
+      <c r="B165" t="s">
+        <v>55</v>
+      </c>
+      <c r="C165" t="s">
+        <v>54</v>
+      </c>
+      <c r="D165" t="s">
+        <v>60</v>
+      </c>
+      <c r="E165" t="s">
+        <v>63</v>
+      </c>
+      <c r="F165" t="s">
+        <v>144</v>
+      </c>
+      <c r="G165" t="s">
+        <v>177</v>
+      </c>
+      <c r="H165" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A166">
+        <v>180</v>
+      </c>
+      <c r="B166" t="s">
+        <v>55</v>
+      </c>
+      <c r="C166" t="s">
+        <v>54</v>
+      </c>
+      <c r="D166" t="s">
+        <v>60</v>
+      </c>
+      <c r="E166" t="s">
+        <v>63</v>
+      </c>
+      <c r="F166" t="s">
+        <v>144</v>
+      </c>
+      <c r="G166" t="s">
+        <v>179</v>
+      </c>
+      <c r="H166" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A167">
+        <v>181</v>
+      </c>
+      <c r="B167" t="s">
+        <v>55</v>
+      </c>
+      <c r="C167" t="s">
+        <v>54</v>
+      </c>
+      <c r="D167" t="s">
+        <v>60</v>
+      </c>
+      <c r="E167" t="s">
+        <v>63</v>
+      </c>
+      <c r="F167" t="s">
+        <v>144</v>
+      </c>
+      <c r="G167" t="s">
+        <v>247</v>
+      </c>
+      <c r="H167" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A168">
+        <v>182</v>
+      </c>
+      <c r="B168" t="s">
+        <v>288</v>
+      </c>
+      <c r="C168" t="s">
+        <v>54</v>
+      </c>
+      <c r="D168" t="s">
+        <v>60</v>
+      </c>
+      <c r="E168" t="s">
+        <v>62</v>
+      </c>
+      <c r="F168" t="s">
+        <v>144</v>
+      </c>
+      <c r="G168" t="s">
+        <v>248</v>
+      </c>
+      <c r="H168" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A169">
+        <v>183</v>
+      </c>
+      <c r="B169" t="s">
+        <v>288</v>
+      </c>
+      <c r="C169" t="s">
+        <v>54</v>
+      </c>
+      <c r="D169" t="s">
+        <v>60</v>
+      </c>
+      <c r="E169" t="s">
+        <v>62</v>
+      </c>
+      <c r="F169" t="s">
+        <v>144</v>
+      </c>
+      <c r="G169" t="s">
+        <v>248</v>
+      </c>
+      <c r="H169" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A170">
+        <v>184</v>
+      </c>
+      <c r="B170" t="s">
+        <v>288</v>
+      </c>
+      <c r="C170" t="s">
+        <v>54</v>
+      </c>
+      <c r="D170" t="s">
+        <v>60</v>
+      </c>
+      <c r="E170" t="s">
+        <v>62</v>
+      </c>
+      <c r="F170" t="s">
+        <v>144</v>
+      </c>
+      <c r="G170" t="s">
+        <v>251</v>
+      </c>
+      <c r="H170" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A171">
+        <v>185</v>
+      </c>
+      <c r="B171" t="s">
+        <v>288</v>
+      </c>
+      <c r="C171" t="s">
+        <v>54</v>
+      </c>
+      <c r="D171" t="s">
+        <v>58</v>
+      </c>
+      <c r="E171" t="s">
+        <v>64</v>
+      </c>
+      <c r="F171" t="s">
+        <v>144</v>
+      </c>
+      <c r="G171" t="s">
+        <v>253</v>
+      </c>
+      <c r="H171" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A172">
+        <v>186</v>
+      </c>
+      <c r="B172" t="s">
+        <v>288</v>
+      </c>
+      <c r="C172" t="s">
+        <v>54</v>
+      </c>
+      <c r="D172" t="s">
+        <v>60</v>
+      </c>
+      <c r="E172" t="s">
+        <v>62</v>
+      </c>
+      <c r="F172" t="s">
+        <v>144</v>
+      </c>
+      <c r="G172" t="s">
+        <v>255</v>
+      </c>
+      <c r="H172" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A173">
+        <v>187</v>
+      </c>
+      <c r="B173" t="s">
+        <v>288</v>
+      </c>
+      <c r="C173" t="s">
+        <v>54</v>
+      </c>
+      <c r="D173" t="s">
+        <v>60</v>
+      </c>
+      <c r="E173" t="s">
+        <v>62</v>
+      </c>
+      <c r="F173" t="s">
+        <v>144</v>
+      </c>
+      <c r="G173" t="s">
+        <v>257</v>
+      </c>
+      <c r="H173" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A174">
+        <v>188</v>
+      </c>
+      <c r="B174" t="s">
+        <v>288</v>
+      </c>
+      <c r="C174" t="s">
+        <v>54</v>
+      </c>
+      <c r="D174" t="s">
+        <v>60</v>
+      </c>
+      <c r="E174" t="s">
+        <v>62</v>
+      </c>
+      <c r="F174" t="s">
+        <v>144</v>
+      </c>
+      <c r="G174" t="s">
+        <v>259</v>
+      </c>
+      <c r="H174" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A175">
+        <v>189</v>
+      </c>
+      <c r="B175" t="s">
+        <v>288</v>
+      </c>
+      <c r="C175" t="s">
+        <v>54</v>
+      </c>
+      <c r="D175" t="s">
+        <v>58</v>
+      </c>
+      <c r="E175" t="s">
+        <v>64</v>
+      </c>
+      <c r="F175" t="s">
+        <v>144</v>
+      </c>
+      <c r="G175" t="s">
+        <v>261</v>
+      </c>
+      <c r="H175" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A176">
+        <v>190</v>
+      </c>
+      <c r="B176" t="s">
+        <v>288</v>
+      </c>
+      <c r="C176" t="s">
+        <v>54</v>
+      </c>
+      <c r="D176" t="s">
+        <v>60</v>
+      </c>
+      <c r="E176" t="s">
+        <v>62</v>
+      </c>
+      <c r="F176" t="s">
+        <v>144</v>
+      </c>
+      <c r="G176" t="s">
+        <v>263</v>
+      </c>
+      <c r="H176" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A177">
+        <v>191</v>
+      </c>
+      <c r="B177" t="s">
+        <v>288</v>
+      </c>
+      <c r="C177" t="s">
+        <v>54</v>
+      </c>
+      <c r="D177" t="s">
+        <v>60</v>
+      </c>
+      <c r="E177" t="s">
+        <v>62</v>
+      </c>
+      <c r="F177" t="s">
+        <v>144</v>
+      </c>
+      <c r="G177" t="s">
+        <v>265</v>
+      </c>
+      <c r="H177" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A178">
+        <v>192</v>
+      </c>
+      <c r="B178" t="s">
+        <v>288</v>
+      </c>
+      <c r="C178" t="s">
+        <v>54</v>
+      </c>
+      <c r="D178" t="s">
+        <v>58</v>
+      </c>
+      <c r="E178" t="s">
+        <v>64</v>
+      </c>
+      <c r="F178" t="s">
+        <v>144</v>
+      </c>
+      <c r="G178" t="s">
+        <v>267</v>
+      </c>
+      <c r="H178" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A179">
+        <v>193</v>
+      </c>
+      <c r="B179" t="s">
+        <v>288</v>
+      </c>
+      <c r="C179" t="s">
+        <v>54</v>
+      </c>
+      <c r="D179" t="s">
+        <v>58</v>
+      </c>
+      <c r="E179" t="s">
+        <v>64</v>
+      </c>
+      <c r="F179" t="s">
+        <v>144</v>
+      </c>
+      <c r="G179" t="s">
+        <v>156</v>
+      </c>
+      <c r="H179" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A180">
+        <v>194</v>
+      </c>
+      <c r="B180" t="s">
+        <v>288</v>
+      </c>
+      <c r="C180" t="s">
+        <v>54</v>
+      </c>
+      <c r="D180" t="s">
+        <v>58</v>
+      </c>
+      <c r="E180" t="s">
+        <v>64</v>
+      </c>
+      <c r="F180" t="s">
+        <v>144</v>
+      </c>
+      <c r="G180" t="s">
+        <v>208</v>
+      </c>
+      <c r="H180" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A181">
+        <v>195</v>
+      </c>
+      <c r="B181" t="s">
+        <v>288</v>
+      </c>
+      <c r="C181" t="s">
+        <v>54</v>
+      </c>
+      <c r="D181" t="s">
+        <v>58</v>
+      </c>
+      <c r="E181" t="s">
+        <v>64</v>
+      </c>
+      <c r="F181" t="s">
+        <v>144</v>
+      </c>
+      <c r="G181" t="s">
+        <v>269</v>
+      </c>
+      <c r="H181" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A182">
+        <v>196</v>
+      </c>
+      <c r="B182" t="s">
+        <v>288</v>
+      </c>
+      <c r="C182" t="s">
+        <v>54</v>
+      </c>
+      <c r="D182" t="s">
+        <v>58</v>
+      </c>
+      <c r="E182" t="s">
+        <v>64</v>
+      </c>
+      <c r="F182" t="s">
+        <v>144</v>
+      </c>
+      <c r="G182" t="s">
+        <v>271</v>
+      </c>
+      <c r="H182" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A183">
+        <v>197</v>
+      </c>
+      <c r="B183" t="s">
+        <v>288</v>
+      </c>
+      <c r="C183" t="s">
+        <v>54</v>
+      </c>
+      <c r="D183" t="s">
+        <v>60</v>
+      </c>
+      <c r="E183" t="s">
+        <v>62</v>
+      </c>
+      <c r="F183" t="s">
+        <v>144</v>
+      </c>
+      <c r="G183" t="s">
+        <v>272</v>
+      </c>
+      <c r="H183" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A184">
+        <v>198</v>
+      </c>
+      <c r="B184" t="s">
+        <v>288</v>
+      </c>
+      <c r="C184" t="s">
+        <v>54</v>
+      </c>
+      <c r="D184" t="s">
+        <v>58</v>
+      </c>
+      <c r="E184" t="s">
+        <v>64</v>
+      </c>
+      <c r="F184" t="s">
+        <v>144</v>
+      </c>
+      <c r="G184" t="s">
+        <v>274</v>
+      </c>
+      <c r="H184" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A185">
+        <v>199</v>
+      </c>
+      <c r="B185" t="s">
+        <v>288</v>
+      </c>
+      <c r="C185" t="s">
+        <v>54</v>
+      </c>
+      <c r="D185" t="s">
+        <v>58</v>
+      </c>
+      <c r="E185" t="s">
+        <v>64</v>
+      </c>
+      <c r="F185" t="s">
+        <v>144</v>
+      </c>
+      <c r="G185" t="s">
+        <v>184</v>
+      </c>
+      <c r="H185" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A186">
+        <v>200</v>
+      </c>
+      <c r="B186" t="s">
+        <v>288</v>
+      </c>
+      <c r="C186" t="s">
+        <v>54</v>
+      </c>
+      <c r="D186" t="s">
+        <v>58</v>
+      </c>
+      <c r="E186" t="s">
+        <v>64</v>
+      </c>
+      <c r="F186" t="s">
+        <v>144</v>
+      </c>
+      <c r="G186" t="s">
+        <v>276</v>
+      </c>
+      <c r="H186" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A187">
+        <v>201</v>
+      </c>
+      <c r="B187" t="s">
+        <v>288</v>
+      </c>
+      <c r="C187" t="s">
+        <v>54</v>
+      </c>
+      <c r="D187" t="s">
+        <v>58</v>
+      </c>
+      <c r="E187" t="s">
+        <v>64</v>
+      </c>
+      <c r="F187" t="s">
+        <v>144</v>
+      </c>
+      <c r="G187" t="s">
+        <v>278</v>
+      </c>
+      <c r="H187" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A188">
+        <v>202</v>
+      </c>
+      <c r="B188" t="s">
+        <v>288</v>
+      </c>
+      <c r="C188" t="s">
+        <v>54</v>
+      </c>
+      <c r="D188" t="s">
+        <v>58</v>
+      </c>
+      <c r="E188" t="s">
+        <v>64</v>
+      </c>
+      <c r="F188" t="s">
+        <v>144</v>
+      </c>
+      <c r="G188" t="s">
+        <v>280</v>
+      </c>
+      <c r="H188" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A189">
+        <v>203</v>
+      </c>
+      <c r="B189" t="s">
+        <v>288</v>
+      </c>
+      <c r="C189" t="s">
+        <v>54</v>
+      </c>
+      <c r="D189" t="s">
+        <v>58</v>
+      </c>
+      <c r="E189" t="s">
+        <v>64</v>
+      </c>
+      <c r="F189" t="s">
+        <v>144</v>
+      </c>
+      <c r="G189" t="s">
+        <v>282</v>
+      </c>
+      <c r="H189" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A190">
+        <v>204</v>
+      </c>
+      <c r="B190" t="s">
+        <v>288</v>
+      </c>
+      <c r="C190" t="s">
+        <v>54</v>
+      </c>
+      <c r="D190" t="s">
+        <v>58</v>
+      </c>
+      <c r="E190" t="s">
+        <v>64</v>
+      </c>
+      <c r="F190" t="s">
+        <v>144</v>
+      </c>
+      <c r="G190" t="s">
+        <v>284</v>
+      </c>
+      <c r="H190" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A191">
+        <v>205</v>
+      </c>
+      <c r="B191" t="s">
+        <v>288</v>
+      </c>
+      <c r="C191" t="s">
+        <v>54</v>
+      </c>
+      <c r="D191" t="s">
+        <v>58</v>
+      </c>
+      <c r="E191" t="s">
+        <v>64</v>
+      </c>
+      <c r="F191" t="s">
+        <v>144</v>
+      </c>
+      <c r="G191" t="s">
+        <v>286</v>
+      </c>
+      <c r="H191" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A192">
+        <f>A191+1</f>
+        <v>206</v>
+      </c>
+      <c r="B192" t="s">
+        <v>55</v>
+      </c>
+      <c r="C192" t="s">
+        <v>57</v>
+      </c>
+      <c r="D192" t="s">
+        <v>60</v>
+      </c>
+      <c r="E192" t="s">
+        <v>63</v>
+      </c>
+      <c r="F192" t="s">
+        <v>144</v>
+      </c>
+      <c r="G192" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A193">
+        <f t="shared" ref="A193:A206" si="0">A192+1</f>
+        <v>207</v>
+      </c>
+      <c r="B193" t="s">
+        <v>55</v>
+      </c>
+      <c r="C193" t="s">
+        <v>57</v>
+      </c>
+      <c r="D193" t="s">
+        <v>60</v>
+      </c>
+      <c r="E193" t="s">
+        <v>63</v>
+      </c>
+      <c r="F193" t="s">
+        <v>144</v>
+      </c>
+      <c r="G193" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A194">
+        <f t="shared" si="0"/>
+        <v>208</v>
+      </c>
+      <c r="B194" t="s">
+        <v>55</v>
+      </c>
+      <c r="C194" t="s">
+        <v>57</v>
+      </c>
+      <c r="D194" t="s">
+        <v>60</v>
+      </c>
+      <c r="E194" t="s">
+        <v>63</v>
+      </c>
+      <c r="F194" t="s">
+        <v>144</v>
+      </c>
+      <c r="G194" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A195">
+        <f t="shared" si="0"/>
+        <v>209</v>
+      </c>
+      <c r="B195" t="s">
+        <v>55</v>
+      </c>
+      <c r="C195" t="s">
+        <v>57</v>
+      </c>
+      <c r="D195" t="s">
+        <v>60</v>
+      </c>
+      <c r="E195" t="s">
+        <v>63</v>
+      </c>
+      <c r="F195" t="s">
+        <v>144</v>
+      </c>
+      <c r="G195" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A196">
+        <f t="shared" si="0"/>
+        <v>210</v>
+      </c>
+      <c r="B196" t="s">
+        <v>55</v>
+      </c>
+      <c r="C196" t="s">
+        <v>57</v>
+      </c>
+      <c r="D196" t="s">
+        <v>60</v>
+      </c>
+      <c r="E196" t="s">
+        <v>63</v>
+      </c>
+      <c r="F196" t="s">
+        <v>144</v>
+      </c>
+      <c r="G196" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A197">
+        <f t="shared" si="0"/>
+        <v>211</v>
+      </c>
+      <c r="B197" t="s">
+        <v>55</v>
+      </c>
+      <c r="C197" t="s">
+        <v>57</v>
+      </c>
+      <c r="D197" t="s">
+        <v>60</v>
+      </c>
+      <c r="E197" t="s">
+        <v>63</v>
+      </c>
+      <c r="F197" t="s">
+        <v>144</v>
+      </c>
+      <c r="G197" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A198">
+        <f t="shared" si="0"/>
+        <v>212</v>
+      </c>
+      <c r="B198" t="s">
+        <v>56</v>
+      </c>
+      <c r="C198" t="s">
+        <v>57</v>
+      </c>
+      <c r="D198" t="s">
+        <v>59</v>
+      </c>
+      <c r="E198" t="s">
+        <v>61</v>
+      </c>
+      <c r="F198" t="s">
+        <v>144</v>
+      </c>
+      <c r="G198" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A199">
+        <f t="shared" si="0"/>
+        <v>213</v>
+      </c>
+      <c r="B199" t="s">
+        <v>56</v>
+      </c>
+      <c r="C199" t="s">
+        <v>57</v>
+      </c>
+      <c r="D199" t="s">
+        <v>59</v>
+      </c>
+      <c r="E199" t="s">
+        <v>61</v>
+      </c>
+      <c r="F199" t="s">
+        <v>144</v>
+      </c>
+      <c r="G199" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A200">
+        <f t="shared" si="0"/>
+        <v>214</v>
+      </c>
+      <c r="B200" t="s">
+        <v>56</v>
+      </c>
+      <c r="C200" t="s">
+        <v>57</v>
+      </c>
+      <c r="D200" t="s">
+        <v>59</v>
+      </c>
+      <c r="E200" t="s">
+        <v>61</v>
+      </c>
+      <c r="F200" t="s">
+        <v>144</v>
+      </c>
+      <c r="G200" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A201">
+        <f t="shared" si="0"/>
+        <v>215</v>
+      </c>
+      <c r="B201" t="s">
+        <v>56</v>
+      </c>
+      <c r="C201" t="s">
+        <v>57</v>
+      </c>
+      <c r="D201" t="s">
+        <v>60</v>
+      </c>
+      <c r="E201" t="s">
+        <v>63</v>
+      </c>
+      <c r="F201" t="s">
+        <v>144</v>
+      </c>
+      <c r="G201" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A202">
+        <f t="shared" si="0"/>
+        <v>216</v>
+      </c>
+      <c r="B202" t="s">
+        <v>56</v>
+      </c>
+      <c r="C202" t="s">
+        <v>57</v>
+      </c>
+      <c r="D202" t="s">
+        <v>60</v>
+      </c>
+      <c r="E202" t="s">
+        <v>61</v>
+      </c>
+      <c r="F202" t="s">
+        <v>144</v>
+      </c>
+      <c r="G202" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A203">
+        <f t="shared" si="0"/>
+        <v>217</v>
+      </c>
+      <c r="B203" t="s">
+        <v>56</v>
+      </c>
+      <c r="C203" t="s">
+        <v>57</v>
+      </c>
+      <c r="D203" t="s">
+        <v>60</v>
+      </c>
+      <c r="E203" t="s">
+        <v>63</v>
+      </c>
+      <c r="F203" t="s">
+        <v>144</v>
+      </c>
+      <c r="G203" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A204">
+        <f t="shared" si="0"/>
+        <v>218</v>
+      </c>
+      <c r="B204" t="s">
+        <v>56</v>
+      </c>
+      <c r="C204" t="s">
+        <v>57</v>
+      </c>
+      <c r="D204" t="s">
+        <v>60</v>
+      </c>
+      <c r="E204" t="s">
+        <v>61</v>
+      </c>
+      <c r="F204" t="s">
+        <v>144</v>
+      </c>
+      <c r="G204" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A205">
+        <f t="shared" si="0"/>
+        <v>219</v>
+      </c>
+      <c r="B205" t="s">
+        <v>56</v>
+      </c>
+      <c r="C205" t="s">
+        <v>57</v>
+      </c>
+      <c r="D205" t="s">
+        <v>60</v>
+      </c>
+      <c r="E205" t="s">
+        <v>61</v>
+      </c>
+      <c r="F205" t="s">
+        <v>144</v>
+      </c>
+      <c r="G205" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A206">
+        <f t="shared" si="0"/>
+        <v>220</v>
+      </c>
+      <c r="B206" t="s">
+        <v>56</v>
+      </c>
+      <c r="C206" t="s">
+        <v>57</v>
+      </c>
+      <c r="D206" t="s">
+        <v>60</v>
+      </c>
+      <c r="E206" t="s">
+        <v>63</v>
+      </c>
+      <c r="F206" t="s">
+        <v>144</v>
+      </c>
+      <c r="G206" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update icon and push first version to the store
</commit_message>
<xml_diff>
--- a/data/AlertsToSimulate.xlsx
+++ b/data/AlertsToSimulate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brice/Developer/public/alertsimulator/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56DCD098-949D-2548-9CCF-70B0F6D84D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68010BE5-F07D-D94F-AFCE-CF1219AFD982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13820" yWindow="500" windowWidth="30240" windowHeight="18800" xr2:uid="{11BBE7C0-3DF5-4C46-A363-C7759B687477}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18800" xr2:uid="{11BBE7C0-3DF5-4C46-A363-C7759B687477}"/>
   </bookViews>
   <sheets>
     <sheet name="Alerts" sheetId="1" r:id="rId1"/>
@@ -1288,7 +1288,7 @@
   <dimension ref="A1:H206"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add memory items for phenom300
</commit_message>
<xml_diff>
--- a/data/AlertsToSimulate.xlsx
+++ b/data/AlertsToSimulate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brice/Developer/public/alertsimulator/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68010BE5-F07D-D94F-AFCE-CF1219AFD982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{548C00B2-BB76-D546-9C83-98908483C460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18800" xr2:uid="{11BBE7C0-3DF5-4C46-A363-C7759B687477}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1412" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1516" uniqueCount="309">
   <si>
     <t>OIL PRESS</t>
   </si>
@@ -907,6 +907,66 @@
   </si>
   <si>
     <t>aircraftName</t>
+  </si>
+  <si>
+    <t>Phenom300</t>
+  </si>
+  <si>
+    <t>SMOKE/FIRE/FUMES</t>
+  </si>
+  <si>
+    <t>Smoke Evacuation</t>
+  </si>
+  <si>
+    <t>Emergency Evacuation</t>
+  </si>
+  <si>
+    <t>Dual Engine Failure</t>
+  </si>
+  <si>
+    <t>Elec Emergency</t>
+  </si>
+  <si>
+    <t>Elec XFR Fail</t>
+  </si>
+  <si>
+    <t>Engine Abnormal Start</t>
+  </si>
+  <si>
+    <t>E1 (2) Engine Fire</t>
+  </si>
+  <si>
+    <t>Cabine Altitude High</t>
+  </si>
+  <si>
+    <t>Severe damage or separation</t>
+  </si>
+  <si>
+    <t>Emergency Descent</t>
+  </si>
+  <si>
+    <t>Gear Lever</t>
+  </si>
+  <si>
+    <t>cannot be moved up</t>
+  </si>
+  <si>
+    <t>Inadvertent Pusher Activation</t>
+  </si>
+  <si>
+    <t>LG Vow SYS Fail</t>
+  </si>
+  <si>
+    <t>Takeoff Engine Failure Above V1</t>
+  </si>
+  <si>
+    <t>Rejected Takeoff below V1</t>
+  </si>
+  <si>
+    <t>Windshear</t>
+  </si>
+  <si>
+    <t>memory</t>
   </si>
 </sst>
 </file>
@@ -1285,10 +1345,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B50ED21-1FB3-1647-9374-5C9653EBF4CC}">
-  <dimension ref="A1:H206"/>
+  <dimension ref="A1:H223"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A192" workbookViewId="0">
+      <selection activeCell="D207" sqref="D207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6573,6 +6633,403 @@
       </c>
       <c r="G206" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A207">
+        <v>300</v>
+      </c>
+      <c r="B207" t="s">
+        <v>55</v>
+      </c>
+      <c r="C207" t="s">
+        <v>308</v>
+      </c>
+      <c r="D207" t="s">
+        <v>59</v>
+      </c>
+      <c r="E207" t="s">
+        <v>60</v>
+      </c>
+      <c r="F207" t="s">
+        <v>289</v>
+      </c>
+      <c r="G207" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A208">
+        <v>301</v>
+      </c>
+      <c r="B208" t="s">
+        <v>55</v>
+      </c>
+      <c r="C208" t="s">
+        <v>308</v>
+      </c>
+      <c r="D208" t="s">
+        <v>59</v>
+      </c>
+      <c r="E208" t="s">
+        <v>60</v>
+      </c>
+      <c r="F208" t="s">
+        <v>289</v>
+      </c>
+      <c r="G208" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A209">
+        <v>302</v>
+      </c>
+      <c r="B209" t="s">
+        <v>55</v>
+      </c>
+      <c r="C209" t="s">
+        <v>308</v>
+      </c>
+      <c r="D209" t="s">
+        <v>59</v>
+      </c>
+      <c r="E209" t="s">
+        <v>60</v>
+      </c>
+      <c r="F209" t="s">
+        <v>289</v>
+      </c>
+      <c r="G209" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A210">
+        <v>303</v>
+      </c>
+      <c r="B210" t="s">
+        <v>55</v>
+      </c>
+      <c r="C210" t="s">
+        <v>308</v>
+      </c>
+      <c r="D210" t="s">
+        <v>59</v>
+      </c>
+      <c r="E210" t="s">
+        <v>60</v>
+      </c>
+      <c r="F210" t="s">
+        <v>289</v>
+      </c>
+      <c r="G210" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="211" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A211">
+        <v>304</v>
+      </c>
+      <c r="B211" t="s">
+        <v>55</v>
+      </c>
+      <c r="C211" t="s">
+        <v>308</v>
+      </c>
+      <c r="D211" t="s">
+        <v>59</v>
+      </c>
+      <c r="E211" t="s">
+        <v>60</v>
+      </c>
+      <c r="F211" t="s">
+        <v>289</v>
+      </c>
+      <c r="G211" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="212" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A212">
+        <v>305</v>
+      </c>
+      <c r="B212" t="s">
+        <v>55</v>
+      </c>
+      <c r="C212" t="s">
+        <v>308</v>
+      </c>
+      <c r="D212" t="s">
+        <v>59</v>
+      </c>
+      <c r="E212" t="s">
+        <v>60</v>
+      </c>
+      <c r="F212" t="s">
+        <v>289</v>
+      </c>
+      <c r="G212" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="213" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A213">
+        <v>306</v>
+      </c>
+      <c r="B213" t="s">
+        <v>55</v>
+      </c>
+      <c r="C213" t="s">
+        <v>308</v>
+      </c>
+      <c r="D213" t="s">
+        <v>59</v>
+      </c>
+      <c r="E213" t="s">
+        <v>60</v>
+      </c>
+      <c r="F213" t="s">
+        <v>289</v>
+      </c>
+      <c r="G213" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="214" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A214">
+        <v>307</v>
+      </c>
+      <c r="B214" t="s">
+        <v>55</v>
+      </c>
+      <c r="C214" t="s">
+        <v>308</v>
+      </c>
+      <c r="D214" t="s">
+        <v>59</v>
+      </c>
+      <c r="E214" t="s">
+        <v>60</v>
+      </c>
+      <c r="F214" t="s">
+        <v>289</v>
+      </c>
+      <c r="G214" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="215" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A215">
+        <v>308</v>
+      </c>
+      <c r="B215" t="s">
+        <v>55</v>
+      </c>
+      <c r="C215" t="s">
+        <v>308</v>
+      </c>
+      <c r="D215" t="s">
+        <v>59</v>
+      </c>
+      <c r="E215" t="s">
+        <v>60</v>
+      </c>
+      <c r="F215" t="s">
+        <v>289</v>
+      </c>
+      <c r="G215" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A216">
+        <v>309</v>
+      </c>
+      <c r="B216" t="s">
+        <v>55</v>
+      </c>
+      <c r="C216" t="s">
+        <v>308</v>
+      </c>
+      <c r="D216" t="s">
+        <v>59</v>
+      </c>
+      <c r="E216" t="s">
+        <v>60</v>
+      </c>
+      <c r="F216" t="s">
+        <v>289</v>
+      </c>
+      <c r="G216" t="s">
+        <v>43</v>
+      </c>
+      <c r="H216" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="217" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A217">
+        <v>310</v>
+      </c>
+      <c r="B217" t="s">
+        <v>55</v>
+      </c>
+      <c r="C217" t="s">
+        <v>308</v>
+      </c>
+      <c r="D217" t="s">
+        <v>59</v>
+      </c>
+      <c r="E217" t="s">
+        <v>60</v>
+      </c>
+      <c r="F217" t="s">
+        <v>289</v>
+      </c>
+      <c r="G217" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="218" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A218">
+        <v>311</v>
+      </c>
+      <c r="B218" t="s">
+        <v>55</v>
+      </c>
+      <c r="C218" t="s">
+        <v>308</v>
+      </c>
+      <c r="D218" t="s">
+        <v>59</v>
+      </c>
+      <c r="E218" t="s">
+        <v>60</v>
+      </c>
+      <c r="F218" t="s">
+        <v>289</v>
+      </c>
+      <c r="G218" t="s">
+        <v>301</v>
+      </c>
+      <c r="H218" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="219" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A219">
+        <v>312</v>
+      </c>
+      <c r="B219" t="s">
+        <v>55</v>
+      </c>
+      <c r="C219" t="s">
+        <v>308</v>
+      </c>
+      <c r="D219" t="s">
+        <v>59</v>
+      </c>
+      <c r="E219" t="s">
+        <v>60</v>
+      </c>
+      <c r="F219" t="s">
+        <v>289</v>
+      </c>
+      <c r="G219" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="220" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A220">
+        <v>313</v>
+      </c>
+      <c r="B220" t="s">
+        <v>55</v>
+      </c>
+      <c r="C220" t="s">
+        <v>308</v>
+      </c>
+      <c r="D220" t="s">
+        <v>59</v>
+      </c>
+      <c r="E220" t="s">
+        <v>60</v>
+      </c>
+      <c r="F220" t="s">
+        <v>289</v>
+      </c>
+      <c r="G220" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="221" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A221">
+        <v>314</v>
+      </c>
+      <c r="B221" t="s">
+        <v>55</v>
+      </c>
+      <c r="C221" t="s">
+        <v>308</v>
+      </c>
+      <c r="D221" t="s">
+        <v>59</v>
+      </c>
+      <c r="E221" t="s">
+        <v>60</v>
+      </c>
+      <c r="F221" t="s">
+        <v>289</v>
+      </c>
+      <c r="G221" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="222" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A222">
+        <v>315</v>
+      </c>
+      <c r="B222" t="s">
+        <v>55</v>
+      </c>
+      <c r="C222" t="s">
+        <v>308</v>
+      </c>
+      <c r="D222" t="s">
+        <v>59</v>
+      </c>
+      <c r="E222" t="s">
+        <v>60</v>
+      </c>
+      <c r="F222" t="s">
+        <v>289</v>
+      </c>
+      <c r="G222" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="223" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A223">
+        <v>316</v>
+      </c>
+      <c r="B223" t="s">
+        <v>55</v>
+      </c>
+      <c r="C223" t="s">
+        <v>308</v>
+      </c>
+      <c r="D223" t="s">
+        <v>59</v>
+      </c>
+      <c r="E223" t="s">
+        <v>60</v>
+      </c>
+      <c r="F223" t="s">
+        <v>289</v>
+      </c>
+      <c r="G223" t="s">
+        <v>307</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
better parsing of sf50
</commit_message>
<xml_diff>
--- a/data/AlertsToSimulate.xlsx
+++ b/data/AlertsToSimulate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brice/Developer/public/alertsimulator/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6CB66AD-55C6-6940-9C20-CD4B85F12810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA7C239-36E5-4D4D-8202-9A8424905577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21480" yWindow="580" windowWidth="27680" windowHeight="25960" xr2:uid="{11BBE7C0-3DF5-4C46-A363-C7759B687477}"/>
+    <workbookView xWindow="23080" yWindow="1140" windowWidth="27680" windowHeight="25960" xr2:uid="{11BBE7C0-3DF5-4C46-A363-C7759B687477}"/>
   </bookViews>
   <sheets>
     <sheet name="Alerts" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2781" uniqueCount="567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2813" uniqueCount="596">
   <si>
     <t>OIL PRESS</t>
   </si>
@@ -1485,6 +1485,9 @@
     <t>In Flight</t>
   </si>
   <si>
+    <t>SF50</t>
+  </si>
+  <si>
     <t>Red AFCS annunciator on PFD; red AP flashing on PFD; continuous high-low aural tone.</t>
   </si>
   <si>
@@ -1740,7 +1743,91 @@
     <t>On Ground - Oil filter diff press too high, bypass impending.</t>
   </si>
   <si>
-    <t>sf50</t>
+    <t>Generator 1 current is low.</t>
+  </si>
+  <si>
+    <t>Generator 2 current is low.</t>
+  </si>
+  <si>
+    <t>Loss of forward main power bus voltage, OR Main power bus voltage is low.</t>
+  </si>
+  <si>
+    <t>Oxygen pressure below regulator control (250 PSI), OR Oxygen pressure low (500 PSI).</t>
+  </si>
+  <si>
+    <t>TT2 probe heater failure.</t>
+  </si>
+  <si>
+    <t>Aircraft descending to 14,000 ft.</t>
+  </si>
+  <si>
+    <t>Cabin high altitude detected.</t>
+  </si>
+  <si>
+    <t>Cabin differential pressure is too high.</t>
+  </si>
+  <si>
+    <t>Cabin pressure dump activated.</t>
+  </si>
+  <si>
+    <t>CAPS sequence has been activated.</t>
+  </si>
+  <si>
+    <t>Baggage door is open.</t>
+  </si>
+  <si>
+    <t>Main door is open.</t>
+  </si>
+  <si>
+    <t>Operating on emergency power.</t>
+  </si>
+  <si>
+    <t>N1 is not indicating rotation.</t>
+  </si>
+  <si>
+    <t>Full flaps prohibited in icing conditions.</t>
+  </si>
+  <si>
+    <t>Fuel filter diff press too high, bypass impending.</t>
+  </si>
+  <si>
+    <t>FDU fuel inlet pressure is low.</t>
+  </si>
+  <si>
+    <t>Both fuel control valves have failed.</t>
+  </si>
+  <si>
+    <t>Generator 1 voltage is high.</t>
+  </si>
+  <si>
+    <t>Generator 2 voltage is high.</t>
+  </si>
+  <si>
+    <t>ITT limits exceeded.</t>
+  </si>
+  <si>
+    <t>Landing gear is not down and locked for landing.</t>
+  </si>
+  <si>
+    <t>Ldg gear should be selected down while on ground.</t>
+  </si>
+  <si>
+    <t>N1 speed exceeded.</t>
+  </si>
+  <si>
+    <t>N2 speed exceeded.</t>
+  </si>
+  <si>
+    <t>Engine oil pressure exceedance.</t>
+  </si>
+  <si>
+    <t>Engine oil temperature exceedance.</t>
+  </si>
+  <si>
+    <t>Stick pusher active.</t>
+  </si>
+  <si>
+    <t>TT2 probes pending overheat.</t>
   </si>
 </sst>
 </file>
@@ -2121,8 +2208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B50ED21-1FB3-1647-9374-5C9653EBF4CC}">
   <dimension ref="A1:H416"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A275" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A385" workbookViewId="0">
+      <selection activeCell="D233" sqref="D233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7809,7 +7896,7 @@
         <v>62</v>
       </c>
       <c r="F224" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G224" t="s">
         <v>309</v>
@@ -7832,7 +7919,7 @@
         <v>62</v>
       </c>
       <c r="F225" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G225" t="s">
         <v>310</v>
@@ -7855,7 +7942,7 @@
         <v>62</v>
       </c>
       <c r="F226" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G226" t="s">
         <v>311</v>
@@ -7878,7 +7965,7 @@
         <v>62</v>
       </c>
       <c r="F227" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G227" t="s">
         <v>312</v>
@@ -7901,7 +7988,7 @@
         <v>62</v>
       </c>
       <c r="F228" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G228" t="s">
         <v>313</v>
@@ -7924,7 +8011,7 @@
         <v>62</v>
       </c>
       <c r="F229" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G229" t="s">
         <v>314</v>
@@ -7947,7 +8034,7 @@
         <v>62</v>
       </c>
       <c r="F230" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G230" t="s">
         <v>315</v>
@@ -7970,7 +8057,7 @@
         <v>62</v>
       </c>
       <c r="F231" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G231" t="s">
         <v>316</v>
@@ -7993,7 +8080,7 @@
         <v>62</v>
       </c>
       <c r="F232" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G232" t="s">
         <v>317</v>
@@ -8016,7 +8103,7 @@
         <v>62</v>
       </c>
       <c r="F233" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G233" t="s">
         <v>318</v>
@@ -8039,7 +8126,7 @@
         <v>62</v>
       </c>
       <c r="F234" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G234" t="s">
         <v>319</v>
@@ -8062,7 +8149,7 @@
         <v>62</v>
       </c>
       <c r="F235" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G235" t="s">
         <v>320</v>
@@ -8085,7 +8172,7 @@
         <v>62</v>
       </c>
       <c r="F236" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G236" t="s">
         <v>321</v>
@@ -8108,13 +8195,13 @@
         <v>62</v>
       </c>
       <c r="F237" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G237" t="s">
         <v>322</v>
       </c>
       <c r="H237" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="238" spans="1:8" x14ac:dyDescent="0.2">
@@ -8134,13 +8221,13 @@
         <v>62</v>
       </c>
       <c r="F238" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G238" t="s">
         <v>323</v>
       </c>
       <c r="H238" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row r="239" spans="1:8" x14ac:dyDescent="0.2">
@@ -8160,13 +8247,13 @@
         <v>62</v>
       </c>
       <c r="F239" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G239" t="s">
         <v>324</v>
       </c>
       <c r="H239" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
     </row>
     <row r="240" spans="1:8" x14ac:dyDescent="0.2">
@@ -8186,13 +8273,13 @@
         <v>62</v>
       </c>
       <c r="F240" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G240" t="s">
         <v>325</v>
       </c>
       <c r="H240" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
     <row r="241" spans="1:8" x14ac:dyDescent="0.2">
@@ -8212,13 +8299,13 @@
         <v>62</v>
       </c>
       <c r="F241" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G241" t="s">
         <v>326</v>
       </c>
       <c r="H241" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
     </row>
     <row r="242" spans="1:8" x14ac:dyDescent="0.2">
@@ -8238,13 +8325,13 @@
         <v>62</v>
       </c>
       <c r="F242" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G242" t="s">
         <v>327</v>
       </c>
       <c r="H242" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
     </row>
     <row r="243" spans="1:8" x14ac:dyDescent="0.2">
@@ -8264,13 +8351,13 @@
         <v>62</v>
       </c>
       <c r="F243" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G243" t="s">
         <v>328</v>
       </c>
       <c r="H243" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="244" spans="1:8" x14ac:dyDescent="0.2">
@@ -8290,13 +8377,13 @@
         <v>62</v>
       </c>
       <c r="F244" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G244" t="s">
         <v>329</v>
       </c>
       <c r="H244" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
     </row>
     <row r="245" spans="1:8" x14ac:dyDescent="0.2">
@@ -8316,13 +8403,13 @@
         <v>62</v>
       </c>
       <c r="F245" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G245" t="s">
         <v>24</v>
       </c>
       <c r="H245" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="246" spans="1:8" x14ac:dyDescent="0.2">
@@ -8342,13 +8429,13 @@
         <v>62</v>
       </c>
       <c r="F246" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G246" t="s">
         <v>330</v>
       </c>
       <c r="H246" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="247" spans="1:8" x14ac:dyDescent="0.2">
@@ -8368,13 +8455,13 @@
         <v>62</v>
       </c>
       <c r="F247" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G247" t="s">
         <v>331</v>
       </c>
       <c r="H247" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
     </row>
     <row r="248" spans="1:8" x14ac:dyDescent="0.2">
@@ -8394,13 +8481,13 @@
         <v>62</v>
       </c>
       <c r="F248" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G248" t="s">
         <v>332</v>
       </c>
       <c r="H248" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
     </row>
     <row r="249" spans="1:8" x14ac:dyDescent="0.2">
@@ -8420,13 +8507,13 @@
         <v>62</v>
       </c>
       <c r="F249" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G249" t="s">
         <v>333</v>
       </c>
       <c r="H249" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="250" spans="1:8" x14ac:dyDescent="0.2">
@@ -8446,13 +8533,13 @@
         <v>62</v>
       </c>
       <c r="F250" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G250" t="s">
         <v>334</v>
       </c>
       <c r="H250" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="251" spans="1:8" x14ac:dyDescent="0.2">
@@ -8472,13 +8559,13 @@
         <v>62</v>
       </c>
       <c r="F251" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G251" t="s">
         <v>335</v>
       </c>
       <c r="H251" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="252" spans="1:8" x14ac:dyDescent="0.2">
@@ -8498,13 +8585,13 @@
         <v>62</v>
       </c>
       <c r="F252" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G252" t="s">
         <v>336</v>
       </c>
       <c r="H252" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="253" spans="1:8" x14ac:dyDescent="0.2">
@@ -8524,13 +8611,13 @@
         <v>62</v>
       </c>
       <c r="F253" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G253" t="s">
         <v>337</v>
       </c>
       <c r="H253" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="254" spans="1:8" x14ac:dyDescent="0.2">
@@ -8538,7 +8625,7 @@
         <v>1030</v>
       </c>
       <c r="B254" t="s">
-        <v>54</v>
+        <v>287</v>
       </c>
       <c r="C254" t="s">
         <v>53</v>
@@ -8550,13 +8637,13 @@
         <v>62</v>
       </c>
       <c r="F254" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G254" t="s">
         <v>338</v>
       </c>
       <c r="H254" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
     <row r="255" spans="1:8" x14ac:dyDescent="0.2">
@@ -8564,7 +8651,7 @@
         <v>1031</v>
       </c>
       <c r="B255" t="s">
-        <v>54</v>
+        <v>287</v>
       </c>
       <c r="C255" t="s">
         <v>53</v>
@@ -8576,13 +8663,13 @@
         <v>62</v>
       </c>
       <c r="F255" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G255" t="s">
         <v>339</v>
       </c>
       <c r="H255" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="256" spans="1:8" x14ac:dyDescent="0.2">
@@ -8590,7 +8677,7 @@
         <v>1032</v>
       </c>
       <c r="B256" t="s">
-        <v>54</v>
+        <v>287</v>
       </c>
       <c r="C256" t="s">
         <v>53</v>
@@ -8602,7 +8689,7 @@
         <v>62</v>
       </c>
       <c r="F256" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G256" t="s">
         <v>340</v>
@@ -8628,13 +8715,13 @@
         <v>62</v>
       </c>
       <c r="F257" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G257" t="s">
         <v>341</v>
       </c>
       <c r="H257" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
     </row>
     <row r="258" spans="1:8" x14ac:dyDescent="0.2">
@@ -8654,13 +8741,13 @@
         <v>62</v>
       </c>
       <c r="F258" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G258" t="s">
         <v>342</v>
       </c>
       <c r="H258" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="259" spans="1:8" x14ac:dyDescent="0.2">
@@ -8680,13 +8767,13 @@
         <v>62</v>
       </c>
       <c r="F259" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G259" t="s">
         <v>343</v>
       </c>
       <c r="H259" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="260" spans="1:8" x14ac:dyDescent="0.2">
@@ -8706,7 +8793,7 @@
         <v>62</v>
       </c>
       <c r="F260" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G260" t="s">
         <v>344</v>
@@ -8729,13 +8816,13 @@
         <v>62</v>
       </c>
       <c r="F261" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G261" t="s">
         <v>345</v>
       </c>
       <c r="H261" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="262" spans="1:8" x14ac:dyDescent="0.2">
@@ -8743,7 +8830,7 @@
         <v>1038</v>
       </c>
       <c r="B262" t="s">
-        <v>54</v>
+        <v>287</v>
       </c>
       <c r="C262" t="s">
         <v>53</v>
@@ -8755,13 +8842,13 @@
         <v>62</v>
       </c>
       <c r="F262" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G262" t="s">
         <v>346</v>
       </c>
       <c r="H262" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
     <row r="263" spans="1:8" x14ac:dyDescent="0.2">
@@ -8781,13 +8868,13 @@
         <v>62</v>
       </c>
       <c r="F263" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G263" t="s">
         <v>347</v>
       </c>
       <c r="H263" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
     </row>
     <row r="264" spans="1:8" x14ac:dyDescent="0.2">
@@ -8807,13 +8894,13 @@
         <v>62</v>
       </c>
       <c r="F264" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G264" t="s">
         <v>348</v>
       </c>
       <c r="H264" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="265" spans="1:8" x14ac:dyDescent="0.2">
@@ -8833,13 +8920,13 @@
         <v>62</v>
       </c>
       <c r="F265" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G265" t="s">
         <v>349</v>
       </c>
       <c r="H265" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
     </row>
     <row r="266" spans="1:8" x14ac:dyDescent="0.2">
@@ -8859,7 +8946,7 @@
         <v>62</v>
       </c>
       <c r="F266" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G266" t="s">
         <v>350</v>
@@ -8873,7 +8960,7 @@
         <v>1043</v>
       </c>
       <c r="B267" t="s">
-        <v>54</v>
+        <v>287</v>
       </c>
       <c r="C267" t="s">
         <v>53</v>
@@ -8885,13 +8972,13 @@
         <v>62</v>
       </c>
       <c r="F267" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G267" t="s">
         <v>351</v>
       </c>
       <c r="H267" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
     <row r="268" spans="1:8" x14ac:dyDescent="0.2">
@@ -8899,7 +8986,7 @@
         <v>1044</v>
       </c>
       <c r="B268" t="s">
-        <v>54</v>
+        <v>287</v>
       </c>
       <c r="C268" t="s">
         <v>53</v>
@@ -8911,13 +8998,13 @@
         <v>62</v>
       </c>
       <c r="F268" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G268" t="s">
         <v>352</v>
       </c>
       <c r="H268" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row r="269" spans="1:8" x14ac:dyDescent="0.2">
@@ -8937,7 +9024,7 @@
         <v>62</v>
       </c>
       <c r="F269" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G269" t="s">
         <v>353</v>
@@ -8960,7 +9047,7 @@
         <v>62</v>
       </c>
       <c r="F270" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G270" t="s">
         <v>354</v>
@@ -8986,13 +9073,13 @@
         <v>62</v>
       </c>
       <c r="F271" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G271" t="s">
         <v>355</v>
       </c>
       <c r="H271" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
     </row>
     <row r="272" spans="1:8" x14ac:dyDescent="0.2">
@@ -9012,13 +9099,13 @@
         <v>62</v>
       </c>
       <c r="F272" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G272" t="s">
         <v>356</v>
       </c>
       <c r="H272" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="273" spans="1:8" x14ac:dyDescent="0.2">
@@ -9038,7 +9125,7 @@
         <v>62</v>
       </c>
       <c r="F273" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G273" t="s">
         <v>357</v>
@@ -9049,7 +9136,7 @@
         <v>1050</v>
       </c>
       <c r="B274" t="s">
-        <v>54</v>
+        <v>287</v>
       </c>
       <c r="C274" t="s">
         <v>53</v>
@@ -9061,13 +9148,13 @@
         <v>62</v>
       </c>
       <c r="F274" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G274" t="s">
         <v>358</v>
       </c>
       <c r="H274" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="275" spans="1:8" x14ac:dyDescent="0.2">
@@ -9075,7 +9162,7 @@
         <v>1051</v>
       </c>
       <c r="B275" t="s">
-        <v>54</v>
+        <v>287</v>
       </c>
       <c r="C275" t="s">
         <v>53</v>
@@ -9087,13 +9174,13 @@
         <v>62</v>
       </c>
       <c r="F275" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G275" t="s">
         <v>359</v>
       </c>
       <c r="H275" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="276" spans="1:8" x14ac:dyDescent="0.2">
@@ -9113,13 +9200,13 @@
         <v>62</v>
       </c>
       <c r="F276" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G276" t="s">
         <v>360</v>
       </c>
       <c r="H276" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
     <row r="277" spans="1:8" x14ac:dyDescent="0.2">
@@ -9139,13 +9226,13 @@
         <v>62</v>
       </c>
       <c r="F277" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G277" t="s">
         <v>361</v>
       </c>
       <c r="H277" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="278" spans="1:8" x14ac:dyDescent="0.2">
@@ -9165,7 +9252,7 @@
         <v>62</v>
       </c>
       <c r="F278" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G278" t="s">
         <v>362</v>
@@ -9188,13 +9275,13 @@
         <v>62</v>
       </c>
       <c r="F279" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G279" t="s">
         <v>363</v>
       </c>
       <c r="H279" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row r="280" spans="1:8" x14ac:dyDescent="0.2">
@@ -9214,13 +9301,13 @@
         <v>62</v>
       </c>
       <c r="F280" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G280" t="s">
         <v>364</v>
       </c>
       <c r="H280" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="281" spans="1:8" x14ac:dyDescent="0.2">
@@ -9240,13 +9327,13 @@
         <v>62</v>
       </c>
       <c r="F281" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G281" t="s">
         <v>6</v>
       </c>
       <c r="H281" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="282" spans="1:8" x14ac:dyDescent="0.2">
@@ -9266,7 +9353,7 @@
         <v>62</v>
       </c>
       <c r="F282" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G282" t="s">
         <v>365</v>
@@ -9289,13 +9376,13 @@
         <v>62</v>
       </c>
       <c r="F283" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G283" t="s">
         <v>366</v>
       </c>
       <c r="H283" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="284" spans="1:8" x14ac:dyDescent="0.2">
@@ -9315,13 +9402,13 @@
         <v>62</v>
       </c>
       <c r="F284" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G284" t="s">
         <v>367</v>
       </c>
       <c r="H284" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="285" spans="1:8" x14ac:dyDescent="0.2">
@@ -9329,7 +9416,7 @@
         <v>1061</v>
       </c>
       <c r="B285" t="s">
-        <v>54</v>
+        <v>287</v>
       </c>
       <c r="C285" t="s">
         <v>53</v>
@@ -9341,13 +9428,13 @@
         <v>62</v>
       </c>
       <c r="F285" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G285" t="s">
         <v>367</v>
       </c>
       <c r="H285" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="286" spans="1:8" x14ac:dyDescent="0.2">
@@ -9367,13 +9454,13 @@
         <v>62</v>
       </c>
       <c r="F286" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G286" t="s">
         <v>368</v>
       </c>
       <c r="H286" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="287" spans="1:8" x14ac:dyDescent="0.2">
@@ -9393,13 +9480,13 @@
         <v>62</v>
       </c>
       <c r="F287" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G287" t="s">
         <v>369</v>
       </c>
       <c r="H287" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row r="288" spans="1:8" x14ac:dyDescent="0.2">
@@ -9407,7 +9494,7 @@
         <v>1064</v>
       </c>
       <c r="B288" t="s">
-        <v>54</v>
+        <v>287</v>
       </c>
       <c r="C288" t="s">
         <v>53</v>
@@ -9419,13 +9506,13 @@
         <v>62</v>
       </c>
       <c r="F288" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G288" t="s">
         <v>370</v>
       </c>
       <c r="H288" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
     <row r="289" spans="1:8" x14ac:dyDescent="0.2">
@@ -9445,13 +9532,13 @@
         <v>62</v>
       </c>
       <c r="F289" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G289" t="s">
         <v>371</v>
       </c>
       <c r="H289" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="290" spans="1:8" x14ac:dyDescent="0.2">
@@ -9459,7 +9546,7 @@
         <v>1066</v>
       </c>
       <c r="B290" t="s">
-        <v>54</v>
+        <v>287</v>
       </c>
       <c r="C290" t="s">
         <v>53</v>
@@ -9471,13 +9558,13 @@
         <v>62</v>
       </c>
       <c r="F290" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G290" t="s">
         <v>372</v>
       </c>
       <c r="H290" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
     </row>
     <row r="291" spans="1:8" x14ac:dyDescent="0.2">
@@ -9497,13 +9584,13 @@
         <v>62</v>
       </c>
       <c r="F291" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G291" t="s">
         <v>373</v>
       </c>
       <c r="H291" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="292" spans="1:8" x14ac:dyDescent="0.2">
@@ -9523,7 +9610,7 @@
         <v>62</v>
       </c>
       <c r="F292" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G292" t="s">
         <v>374</v>
@@ -9546,7 +9633,7 @@
         <v>62</v>
       </c>
       <c r="F293" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G293" t="s">
         <v>375</v>
@@ -9569,13 +9656,13 @@
         <v>62</v>
       </c>
       <c r="F294" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G294" t="s">
         <v>376</v>
       </c>
       <c r="H294" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row r="295" spans="1:8" x14ac:dyDescent="0.2">
@@ -9595,10 +9682,13 @@
         <v>62</v>
       </c>
       <c r="F295" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G295" t="s">
         <v>377</v>
+      </c>
+      <c r="H295" t="s">
+        <v>567</v>
       </c>
     </row>
     <row r="296" spans="1:8" x14ac:dyDescent="0.2">
@@ -9618,10 +9708,13 @@
         <v>62</v>
       </c>
       <c r="F296" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G296" t="s">
         <v>378</v>
+      </c>
+      <c r="H296" t="s">
+        <v>568</v>
       </c>
     </row>
     <row r="297" spans="1:8" x14ac:dyDescent="0.2">
@@ -9641,7 +9734,7 @@
         <v>62</v>
       </c>
       <c r="F297" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G297" t="s">
         <v>379</v>
@@ -9667,13 +9760,13 @@
         <v>62</v>
       </c>
       <c r="F298" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G298" t="s">
         <v>380</v>
       </c>
       <c r="H298" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
     </row>
     <row r="299" spans="1:8" x14ac:dyDescent="0.2">
@@ -9693,13 +9786,13 @@
         <v>62</v>
       </c>
       <c r="F299" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G299" t="s">
         <v>381</v>
       </c>
       <c r="H299" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row r="300" spans="1:8" x14ac:dyDescent="0.2">
@@ -9719,13 +9812,13 @@
         <v>62</v>
       </c>
       <c r="F300" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G300" t="s">
         <v>382</v>
       </c>
       <c r="H300" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="301" spans="1:8" x14ac:dyDescent="0.2">
@@ -9745,7 +9838,7 @@
         <v>62</v>
       </c>
       <c r="F301" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G301" t="s">
         <v>383</v>
@@ -9768,7 +9861,7 @@
         <v>62</v>
       </c>
       <c r="F302" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G302" t="s">
         <v>384</v>
@@ -9791,13 +9884,13 @@
         <v>62</v>
       </c>
       <c r="F303" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G303" t="s">
         <v>385</v>
       </c>
       <c r="H303" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
     </row>
     <row r="304" spans="1:8" x14ac:dyDescent="0.2">
@@ -9805,7 +9898,7 @@
         <v>1080</v>
       </c>
       <c r="B304" t="s">
-        <v>54</v>
+        <v>287</v>
       </c>
       <c r="C304" t="s">
         <v>53</v>
@@ -9817,13 +9910,13 @@
         <v>62</v>
       </c>
       <c r="F304" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G304" t="s">
         <v>385</v>
       </c>
       <c r="H304" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
     </row>
     <row r="305" spans="1:8" x14ac:dyDescent="0.2">
@@ -9843,13 +9936,13 @@
         <v>62</v>
       </c>
       <c r="F305" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G305" t="s">
         <v>386</v>
       </c>
       <c r="H305" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
     </row>
     <row r="306" spans="1:8" x14ac:dyDescent="0.2">
@@ -9857,7 +9950,7 @@
         <v>1082</v>
       </c>
       <c r="B306" t="s">
-        <v>54</v>
+        <v>287</v>
       </c>
       <c r="C306" t="s">
         <v>53</v>
@@ -9869,13 +9962,13 @@
         <v>62</v>
       </c>
       <c r="F306" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G306" t="s">
         <v>386</v>
       </c>
       <c r="H306" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row r="307" spans="1:8" x14ac:dyDescent="0.2">
@@ -9895,13 +9988,13 @@
         <v>62</v>
       </c>
       <c r="F307" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G307" t="s">
         <v>387</v>
       </c>
       <c r="H307" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
     </row>
     <row r="308" spans="1:8" x14ac:dyDescent="0.2">
@@ -9921,7 +10014,7 @@
         <v>62</v>
       </c>
       <c r="F308" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G308" t="s">
         <v>388</v>
@@ -9944,7 +10037,7 @@
         <v>62</v>
       </c>
       <c r="F309" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G309" t="s">
         <v>389</v>
@@ -9967,13 +10060,13 @@
         <v>62</v>
       </c>
       <c r="F310" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G310" t="s">
         <v>390</v>
       </c>
       <c r="H310" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
     </row>
     <row r="311" spans="1:8" x14ac:dyDescent="0.2">
@@ -9993,13 +10086,13 @@
         <v>62</v>
       </c>
       <c r="F311" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G311" t="s">
         <v>391</v>
       </c>
       <c r="H311" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
     </row>
     <row r="312" spans="1:8" x14ac:dyDescent="0.2">
@@ -10019,13 +10112,13 @@
         <v>62</v>
       </c>
       <c r="F312" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G312" t="s">
         <v>392</v>
       </c>
       <c r="H312" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="313" spans="1:8" x14ac:dyDescent="0.2">
@@ -10045,13 +10138,13 @@
         <v>62</v>
       </c>
       <c r="F313" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G313" t="s">
         <v>393</v>
       </c>
       <c r="H313" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="314" spans="1:8" x14ac:dyDescent="0.2">
@@ -10071,10 +10164,13 @@
         <v>62</v>
       </c>
       <c r="F314" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G314" t="s">
         <v>394</v>
+      </c>
+      <c r="H314" t="s">
+        <v>569</v>
       </c>
     </row>
     <row r="315" spans="1:8" x14ac:dyDescent="0.2">
@@ -10082,7 +10178,7 @@
         <v>1091</v>
       </c>
       <c r="B315" t="s">
-        <v>54</v>
+        <v>287</v>
       </c>
       <c r="C315" t="s">
         <v>53</v>
@@ -10094,13 +10190,13 @@
         <v>62</v>
       </c>
       <c r="F315" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G315" t="s">
         <v>395</v>
       </c>
       <c r="H315" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="316" spans="1:8" x14ac:dyDescent="0.2">
@@ -10120,13 +10216,13 @@
         <v>62</v>
       </c>
       <c r="F316" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G316" t="s">
         <v>136</v>
       </c>
       <c r="H316" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row r="317" spans="1:8" x14ac:dyDescent="0.2">
@@ -10146,13 +10242,13 @@
         <v>62</v>
       </c>
       <c r="F317" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G317" t="s">
         <v>137</v>
       </c>
       <c r="H317" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="318" spans="1:8" x14ac:dyDescent="0.2">
@@ -10172,13 +10268,13 @@
         <v>62</v>
       </c>
       <c r="F318" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G318" t="s">
         <v>396</v>
       </c>
       <c r="H318" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="319" spans="1:8" x14ac:dyDescent="0.2">
@@ -10198,13 +10294,13 @@
         <v>62</v>
       </c>
       <c r="F319" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G319" t="s">
         <v>397</v>
       </c>
       <c r="H319" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
     </row>
     <row r="320" spans="1:8" x14ac:dyDescent="0.2">
@@ -10224,7 +10320,7 @@
         <v>62</v>
       </c>
       <c r="F320" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G320" t="s">
         <v>398</v>
@@ -10238,7 +10334,7 @@
         <v>1097</v>
       </c>
       <c r="B321" t="s">
-        <v>54</v>
+        <v>287</v>
       </c>
       <c r="C321" t="s">
         <v>53</v>
@@ -10250,7 +10346,7 @@
         <v>62</v>
       </c>
       <c r="F321" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G321" t="s">
         <v>398</v>
@@ -10276,13 +10372,13 @@
         <v>62</v>
       </c>
       <c r="F322" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G322" t="s">
         <v>399</v>
       </c>
       <c r="H322" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
     <row r="323" spans="1:8" x14ac:dyDescent="0.2">
@@ -10302,10 +10398,13 @@
         <v>62</v>
       </c>
       <c r="F323" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G323" t="s">
         <v>400</v>
+      </c>
+      <c r="H323" t="s">
+        <v>570</v>
       </c>
     </row>
     <row r="324" spans="1:8" x14ac:dyDescent="0.2">
@@ -10325,7 +10424,7 @@
         <v>62</v>
       </c>
       <c r="F324" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G324" t="s">
         <v>401</v>
@@ -10351,13 +10450,13 @@
         <v>62</v>
       </c>
       <c r="F325" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G325" t="s">
         <v>402</v>
       </c>
       <c r="H325" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="326" spans="1:8" x14ac:dyDescent="0.2">
@@ -10377,13 +10476,13 @@
         <v>62</v>
       </c>
       <c r="F326" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G326" t="s">
         <v>403</v>
       </c>
       <c r="H326" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
     </row>
     <row r="327" spans="1:8" x14ac:dyDescent="0.2">
@@ -10403,13 +10502,13 @@
         <v>62</v>
       </c>
       <c r="F327" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G327" t="s">
         <v>404</v>
       </c>
       <c r="H327" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row r="328" spans="1:8" x14ac:dyDescent="0.2">
@@ -10429,13 +10528,13 @@
         <v>62</v>
       </c>
       <c r="F328" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G328" t="s">
         <v>405</v>
       </c>
       <c r="H328" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="329" spans="1:8" x14ac:dyDescent="0.2">
@@ -10455,13 +10554,13 @@
         <v>62</v>
       </c>
       <c r="F329" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G329" t="s">
         <v>406</v>
       </c>
       <c r="H329" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
     <row r="330" spans="1:8" x14ac:dyDescent="0.2">
@@ -10481,13 +10580,13 @@
         <v>62</v>
       </c>
       <c r="F330" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G330" t="s">
         <v>407</v>
       </c>
       <c r="H330" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="331" spans="1:8" x14ac:dyDescent="0.2">
@@ -10495,7 +10594,7 @@
         <v>1107</v>
       </c>
       <c r="B331" t="s">
-        <v>54</v>
+        <v>287</v>
       </c>
       <c r="C331" t="s">
         <v>53</v>
@@ -10507,7 +10606,7 @@
         <v>62</v>
       </c>
       <c r="F331" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G331" t="s">
         <v>408</v>
@@ -10530,13 +10629,13 @@
         <v>62</v>
       </c>
       <c r="F332" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G332" t="s">
         <v>409</v>
       </c>
       <c r="H332" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="333" spans="1:8" x14ac:dyDescent="0.2">
@@ -10556,13 +10655,13 @@
         <v>62</v>
       </c>
       <c r="F333" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G333" t="s">
         <v>410</v>
       </c>
       <c r="H333" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
     </row>
     <row r="334" spans="1:8" x14ac:dyDescent="0.2">
@@ -10570,7 +10669,7 @@
         <v>1110</v>
       </c>
       <c r="B334" t="s">
-        <v>54</v>
+        <v>287</v>
       </c>
       <c r="C334" t="s">
         <v>53</v>
@@ -10582,13 +10681,13 @@
         <v>62</v>
       </c>
       <c r="F334" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G334" t="s">
         <v>411</v>
       </c>
       <c r="H334" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="335" spans="1:8" x14ac:dyDescent="0.2">
@@ -10608,13 +10707,13 @@
         <v>62</v>
       </c>
       <c r="F335" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G335" t="s">
         <v>412</v>
       </c>
       <c r="H335" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
     <row r="336" spans="1:8" x14ac:dyDescent="0.2">
@@ -10634,13 +10733,13 @@
         <v>62</v>
       </c>
       <c r="F336" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G336" t="s">
         <v>413</v>
       </c>
       <c r="H336" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
     </row>
     <row r="337" spans="1:8" x14ac:dyDescent="0.2">
@@ -10648,7 +10747,7 @@
         <v>1113</v>
       </c>
       <c r="B337" t="s">
-        <v>54</v>
+        <v>287</v>
       </c>
       <c r="C337" t="s">
         <v>53</v>
@@ -10660,13 +10759,13 @@
         <v>62</v>
       </c>
       <c r="F337" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G337" t="s">
         <v>413</v>
       </c>
       <c r="H337" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
     </row>
     <row r="338" spans="1:8" x14ac:dyDescent="0.2">
@@ -10686,13 +10785,13 @@
         <v>62</v>
       </c>
       <c r="F338" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G338" t="s">
         <v>414</v>
       </c>
       <c r="H338" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="339" spans="1:8" x14ac:dyDescent="0.2">
@@ -10700,7 +10799,7 @@
         <v>1115</v>
       </c>
       <c r="B339" t="s">
-        <v>54</v>
+        <v>287</v>
       </c>
       <c r="C339" t="s">
         <v>53</v>
@@ -10712,7 +10811,7 @@
         <v>62</v>
       </c>
       <c r="F339" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G339" t="s">
         <v>415</v>
@@ -10735,13 +10834,13 @@
         <v>62</v>
       </c>
       <c r="F340" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G340" t="s">
         <v>416</v>
       </c>
       <c r="H340" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="341" spans="1:8" x14ac:dyDescent="0.2">
@@ -10761,7 +10860,7 @@
         <v>62</v>
       </c>
       <c r="F341" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G341" t="s">
         <v>14</v>
@@ -10775,7 +10874,7 @@
         <v>1118</v>
       </c>
       <c r="B342" t="s">
-        <v>54</v>
+        <v>287</v>
       </c>
       <c r="C342" t="s">
         <v>53</v>
@@ -10787,7 +10886,7 @@
         <v>62</v>
       </c>
       <c r="F342" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G342" t="s">
         <v>417</v>
@@ -10813,13 +10912,13 @@
         <v>62</v>
       </c>
       <c r="F343" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G343" t="s">
         <v>418</v>
       </c>
       <c r="H343" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
     </row>
     <row r="344" spans="1:8" x14ac:dyDescent="0.2">
@@ -10827,7 +10926,7 @@
         <v>1120</v>
       </c>
       <c r="B344" t="s">
-        <v>54</v>
+        <v>287</v>
       </c>
       <c r="C344" t="s">
         <v>53</v>
@@ -10839,13 +10938,13 @@
         <v>62</v>
       </c>
       <c r="F344" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G344" t="s">
         <v>418</v>
       </c>
       <c r="H344" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
     </row>
     <row r="345" spans="1:8" x14ac:dyDescent="0.2">
@@ -10865,13 +10964,13 @@
         <v>62</v>
       </c>
       <c r="F345" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G345" t="s">
         <v>419</v>
       </c>
       <c r="H345" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
     <row r="346" spans="1:8" x14ac:dyDescent="0.2">
@@ -10891,13 +10990,13 @@
         <v>62</v>
       </c>
       <c r="F346" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G346" t="s">
         <v>420</v>
       </c>
       <c r="H346" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
     <row r="347" spans="1:8" x14ac:dyDescent="0.2">
@@ -10917,10 +11016,13 @@
         <v>62</v>
       </c>
       <c r="F347" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G347" t="s">
         <v>421</v>
+      </c>
+      <c r="H347" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="348" spans="1:8" x14ac:dyDescent="0.2">
@@ -10928,7 +11030,7 @@
         <v>1124</v>
       </c>
       <c r="B348" t="s">
-        <v>54</v>
+        <v>287</v>
       </c>
       <c r="C348" t="s">
         <v>53</v>
@@ -10940,13 +11042,13 @@
         <v>62</v>
       </c>
       <c r="F348" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G348" t="s">
         <v>422</v>
       </c>
       <c r="H348" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="349" spans="1:8" x14ac:dyDescent="0.2">
@@ -10966,13 +11068,13 @@
         <v>62</v>
       </c>
       <c r="F349" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G349" t="s">
         <v>423</v>
       </c>
       <c r="H349" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="350" spans="1:8" x14ac:dyDescent="0.2">
@@ -10992,13 +11094,13 @@
         <v>62</v>
       </c>
       <c r="F350" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G350" t="s">
         <v>424</v>
       </c>
       <c r="H350" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
     </row>
     <row r="351" spans="1:8" x14ac:dyDescent="0.2">
@@ -11018,7 +11120,7 @@
         <v>60</v>
       </c>
       <c r="F351" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G351" t="s">
         <v>425</v>
@@ -11041,7 +11143,7 @@
         <v>60</v>
       </c>
       <c r="F352" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G352" t="s">
         <v>426</v>
@@ -11064,7 +11166,7 @@
         <v>60</v>
       </c>
       <c r="F353" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G353" t="s">
         <v>427</v>
@@ -11087,7 +11189,7 @@
         <v>60</v>
       </c>
       <c r="F354" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G354" t="s">
         <v>428</v>
@@ -11110,7 +11212,7 @@
         <v>60</v>
       </c>
       <c r="F355" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G355" t="s">
         <v>429</v>
@@ -11133,7 +11235,7 @@
         <v>60</v>
       </c>
       <c r="F356" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G356" t="s">
         <v>430</v>
@@ -11156,7 +11258,7 @@
         <v>60</v>
       </c>
       <c r="F357" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G357" t="s">
         <v>431</v>
@@ -11179,7 +11281,7 @@
         <v>60</v>
       </c>
       <c r="F358" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G358" t="s">
         <v>432</v>
@@ -11202,7 +11304,7 @@
         <v>60</v>
       </c>
       <c r="F359" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G359" t="s">
         <v>433</v>
@@ -11225,7 +11327,7 @@
         <v>60</v>
       </c>
       <c r="F360" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G360" t="s">
         <v>434</v>
@@ -11248,7 +11350,7 @@
         <v>60</v>
       </c>
       <c r="F361" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G361" t="s">
         <v>435</v>
@@ -11271,7 +11373,7 @@
         <v>60</v>
       </c>
       <c r="F362" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G362" t="s">
         <v>436</v>
@@ -11294,7 +11396,7 @@
         <v>60</v>
       </c>
       <c r="F363" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G363" t="s">
         <v>437</v>
@@ -11317,7 +11419,7 @@
         <v>60</v>
       </c>
       <c r="F364" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G364" t="s">
         <v>438</v>
@@ -11340,7 +11442,7 @@
         <v>60</v>
       </c>
       <c r="F365" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G365" t="s">
         <v>439</v>
@@ -11363,7 +11465,7 @@
         <v>60</v>
       </c>
       <c r="F366" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G366" t="s">
         <v>299</v>
@@ -11386,7 +11488,7 @@
         <v>60</v>
       </c>
       <c r="F367" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G367" t="s">
         <v>440</v>
@@ -11409,13 +11511,13 @@
         <v>60</v>
       </c>
       <c r="F368" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G368" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="369" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A369">
         <v>1145</v>
       </c>
@@ -11432,13 +11534,13 @@
         <v>60</v>
       </c>
       <c r="F369" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G369" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="370" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A370">
         <v>1146</v>
       </c>
@@ -11455,13 +11557,13 @@
         <v>60</v>
       </c>
       <c r="F370" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G370" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="371" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A371">
         <v>1147</v>
       </c>
@@ -11478,13 +11580,13 @@
         <v>60</v>
       </c>
       <c r="F371" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G371" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="372" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A372">
         <v>1148</v>
       </c>
@@ -11501,13 +11603,13 @@
         <v>60</v>
       </c>
       <c r="F372" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G372" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="373" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A373">
         <v>1149</v>
       </c>
@@ -11524,13 +11626,13 @@
         <v>60</v>
       </c>
       <c r="F373" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G373" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="374" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A374">
         <v>1150</v>
       </c>
@@ -11547,13 +11649,13 @@
         <v>60</v>
       </c>
       <c r="F374" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G374" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="375" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A375">
         <v>1151</v>
       </c>
@@ -11570,13 +11672,13 @@
         <v>60</v>
       </c>
       <c r="F375" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G375" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="376" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A376">
         <v>1152</v>
       </c>
@@ -11593,18 +11695,18 @@
         <v>60</v>
       </c>
       <c r="F376" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G376" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="377" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A377">
         <v>1153</v>
       </c>
       <c r="B377" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C377" t="s">
         <v>53</v>
@@ -11616,18 +11718,21 @@
         <v>60</v>
       </c>
       <c r="F377" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G377" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="378" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H377" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="378" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A378">
         <v>1154</v>
       </c>
       <c r="B378" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C378" t="s">
         <v>53</v>
@@ -11639,18 +11744,21 @@
         <v>60</v>
       </c>
       <c r="F378" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G378" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="379" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H378" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="379" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A379">
         <v>1155</v>
       </c>
       <c r="B379" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C379" t="s">
         <v>53</v>
@@ -11662,18 +11770,21 @@
         <v>60</v>
       </c>
       <c r="F379" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G379" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="380" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H379" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="380" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A380">
         <v>1156</v>
       </c>
       <c r="B380" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C380" t="s">
         <v>53</v>
@@ -11685,18 +11796,21 @@
         <v>60</v>
       </c>
       <c r="F380" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G380" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="381" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H380" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="381" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A381">
         <v>1157</v>
       </c>
       <c r="B381" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C381" t="s">
         <v>53</v>
@@ -11708,18 +11822,21 @@
         <v>60</v>
       </c>
       <c r="F381" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G381" t="s">
         <v>454</v>
       </c>
-    </row>
-    <row r="382" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H381" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="382" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A382">
         <v>1158</v>
       </c>
       <c r="B382" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C382" t="s">
         <v>53</v>
@@ -11731,18 +11848,21 @@
         <v>60</v>
       </c>
       <c r="F382" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G382" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="383" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H382" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="383" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A383">
         <v>1159</v>
       </c>
       <c r="B383" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C383" t="s">
         <v>53</v>
@@ -11754,18 +11874,21 @@
         <v>60</v>
       </c>
       <c r="F383" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G383" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="384" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H383" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="384" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A384">
         <v>1160</v>
       </c>
       <c r="B384" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C384" t="s">
         <v>53</v>
@@ -11777,10 +11900,13 @@
         <v>60</v>
       </c>
       <c r="F384" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G384" t="s">
         <v>457</v>
+      </c>
+      <c r="H384" t="s">
+        <v>579</v>
       </c>
     </row>
     <row r="385" spans="1:8" x14ac:dyDescent="0.2">
@@ -11788,7 +11914,7 @@
         <v>1161</v>
       </c>
       <c r="B385" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C385" t="s">
         <v>53</v>
@@ -11800,7 +11926,7 @@
         <v>60</v>
       </c>
       <c r="F385" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G385" t="s">
         <v>458</v>
@@ -11814,7 +11940,7 @@
         <v>1162</v>
       </c>
       <c r="B386" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C386" t="s">
         <v>53</v>
@@ -11826,7 +11952,7 @@
         <v>60</v>
       </c>
       <c r="F386" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G386" t="s">
         <v>458</v>
@@ -11840,7 +11966,7 @@
         <v>1163</v>
       </c>
       <c r="B387" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C387" t="s">
         <v>53</v>
@@ -11852,10 +11978,13 @@
         <v>60</v>
       </c>
       <c r="F387" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G387" t="s">
         <v>459</v>
+      </c>
+      <c r="H387" t="s">
+        <v>580</v>
       </c>
     </row>
     <row r="388" spans="1:8" x14ac:dyDescent="0.2">
@@ -11863,7 +11992,7 @@
         <v>1164</v>
       </c>
       <c r="B388" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C388" t="s">
         <v>53</v>
@@ -11875,7 +12004,7 @@
         <v>60</v>
       </c>
       <c r="F388" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G388" t="s">
         <v>354</v>
@@ -11889,7 +12018,7 @@
         <v>1165</v>
       </c>
       <c r="B389" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C389" t="s">
         <v>53</v>
@@ -11901,10 +12030,13 @@
         <v>60</v>
       </c>
       <c r="F389" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G389" t="s">
         <v>460</v>
+      </c>
+      <c r="H389" t="s">
+        <v>510</v>
       </c>
     </row>
     <row r="390" spans="1:8" x14ac:dyDescent="0.2">
@@ -11912,7 +12044,7 @@
         <v>1166</v>
       </c>
       <c r="B390" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C390" t="s">
         <v>53</v>
@@ -11924,13 +12056,13 @@
         <v>60</v>
       </c>
       <c r="F390" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G390" t="s">
         <v>355</v>
       </c>
       <c r="H390" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
     </row>
     <row r="391" spans="1:8" x14ac:dyDescent="0.2">
@@ -11938,7 +12070,7 @@
         <v>1167</v>
       </c>
       <c r="B391" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C391" t="s">
         <v>53</v>
@@ -11950,7 +12082,7 @@
         <v>60</v>
       </c>
       <c r="F391" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G391" t="s">
         <v>461</v>
@@ -11964,7 +12096,7 @@
         <v>1168</v>
       </c>
       <c r="B392" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C392" t="s">
         <v>53</v>
@@ -11976,10 +12108,13 @@
         <v>60</v>
       </c>
       <c r="F392" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G392" t="s">
         <v>40</v>
+      </c>
+      <c r="H392" t="s">
+        <v>581</v>
       </c>
     </row>
     <row r="393" spans="1:8" x14ac:dyDescent="0.2">
@@ -11987,7 +12122,7 @@
         <v>1169</v>
       </c>
       <c r="B393" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C393" t="s">
         <v>53</v>
@@ -11999,10 +12134,13 @@
         <v>60</v>
       </c>
       <c r="F393" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G393" t="s">
         <v>462</v>
+      </c>
+      <c r="H393" t="s">
+        <v>582</v>
       </c>
     </row>
     <row r="394" spans="1:8" x14ac:dyDescent="0.2">
@@ -12010,7 +12148,7 @@
         <v>1170</v>
       </c>
       <c r="B394" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C394" t="s">
         <v>53</v>
@@ -12022,13 +12160,13 @@
         <v>60</v>
       </c>
       <c r="F394" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G394" t="s">
         <v>6</v>
       </c>
       <c r="H394" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="395" spans="1:8" x14ac:dyDescent="0.2">
@@ -12036,7 +12174,7 @@
         <v>1171</v>
       </c>
       <c r="B395" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C395" t="s">
         <v>53</v>
@@ -12048,7 +12186,7 @@
         <v>60</v>
       </c>
       <c r="F395" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G395" t="s">
         <v>365</v>
@@ -12059,7 +12197,7 @@
         <v>1172</v>
       </c>
       <c r="B396" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C396" t="s">
         <v>53</v>
@@ -12071,10 +12209,13 @@
         <v>60</v>
       </c>
       <c r="F396" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G396" t="s">
         <v>463</v>
+      </c>
+      <c r="H396" t="s">
+        <v>583</v>
       </c>
     </row>
     <row r="397" spans="1:8" x14ac:dyDescent="0.2">
@@ -12082,7 +12223,7 @@
         <v>1173</v>
       </c>
       <c r="B397" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C397" t="s">
         <v>53</v>
@@ -12094,13 +12235,13 @@
         <v>60</v>
       </c>
       <c r="F397" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G397" t="s">
         <v>373</v>
       </c>
       <c r="H397" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="398" spans="1:8" x14ac:dyDescent="0.2">
@@ -12108,7 +12249,7 @@
         <v>1174</v>
       </c>
       <c r="B398" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C398" t="s">
         <v>53</v>
@@ -12120,10 +12261,13 @@
         <v>60</v>
       </c>
       <c r="F398" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G398" t="s">
         <v>464</v>
+      </c>
+      <c r="H398" t="s">
+        <v>584</v>
       </c>
     </row>
     <row r="399" spans="1:8" x14ac:dyDescent="0.2">
@@ -12131,7 +12275,7 @@
         <v>1175</v>
       </c>
       <c r="B399" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C399" t="s">
         <v>53</v>
@@ -12143,10 +12287,13 @@
         <v>60</v>
       </c>
       <c r="F399" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G399" t="s">
         <v>377</v>
+      </c>
+      <c r="H399" t="s">
+        <v>567</v>
       </c>
     </row>
     <row r="400" spans="1:8" x14ac:dyDescent="0.2">
@@ -12154,7 +12301,7 @@
         <v>1176</v>
       </c>
       <c r="B400" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C400" t="s">
         <v>53</v>
@@ -12166,10 +12313,13 @@
         <v>60</v>
       </c>
       <c r="F400" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G400" t="s">
         <v>465</v>
+      </c>
+      <c r="H400" t="s">
+        <v>585</v>
       </c>
     </row>
     <row r="401" spans="1:8" x14ac:dyDescent="0.2">
@@ -12177,7 +12327,7 @@
         <v>1177</v>
       </c>
       <c r="B401" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C401" t="s">
         <v>53</v>
@@ -12189,10 +12339,13 @@
         <v>60</v>
       </c>
       <c r="F401" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G401" t="s">
         <v>378</v>
+      </c>
+      <c r="H401" t="s">
+        <v>568</v>
       </c>
     </row>
     <row r="402" spans="1:8" x14ac:dyDescent="0.2">
@@ -12200,7 +12353,7 @@
         <v>1178</v>
       </c>
       <c r="B402" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C402" t="s">
         <v>53</v>
@@ -12212,10 +12365,13 @@
         <v>60</v>
       </c>
       <c r="F402" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G402" t="s">
         <v>466</v>
+      </c>
+      <c r="H402" t="s">
+        <v>586</v>
       </c>
     </row>
     <row r="403" spans="1:8" x14ac:dyDescent="0.2">
@@ -12223,7 +12379,7 @@
         <v>1179</v>
       </c>
       <c r="B403" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C403" t="s">
         <v>53</v>
@@ -12235,10 +12391,13 @@
         <v>60</v>
       </c>
       <c r="F403" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G403" t="s">
         <v>467</v>
+      </c>
+      <c r="H403" t="s">
+        <v>587</v>
       </c>
     </row>
     <row r="404" spans="1:8" x14ac:dyDescent="0.2">
@@ -12246,7 +12405,7 @@
         <v>1180</v>
       </c>
       <c r="B404" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C404" t="s">
         <v>53</v>
@@ -12258,10 +12417,13 @@
         <v>60</v>
       </c>
       <c r="F404" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G404" t="s">
         <v>468</v>
+      </c>
+      <c r="H404" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="405" spans="1:8" x14ac:dyDescent="0.2">
@@ -12269,7 +12431,7 @@
         <v>1181</v>
       </c>
       <c r="B405" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C405" t="s">
         <v>53</v>
@@ -12281,10 +12443,13 @@
         <v>60</v>
       </c>
       <c r="F405" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G405" t="s">
         <v>469</v>
+      </c>
+      <c r="H405" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="406" spans="1:8" x14ac:dyDescent="0.2">
@@ -12292,7 +12457,7 @@
         <v>1182</v>
       </c>
       <c r="B406" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C406" t="s">
         <v>53</v>
@@ -12304,10 +12469,13 @@
         <v>60</v>
       </c>
       <c r="F406" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G406" t="s">
         <v>470</v>
+      </c>
+      <c r="H406" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="407" spans="1:8" x14ac:dyDescent="0.2">
@@ -12315,7 +12483,7 @@
         <v>1183</v>
       </c>
       <c r="B407" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C407" t="s">
         <v>53</v>
@@ -12327,10 +12495,13 @@
         <v>60</v>
       </c>
       <c r="F407" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G407" t="s">
         <v>471</v>
+      </c>
+      <c r="H407" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="408" spans="1:8" x14ac:dyDescent="0.2">
@@ -12338,7 +12509,7 @@
         <v>1184</v>
       </c>
       <c r="B408" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C408" t="s">
         <v>53</v>
@@ -12350,7 +12521,7 @@
         <v>60</v>
       </c>
       <c r="F408" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G408" t="s">
         <v>472</v>
@@ -12364,7 +12535,7 @@
         <v>1185</v>
       </c>
       <c r="B409" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C409" t="s">
         <v>53</v>
@@ -12376,13 +12547,13 @@
         <v>60</v>
       </c>
       <c r="F409" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G409" t="s">
         <v>396</v>
       </c>
       <c r="H409" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="410" spans="1:8" x14ac:dyDescent="0.2">
@@ -12390,7 +12561,7 @@
         <v>1186</v>
       </c>
       <c r="B410" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C410" t="s">
         <v>53</v>
@@ -12402,10 +12573,13 @@
         <v>60</v>
       </c>
       <c r="F410" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G410" t="s">
         <v>473</v>
+      </c>
+      <c r="H410" t="s">
+        <v>592</v>
       </c>
     </row>
     <row r="411" spans="1:8" x14ac:dyDescent="0.2">
@@ -12413,7 +12587,7 @@
         <v>1187</v>
       </c>
       <c r="B411" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C411" t="s">
         <v>53</v>
@@ -12425,10 +12599,13 @@
         <v>60</v>
       </c>
       <c r="F411" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G411" t="s">
         <v>474</v>
+      </c>
+      <c r="H411" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="412" spans="1:8" x14ac:dyDescent="0.2">
@@ -12448,7 +12625,7 @@
         <v>60</v>
       </c>
       <c r="F412" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G412" t="s">
         <v>475</v>
@@ -12459,7 +12636,7 @@
         <v>1189</v>
       </c>
       <c r="B413" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C413" t="s">
         <v>53</v>
@@ -12471,10 +12648,13 @@
         <v>60</v>
       </c>
       <c r="F413" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G413" t="s">
         <v>476</v>
+      </c>
+      <c r="H413" t="s">
+        <v>594</v>
       </c>
     </row>
     <row r="414" spans="1:8" x14ac:dyDescent="0.2">
@@ -12482,7 +12662,7 @@
         <v>1190</v>
       </c>
       <c r="B414" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C414" t="s">
         <v>53</v>
@@ -12494,7 +12674,7 @@
         <v>60</v>
       </c>
       <c r="F414" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G414" t="s">
         <v>417</v>
@@ -12508,7 +12688,7 @@
         <v>1191</v>
       </c>
       <c r="B415" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C415" t="s">
         <v>53</v>
@@ -12520,7 +12700,7 @@
         <v>60</v>
       </c>
       <c r="F415" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G415" t="s">
         <v>477</v>
@@ -12534,7 +12714,7 @@
         <v>1192</v>
       </c>
       <c r="B416" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C416" t="s">
         <v>53</v>
@@ -12546,10 +12726,13 @@
         <v>60</v>
       </c>
       <c r="F416" t="s">
-        <v>566</v>
+        <v>481</v>
       </c>
       <c r="G416" t="s">
         <v>478</v>
+      </c>
+      <c r="H416" t="s">
+        <v>595</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Setup requirements for venv, added epic and update_alerts.py has a validation mode
</commit_message>
<xml_diff>
--- a/data/AlertsToSimulate.xlsx
+++ b/data/AlertsToSimulate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brice/Developer/public/alertsimulator/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA7C239-36E5-4D4D-8202-9A8424905577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B2DFDAC-A620-3947-9D1F-198FD43C248E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23080" yWindow="1140" windowWidth="27680" windowHeight="25960" xr2:uid="{11BBE7C0-3DF5-4C46-A363-C7759B687477}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{11BBE7C0-3DF5-4C46-A363-C7759B687477}"/>
   </bookViews>
   <sheets>
     <sheet name="Alerts" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Alerts!$B$1:$F$85</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2813" uniqueCount="596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3457" uniqueCount="775">
   <si>
     <t>OIL PRESS</t>
   </si>
@@ -1828,6 +1828,543 @@
   </si>
   <si>
     <t>TT2 probes pending overheat.</t>
+  </si>
+  <si>
+    <t>E1000GX</t>
+  </si>
+  <si>
+    <t>REJECTED TAKEOFF</t>
+  </si>
+  <si>
+    <t>Abort takeoff safely.</t>
+  </si>
+  <si>
+    <t>ENGINE START ABORT</t>
+  </si>
+  <si>
+    <t>Abort engine start.</t>
+  </si>
+  <si>
+    <t>ENGINE FAILURE AFTER TAKEOFF</t>
+  </si>
+  <si>
+    <t>Engine failure at low altitude after takeoff.</t>
+  </si>
+  <si>
+    <t>ENGINE FAILURE IN FLIGHT</t>
+  </si>
+  <si>
+    <t>Manage engine failure in flight.</t>
+  </si>
+  <si>
+    <t>PARTIAL POWER LOSS</t>
+  </si>
+  <si>
+    <t>Partial or erratic power loss.</t>
+  </si>
+  <si>
+    <t>EMERGENCY DESCENT</t>
+  </si>
+  <si>
+    <t>Emergency descent procedure.</t>
+  </si>
+  <si>
+    <t>AIR START</t>
+  </si>
+  <si>
+    <t>Restart engine in air.</t>
+  </si>
+  <si>
+    <t>ENGINE FIRE ON GROUND</t>
+  </si>
+  <si>
+    <t>Engine or cabin fire during start/ground.</t>
+  </si>
+  <si>
+    <t>ENGINE FIRE IN FLIGHT</t>
+  </si>
+  <si>
+    <t>Engine fire in flight.</t>
+  </si>
+  <si>
+    <t>CABIN ELECTRICAL FIRE</t>
+  </si>
+  <si>
+    <t>Electrical fire in cabin.</t>
+  </si>
+  <si>
+    <t>CABIN NON-ELECTRICAL FIRE</t>
+  </si>
+  <si>
+    <t>Non-electrical fire in cabin.</t>
+  </si>
+  <si>
+    <t>SMOKE EVACUATION</t>
+  </si>
+  <si>
+    <t>Evacuate smoke from cockpit/cabin.</t>
+  </si>
+  <si>
+    <t>FORCED LANDING</t>
+  </si>
+  <si>
+    <t>Perform forced landing.</t>
+  </si>
+  <si>
+    <t>LANDING GEAR UP</t>
+  </si>
+  <si>
+    <t>Landing with gear up.</t>
+  </si>
+  <si>
+    <t>LANDING WITHOUT ELEVATOR CONTROL</t>
+  </si>
+  <si>
+    <t>Landing with no elevator control.</t>
+  </si>
+  <si>
+    <t>STALL PREVENTION SYSTEM FAILURE</t>
+  </si>
+  <si>
+    <t>Pusher/shaker system anomaly.</t>
+  </si>
+  <si>
+    <t>AUTOPILOT MALFUNCTION</t>
+  </si>
+  <si>
+    <t>Autopilot or yaw damper malfunction.</t>
+  </si>
+  <si>
+    <t>TOTAL ELECTRICAL FAILURE</t>
+  </si>
+  <si>
+    <t>Complete electrical system failure.</t>
+  </si>
+  <si>
+    <t>PFD/MFD FAILURE</t>
+  </si>
+  <si>
+    <t>Primary or Multi-Function Display failure.</t>
+  </si>
+  <si>
+    <t>ADAHRS FAILURE</t>
+  </si>
+  <si>
+    <t>Air Data and Attitude Heading Reference System failure.</t>
+  </si>
+  <si>
+    <t>AIRSPEED INDICATION FAILURE</t>
+  </si>
+  <si>
+    <t>Failure of airspeed indicator.</t>
+  </si>
+  <si>
+    <t>ALTITUDE INDICATION FAILURE</t>
+  </si>
+  <si>
+    <t>Failure of altitude indicator.</t>
+  </si>
+  <si>
+    <t>RVSM AUTOPILOT PERFORMANCE</t>
+  </si>
+  <si>
+    <t>Autopilot unable to maintain RVSM limits.</t>
+  </si>
+  <si>
+    <t>OXYGEN USE - FRONT SEATS</t>
+  </si>
+  <si>
+    <t>Use oxygen system.</t>
+  </si>
+  <si>
+    <t>CRACKED WINDSHIELD</t>
+  </si>
+  <si>
+    <t>Manage cracked/delaminated windshield.</t>
+  </si>
+  <si>
+    <t>EXIT SEVERE ICING CONDITIONS</t>
+  </si>
+  <si>
+    <t>Exit severe icing or SLD conditions.</t>
+  </si>
+  <si>
+    <t>ENGINE DOES NOT SHUT DOWN</t>
+  </si>
+  <si>
+    <t>Engine continues running after shutdown.</t>
+  </si>
+  <si>
+    <t>GEAR FAILS TO RETRACT</t>
+  </si>
+  <si>
+    <t>Landing gear fails to retract after takeoff.</t>
+  </si>
+  <si>
+    <t>GEAR FAILS TO EXTEND</t>
+  </si>
+  <si>
+    <t>Landing gear fails to extend before landing.</t>
+  </si>
+  <si>
+    <t>LANDING WITH MAIN GEAR UNSAFE</t>
+  </si>
+  <si>
+    <t>Landing with main gear unsafe.</t>
+  </si>
+  <si>
+    <t>LANDING WITH NOSE GEAR UNSAFE</t>
+  </si>
+  <si>
+    <t>Landing with nose gear unsafe.</t>
+  </si>
+  <si>
+    <t>FLAT TIRE DURING LANDING</t>
+  </si>
+  <si>
+    <t>Landing with flat tire.</t>
+  </si>
+  <si>
+    <t>LANDING WITH BRAKE FAILURE</t>
+  </si>
+  <si>
+    <t>Landing with failed brakes.</t>
+  </si>
+  <si>
+    <t>CABIN DOES NOT DEPRESSURIZE</t>
+  </si>
+  <si>
+    <t>Cabin fails to depressurize before landing.</t>
+  </si>
+  <si>
+    <t>INTERNAL WINDSHIELD FOGGING</t>
+  </si>
+  <si>
+    <t>Internal windshield frosting/moisture.</t>
+  </si>
+  <si>
+    <t>Aircraft descending automatically.</t>
+  </si>
+  <si>
+    <t>CABIN ALT HIGH</t>
+  </si>
+  <si>
+    <t>Cabin altitude excessive.</t>
+  </si>
+  <si>
+    <t>CHECK GEAR</t>
+  </si>
+  <si>
+    <t>Landing gear status warning.</t>
+  </si>
+  <si>
+    <t>DE-ICE FAIL</t>
+  </si>
+  <si>
+    <t>De-ice system failure.</t>
+  </si>
+  <si>
+    <t>DOOR UNLOCKED</t>
+  </si>
+  <si>
+    <t>Door is unlocked.</t>
+  </si>
+  <si>
+    <t>ENGINE CHIP</t>
+  </si>
+  <si>
+    <t>Metal detected in engine.</t>
+  </si>
+  <si>
+    <t>GEN FAIL</t>
+  </si>
+  <si>
+    <t>Generator failure.</t>
+  </si>
+  <si>
+    <t>ITT HIGH</t>
+  </si>
+  <si>
+    <t>Interstage turbine temperature high.</t>
+  </si>
+  <si>
+    <t>NG HIGH</t>
+  </si>
+  <si>
+    <t>Gas generator speed high.</t>
+  </si>
+  <si>
+    <t>NP HIGH</t>
+  </si>
+  <si>
+    <t>Propeller RPM high.</t>
+  </si>
+  <si>
+    <t>OIL PRESS LOW</t>
+  </si>
+  <si>
+    <t>Oil pressure low.</t>
+  </si>
+  <si>
+    <t>OIL TEMP HIGH</t>
+  </si>
+  <si>
+    <t>Oil temperature high.</t>
+  </si>
+  <si>
+    <t>OVERSPEED</t>
+  </si>
+  <si>
+    <t>Aircraft overspeed.</t>
+  </si>
+  <si>
+    <t>PUSHER ICE MODE</t>
+  </si>
+  <si>
+    <t>Pusher in ice mode.</t>
+  </si>
+  <si>
+    <t>RUD LIM FAIL</t>
+  </si>
+  <si>
+    <t>Rudder limiter failure.</t>
+  </si>
+  <si>
+    <t>STICK PUSH</t>
+  </si>
+  <si>
+    <t>Stick push activated.</t>
+  </si>
+  <si>
+    <t>STICK SHAKER</t>
+  </si>
+  <si>
+    <t>Stick shaker activated.</t>
+  </si>
+  <si>
+    <t>TORQUE HIGH</t>
+  </si>
+  <si>
+    <t>Engine torque high.</t>
+  </si>
+  <si>
+    <t>UNDERSPEED PROTECT ACTIVE</t>
+  </si>
+  <si>
+    <t>Underspeed protection active.</t>
+  </si>
+  <si>
+    <t>WSH HEAT ON</t>
+  </si>
+  <si>
+    <t>Windshield heat on.</t>
+  </si>
+  <si>
+    <t>ALTERNATOR ON</t>
+  </si>
+  <si>
+    <t>Alternator is online.</t>
+  </si>
+  <si>
+    <t>AUTO FUEL OFF</t>
+  </si>
+  <si>
+    <t>Automatic fuel system off.</t>
+  </si>
+  <si>
+    <t>AUTO PTRM FAIL</t>
+  </si>
+  <si>
+    <t>Autopilot trim fail.</t>
+  </si>
+  <si>
+    <t>BATT VOLTS LO</t>
+  </si>
+  <si>
+    <t>Battery voltage low.</t>
+  </si>
+  <si>
+    <t>DIFF P HIGH</t>
+  </si>
+  <si>
+    <t>Differential pressure high.</t>
+  </si>
+  <si>
+    <t>DOOR SEAL OFF</t>
+  </si>
+  <si>
+    <t>Door seal not inflated.</t>
+  </si>
+  <si>
+    <t>DUCT TEMP HIGH</t>
+  </si>
+  <si>
+    <t>Duct temperature high.</t>
+  </si>
+  <si>
+    <t>Flap system failure.</t>
+  </si>
+  <si>
+    <t>FUEL FILT BLOCK</t>
+  </si>
+  <si>
+    <t>Fuel filter blocked.</t>
+  </si>
+  <si>
+    <t>Fuel imbalance detected.</t>
+  </si>
+  <si>
+    <t>FUEL PRESS LOW</t>
+  </si>
+  <si>
+    <t>Fuel pressure low.</t>
+  </si>
+  <si>
+    <t>FUEL PUMP OFF</t>
+  </si>
+  <si>
+    <t>Fuel pump off.</t>
+  </si>
+  <si>
+    <t>FUEL QTY LOW</t>
+  </si>
+  <si>
+    <t>Fuel quantity low.</t>
+  </si>
+  <si>
+    <t>GEAR MISCOMP</t>
+  </si>
+  <si>
+    <t>Gear configuration mismatch.</t>
+  </si>
+  <si>
+    <t>HYD PRESS</t>
+  </si>
+  <si>
+    <t>Hydraulic pressure abnormal.</t>
+  </si>
+  <si>
+    <t>ICE</t>
+  </si>
+  <si>
+    <t>Icing detected.</t>
+  </si>
+  <si>
+    <t>ICE DETECT FAIL</t>
+  </si>
+  <si>
+    <t>Ice detection system failure.</t>
+  </si>
+  <si>
+    <t>INERT SEP FAIL</t>
+  </si>
+  <si>
+    <t>Inertial separator failure.</t>
+  </si>
+  <si>
+    <t>MAN PTRM FAIL</t>
+  </si>
+  <si>
+    <t>Manual pitch trim fail.</t>
+  </si>
+  <si>
+    <t>MISTRIM</t>
+  </si>
+  <si>
+    <t>Pitch mistrim detected.</t>
+  </si>
+  <si>
+    <t>NITROGEN LOW</t>
+  </si>
+  <si>
+    <t>Windshield nitrogen low.</t>
+  </si>
+  <si>
+    <t>OAT FAIL</t>
+  </si>
+  <si>
+    <t>Outside air temperature sensor fail.</t>
+  </si>
+  <si>
+    <t>OXY SYS OFF</t>
+  </si>
+  <si>
+    <t>Oxygen system is off.</t>
+  </si>
+  <si>
+    <t>OXYGEN LOW</t>
+  </si>
+  <si>
+    <t>Oxygen quantity low.</t>
+  </si>
+  <si>
+    <t>PITOT HEAT OFF</t>
+  </si>
+  <si>
+    <t>Pitot heat off.</t>
+  </si>
+  <si>
+    <t>PITOT HT FAIL</t>
+  </si>
+  <si>
+    <t>Pitot heat system fail.</t>
+  </si>
+  <si>
+    <t>PITOT RELAY FAIL</t>
+  </si>
+  <si>
+    <t>Pitot heat relay fail.</t>
+  </si>
+  <si>
+    <t>PRESS AIR OFF</t>
+  </si>
+  <si>
+    <t>Pressurization air off.</t>
+  </si>
+  <si>
+    <t>PROP HEAT FAIL</t>
+  </si>
+  <si>
+    <t>Propeller heat failure.</t>
+  </si>
+  <si>
+    <t>PUSH MODE FAIL</t>
+  </si>
+  <si>
+    <t>Pusher system fail.</t>
+  </si>
+  <si>
+    <t>PUSHER OFF</t>
+  </si>
+  <si>
+    <t>Stick pusher off.</t>
+  </si>
+  <si>
+    <t>STALL CMP FAIL</t>
+  </si>
+  <si>
+    <t>Stall computer failure.</t>
+  </si>
+  <si>
+    <t>STALL HT FAIL</t>
+  </si>
+  <si>
+    <t>Stall heater failure.</t>
+  </si>
+  <si>
+    <t>STARTER ON</t>
+  </si>
+  <si>
+    <t>Starter motor engaged.</t>
+  </si>
+  <si>
+    <t>TRIM DISC</t>
+  </si>
+  <si>
+    <t>Trim disconnect.</t>
+  </si>
+  <si>
+    <t>Windshield heat active.</t>
   </si>
 </sst>
 </file>
@@ -2206,10 +2743,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B50ED21-1FB3-1647-9374-5C9653EBF4CC}">
-  <dimension ref="A1:H416"/>
+  <dimension ref="A1:H508"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A385" workbookViewId="0">
-      <selection activeCell="D233" sqref="D233"/>
+    <sheetView tabSelected="1" topLeftCell="A416" workbookViewId="0">
+      <selection activeCell="A422" sqref="A422"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12733,6 +13270,2398 @@
       </c>
       <c r="H416" t="s">
         <v>595</v>
+      </c>
+    </row>
+    <row r="417" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A417">
+        <v>1200</v>
+      </c>
+      <c r="B417" t="s">
+        <v>55</v>
+      </c>
+      <c r="C417" t="s">
+        <v>56</v>
+      </c>
+      <c r="D417" t="s">
+        <v>59</v>
+      </c>
+      <c r="E417" t="s">
+        <v>60</v>
+      </c>
+      <c r="F417" t="s">
+        <v>596</v>
+      </c>
+      <c r="G417" t="s">
+        <v>597</v>
+      </c>
+      <c r="H417" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="418" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A418">
+        <v>1201</v>
+      </c>
+      <c r="B418" t="s">
+        <v>55</v>
+      </c>
+      <c r="C418" t="s">
+        <v>56</v>
+      </c>
+      <c r="D418" t="s">
+        <v>59</v>
+      </c>
+      <c r="E418" t="s">
+        <v>60</v>
+      </c>
+      <c r="F418" t="s">
+        <v>596</v>
+      </c>
+      <c r="G418" t="s">
+        <v>599</v>
+      </c>
+      <c r="H418" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="419" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A419">
+        <v>1202</v>
+      </c>
+      <c r="B419" t="s">
+        <v>55</v>
+      </c>
+      <c r="C419" t="s">
+        <v>56</v>
+      </c>
+      <c r="D419" t="s">
+        <v>59</v>
+      </c>
+      <c r="E419" t="s">
+        <v>60</v>
+      </c>
+      <c r="F419" t="s">
+        <v>596</v>
+      </c>
+      <c r="G419" t="s">
+        <v>601</v>
+      </c>
+      <c r="H419" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="420" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A420">
+        <v>1203</v>
+      </c>
+      <c r="B420" t="s">
+        <v>55</v>
+      </c>
+      <c r="C420" t="s">
+        <v>56</v>
+      </c>
+      <c r="D420" t="s">
+        <v>59</v>
+      </c>
+      <c r="E420" t="s">
+        <v>60</v>
+      </c>
+      <c r="F420" t="s">
+        <v>596</v>
+      </c>
+      <c r="G420" t="s">
+        <v>603</v>
+      </c>
+      <c r="H420" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="421" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A421">
+        <v>1204</v>
+      </c>
+      <c r="B421" t="s">
+        <v>55</v>
+      </c>
+      <c r="C421" t="s">
+        <v>56</v>
+      </c>
+      <c r="D421" t="s">
+        <v>59</v>
+      </c>
+      <c r="E421" t="s">
+        <v>62</v>
+      </c>
+      <c r="F421" t="s">
+        <v>596</v>
+      </c>
+      <c r="G421" t="s">
+        <v>605</v>
+      </c>
+      <c r="H421" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="422" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A422">
+        <v>1205</v>
+      </c>
+      <c r="B422" t="s">
+        <v>55</v>
+      </c>
+      <c r="C422" t="s">
+        <v>56</v>
+      </c>
+      <c r="D422" t="s">
+        <v>59</v>
+      </c>
+      <c r="E422" t="s">
+        <v>62</v>
+      </c>
+      <c r="F422" t="s">
+        <v>596</v>
+      </c>
+      <c r="G422" t="s">
+        <v>607</v>
+      </c>
+      <c r="H422" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="423" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A423">
+        <v>1206</v>
+      </c>
+      <c r="B423" t="s">
+        <v>55</v>
+      </c>
+      <c r="C423" t="s">
+        <v>56</v>
+      </c>
+      <c r="D423" t="s">
+        <v>59</v>
+      </c>
+      <c r="E423" t="s">
+        <v>62</v>
+      </c>
+      <c r="F423" t="s">
+        <v>596</v>
+      </c>
+      <c r="G423" t="s">
+        <v>609</v>
+      </c>
+      <c r="H423" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="424" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A424">
+        <v>1207</v>
+      </c>
+      <c r="B424" t="s">
+        <v>55</v>
+      </c>
+      <c r="C424" t="s">
+        <v>56</v>
+      </c>
+      <c r="D424" t="s">
+        <v>59</v>
+      </c>
+      <c r="E424" t="s">
+        <v>60</v>
+      </c>
+      <c r="F424" t="s">
+        <v>596</v>
+      </c>
+      <c r="G424" t="s">
+        <v>611</v>
+      </c>
+      <c r="H424" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="425" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A425">
+        <v>1208</v>
+      </c>
+      <c r="B425" t="s">
+        <v>55</v>
+      </c>
+      <c r="C425" t="s">
+        <v>56</v>
+      </c>
+      <c r="D425" t="s">
+        <v>59</v>
+      </c>
+      <c r="E425" t="s">
+        <v>60</v>
+      </c>
+      <c r="F425" t="s">
+        <v>596</v>
+      </c>
+      <c r="G425" t="s">
+        <v>613</v>
+      </c>
+      <c r="H425" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="426" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A426">
+        <v>1209</v>
+      </c>
+      <c r="B426" t="s">
+        <v>55</v>
+      </c>
+      <c r="C426" t="s">
+        <v>56</v>
+      </c>
+      <c r="D426" t="s">
+        <v>59</v>
+      </c>
+      <c r="E426" t="s">
+        <v>60</v>
+      </c>
+      <c r="F426" t="s">
+        <v>596</v>
+      </c>
+      <c r="G426" t="s">
+        <v>615</v>
+      </c>
+      <c r="H426" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="427" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A427">
+        <v>1210</v>
+      </c>
+      <c r="B427" t="s">
+        <v>55</v>
+      </c>
+      <c r="C427" t="s">
+        <v>56</v>
+      </c>
+      <c r="D427" t="s">
+        <v>59</v>
+      </c>
+      <c r="E427" t="s">
+        <v>62</v>
+      </c>
+      <c r="F427" t="s">
+        <v>596</v>
+      </c>
+      <c r="G427" t="s">
+        <v>617</v>
+      </c>
+      <c r="H427" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="428" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A428">
+        <v>1211</v>
+      </c>
+      <c r="B428" t="s">
+        <v>55</v>
+      </c>
+      <c r="C428" t="s">
+        <v>56</v>
+      </c>
+      <c r="D428" t="s">
+        <v>59</v>
+      </c>
+      <c r="E428" t="s">
+        <v>62</v>
+      </c>
+      <c r="F428" t="s">
+        <v>596</v>
+      </c>
+      <c r="G428" t="s">
+        <v>619</v>
+      </c>
+      <c r="H428" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="429" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A429">
+        <v>1212</v>
+      </c>
+      <c r="B429" t="s">
+        <v>55</v>
+      </c>
+      <c r="C429" t="s">
+        <v>56</v>
+      </c>
+      <c r="D429" t="s">
+        <v>59</v>
+      </c>
+      <c r="E429" t="s">
+        <v>60</v>
+      </c>
+      <c r="F429" t="s">
+        <v>596</v>
+      </c>
+      <c r="G429" t="s">
+        <v>621</v>
+      </c>
+      <c r="H429" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="430" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A430">
+        <v>1213</v>
+      </c>
+      <c r="B430" t="s">
+        <v>55</v>
+      </c>
+      <c r="C430" t="s">
+        <v>56</v>
+      </c>
+      <c r="D430" t="s">
+        <v>59</v>
+      </c>
+      <c r="E430" t="s">
+        <v>60</v>
+      </c>
+      <c r="F430" t="s">
+        <v>596</v>
+      </c>
+      <c r="G430" t="s">
+        <v>623</v>
+      </c>
+      <c r="H430" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="431" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A431">
+        <v>1214</v>
+      </c>
+      <c r="B431" t="s">
+        <v>55</v>
+      </c>
+      <c r="C431" t="s">
+        <v>56</v>
+      </c>
+      <c r="D431" t="s">
+        <v>59</v>
+      </c>
+      <c r="E431" t="s">
+        <v>60</v>
+      </c>
+      <c r="F431" t="s">
+        <v>596</v>
+      </c>
+      <c r="G431" t="s">
+        <v>625</v>
+      </c>
+      <c r="H431" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="432" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A432">
+        <v>1215</v>
+      </c>
+      <c r="B432" t="s">
+        <v>55</v>
+      </c>
+      <c r="C432" t="s">
+        <v>56</v>
+      </c>
+      <c r="D432" t="s">
+        <v>59</v>
+      </c>
+      <c r="E432" t="s">
+        <v>62</v>
+      </c>
+      <c r="F432" t="s">
+        <v>596</v>
+      </c>
+      <c r="G432" t="s">
+        <v>627</v>
+      </c>
+      <c r="H432" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="433" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A433">
+        <v>1216</v>
+      </c>
+      <c r="B433" t="s">
+        <v>55</v>
+      </c>
+      <c r="C433" t="s">
+        <v>56</v>
+      </c>
+      <c r="D433" t="s">
+        <v>59</v>
+      </c>
+      <c r="E433" t="s">
+        <v>62</v>
+      </c>
+      <c r="F433" t="s">
+        <v>596</v>
+      </c>
+      <c r="G433" t="s">
+        <v>629</v>
+      </c>
+      <c r="H433" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="434" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A434">
+        <v>1217</v>
+      </c>
+      <c r="B434" t="s">
+        <v>55</v>
+      </c>
+      <c r="C434" t="s">
+        <v>56</v>
+      </c>
+      <c r="D434" t="s">
+        <v>59</v>
+      </c>
+      <c r="E434" t="s">
+        <v>62</v>
+      </c>
+      <c r="F434" t="s">
+        <v>596</v>
+      </c>
+      <c r="G434" t="s">
+        <v>631</v>
+      </c>
+      <c r="H434" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="435" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A435">
+        <v>1218</v>
+      </c>
+      <c r="B435" t="s">
+        <v>55</v>
+      </c>
+      <c r="C435" t="s">
+        <v>56</v>
+      </c>
+      <c r="D435" t="s">
+        <v>59</v>
+      </c>
+      <c r="E435" t="s">
+        <v>62</v>
+      </c>
+      <c r="F435" t="s">
+        <v>596</v>
+      </c>
+      <c r="G435" t="s">
+        <v>633</v>
+      </c>
+      <c r="H435" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="436" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A436">
+        <v>1219</v>
+      </c>
+      <c r="B436" t="s">
+        <v>55</v>
+      </c>
+      <c r="C436" t="s">
+        <v>56</v>
+      </c>
+      <c r="D436" t="s">
+        <v>59</v>
+      </c>
+      <c r="E436" t="s">
+        <v>62</v>
+      </c>
+      <c r="F436" t="s">
+        <v>596</v>
+      </c>
+      <c r="G436" t="s">
+        <v>635</v>
+      </c>
+      <c r="H436" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="437" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A437">
+        <v>1220</v>
+      </c>
+      <c r="B437" t="s">
+        <v>55</v>
+      </c>
+      <c r="C437" t="s">
+        <v>56</v>
+      </c>
+      <c r="D437" t="s">
+        <v>59</v>
+      </c>
+      <c r="E437" t="s">
+        <v>62</v>
+      </c>
+      <c r="F437" t="s">
+        <v>596</v>
+      </c>
+      <c r="G437" t="s">
+        <v>637</v>
+      </c>
+      <c r="H437" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="438" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A438">
+        <v>1221</v>
+      </c>
+      <c r="B438" t="s">
+        <v>55</v>
+      </c>
+      <c r="C438" t="s">
+        <v>56</v>
+      </c>
+      <c r="D438" t="s">
+        <v>59</v>
+      </c>
+      <c r="E438" t="s">
+        <v>62</v>
+      </c>
+      <c r="F438" t="s">
+        <v>596</v>
+      </c>
+      <c r="G438" t="s">
+        <v>639</v>
+      </c>
+      <c r="H438" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="439" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A439">
+        <v>1222</v>
+      </c>
+      <c r="B439" t="s">
+        <v>55</v>
+      </c>
+      <c r="C439" t="s">
+        <v>56</v>
+      </c>
+      <c r="D439" t="s">
+        <v>59</v>
+      </c>
+      <c r="E439" t="s">
+        <v>62</v>
+      </c>
+      <c r="F439" t="s">
+        <v>596</v>
+      </c>
+      <c r="G439" t="s">
+        <v>641</v>
+      </c>
+      <c r="H439" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="440" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A440">
+        <v>1223</v>
+      </c>
+      <c r="B440" t="s">
+        <v>55</v>
+      </c>
+      <c r="C440" t="s">
+        <v>56</v>
+      </c>
+      <c r="D440" t="s">
+        <v>59</v>
+      </c>
+      <c r="E440" t="s">
+        <v>61</v>
+      </c>
+      <c r="F440" t="s">
+        <v>596</v>
+      </c>
+      <c r="G440" t="s">
+        <v>643</v>
+      </c>
+      <c r="H440" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="441" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A441">
+        <v>1224</v>
+      </c>
+      <c r="B441" t="s">
+        <v>55</v>
+      </c>
+      <c r="C441" t="s">
+        <v>56</v>
+      </c>
+      <c r="D441" t="s">
+        <v>59</v>
+      </c>
+      <c r="E441" t="s">
+        <v>61</v>
+      </c>
+      <c r="F441" t="s">
+        <v>596</v>
+      </c>
+      <c r="G441" t="s">
+        <v>645</v>
+      </c>
+      <c r="H441" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="442" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A442">
+        <v>1225</v>
+      </c>
+      <c r="B442" t="s">
+        <v>55</v>
+      </c>
+      <c r="C442" t="s">
+        <v>56</v>
+      </c>
+      <c r="D442" t="s">
+        <v>59</v>
+      </c>
+      <c r="E442" t="s">
+        <v>62</v>
+      </c>
+      <c r="F442" t="s">
+        <v>596</v>
+      </c>
+      <c r="G442" t="s">
+        <v>647</v>
+      </c>
+      <c r="H442" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="443" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A443">
+        <v>1226</v>
+      </c>
+      <c r="B443" t="s">
+        <v>54</v>
+      </c>
+      <c r="C443" t="s">
+        <v>56</v>
+      </c>
+      <c r="D443" t="s">
+        <v>59</v>
+      </c>
+      <c r="E443" t="s">
+        <v>61</v>
+      </c>
+      <c r="F443" t="s">
+        <v>596</v>
+      </c>
+      <c r="G443" t="s">
+        <v>649</v>
+      </c>
+      <c r="H443" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="444" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A444">
+        <v>1227</v>
+      </c>
+      <c r="B444" t="s">
+        <v>54</v>
+      </c>
+      <c r="C444" t="s">
+        <v>56</v>
+      </c>
+      <c r="D444" t="s">
+        <v>59</v>
+      </c>
+      <c r="E444" t="s">
+        <v>61</v>
+      </c>
+      <c r="F444" t="s">
+        <v>596</v>
+      </c>
+      <c r="G444" t="s">
+        <v>651</v>
+      </c>
+      <c r="H444" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="445" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A445">
+        <v>1228</v>
+      </c>
+      <c r="B445" t="s">
+        <v>54</v>
+      </c>
+      <c r="C445" t="s">
+        <v>56</v>
+      </c>
+      <c r="D445" t="s">
+        <v>59</v>
+      </c>
+      <c r="E445" t="s">
+        <v>61</v>
+      </c>
+      <c r="F445" t="s">
+        <v>596</v>
+      </c>
+      <c r="G445" t="s">
+        <v>653</v>
+      </c>
+      <c r="H445" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="446" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A446">
+        <v>1229</v>
+      </c>
+      <c r="B446" t="s">
+        <v>54</v>
+      </c>
+      <c r="C446" t="s">
+        <v>56</v>
+      </c>
+      <c r="D446" t="s">
+        <v>59</v>
+      </c>
+      <c r="E446" t="s">
+        <v>61</v>
+      </c>
+      <c r="F446" t="s">
+        <v>596</v>
+      </c>
+      <c r="G446" t="s">
+        <v>655</v>
+      </c>
+      <c r="H446" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="447" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A447">
+        <v>1230</v>
+      </c>
+      <c r="B447" t="s">
+        <v>54</v>
+      </c>
+      <c r="C447" t="s">
+        <v>56</v>
+      </c>
+      <c r="D447" t="s">
+        <v>59</v>
+      </c>
+      <c r="E447" t="s">
+        <v>61</v>
+      </c>
+      <c r="F447" t="s">
+        <v>596</v>
+      </c>
+      <c r="G447" t="s">
+        <v>657</v>
+      </c>
+      <c r="H447" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="448" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A448">
+        <v>1231</v>
+      </c>
+      <c r="B448" t="s">
+        <v>54</v>
+      </c>
+      <c r="C448" t="s">
+        <v>56</v>
+      </c>
+      <c r="D448" t="s">
+        <v>59</v>
+      </c>
+      <c r="E448" t="s">
+        <v>61</v>
+      </c>
+      <c r="F448" t="s">
+        <v>596</v>
+      </c>
+      <c r="G448" t="s">
+        <v>659</v>
+      </c>
+      <c r="H448" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="449" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A449">
+        <v>1232</v>
+      </c>
+      <c r="B449" t="s">
+        <v>54</v>
+      </c>
+      <c r="C449" t="s">
+        <v>56</v>
+      </c>
+      <c r="D449" t="s">
+        <v>59</v>
+      </c>
+      <c r="E449" t="s">
+        <v>61</v>
+      </c>
+      <c r="F449" t="s">
+        <v>596</v>
+      </c>
+      <c r="G449" t="s">
+        <v>661</v>
+      </c>
+      <c r="H449" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="450" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A450">
+        <v>1233</v>
+      </c>
+      <c r="B450" t="s">
+        <v>54</v>
+      </c>
+      <c r="C450" t="s">
+        <v>56</v>
+      </c>
+      <c r="D450" t="s">
+        <v>59</v>
+      </c>
+      <c r="E450" t="s">
+        <v>61</v>
+      </c>
+      <c r="F450" t="s">
+        <v>596</v>
+      </c>
+      <c r="G450" t="s">
+        <v>663</v>
+      </c>
+      <c r="H450" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="451" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A451">
+        <v>1234</v>
+      </c>
+      <c r="B451" t="s">
+        <v>54</v>
+      </c>
+      <c r="C451" t="s">
+        <v>56</v>
+      </c>
+      <c r="D451" t="s">
+        <v>59</v>
+      </c>
+      <c r="E451" t="s">
+        <v>61</v>
+      </c>
+      <c r="F451" t="s">
+        <v>596</v>
+      </c>
+      <c r="G451" t="s">
+        <v>665</v>
+      </c>
+      <c r="H451" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="452" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A452">
+        <v>1235</v>
+      </c>
+      <c r="B452" t="s">
+        <v>55</v>
+      </c>
+      <c r="C452" t="s">
+        <v>53</v>
+      </c>
+      <c r="D452" t="s">
+        <v>59</v>
+      </c>
+      <c r="E452" t="s">
+        <v>60</v>
+      </c>
+      <c r="F452" t="s">
+        <v>596</v>
+      </c>
+      <c r="G452" t="s">
+        <v>450</v>
+      </c>
+      <c r="H452" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="453" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A453">
+        <v>1236</v>
+      </c>
+      <c r="B453" t="s">
+        <v>55</v>
+      </c>
+      <c r="C453" t="s">
+        <v>53</v>
+      </c>
+      <c r="D453" t="s">
+        <v>59</v>
+      </c>
+      <c r="E453" t="s">
+        <v>60</v>
+      </c>
+      <c r="F453" t="s">
+        <v>596</v>
+      </c>
+      <c r="G453" t="s">
+        <v>668</v>
+      </c>
+      <c r="H453" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="454" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A454">
+        <v>1237</v>
+      </c>
+      <c r="B454" t="s">
+        <v>55</v>
+      </c>
+      <c r="C454" t="s">
+        <v>53</v>
+      </c>
+      <c r="D454" t="s">
+        <v>59</v>
+      </c>
+      <c r="E454" t="s">
+        <v>60</v>
+      </c>
+      <c r="F454" t="s">
+        <v>596</v>
+      </c>
+      <c r="G454" t="s">
+        <v>670</v>
+      </c>
+      <c r="H454" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="455" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A455">
+        <v>1238</v>
+      </c>
+      <c r="B455" t="s">
+        <v>55</v>
+      </c>
+      <c r="C455" t="s">
+        <v>53</v>
+      </c>
+      <c r="D455" t="s">
+        <v>59</v>
+      </c>
+      <c r="E455" t="s">
+        <v>60</v>
+      </c>
+      <c r="F455" t="s">
+        <v>596</v>
+      </c>
+      <c r="G455" t="s">
+        <v>672</v>
+      </c>
+      <c r="H455" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="456" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A456">
+        <v>1239</v>
+      </c>
+      <c r="B456" t="s">
+        <v>55</v>
+      </c>
+      <c r="C456" t="s">
+        <v>53</v>
+      </c>
+      <c r="D456" t="s">
+        <v>59</v>
+      </c>
+      <c r="E456" t="s">
+        <v>60</v>
+      </c>
+      <c r="F456" t="s">
+        <v>596</v>
+      </c>
+      <c r="G456" t="s">
+        <v>674</v>
+      </c>
+      <c r="H456" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="457" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A457">
+        <v>1240</v>
+      </c>
+      <c r="B457" t="s">
+        <v>55</v>
+      </c>
+      <c r="C457" t="s">
+        <v>53</v>
+      </c>
+      <c r="D457" t="s">
+        <v>59</v>
+      </c>
+      <c r="E457" t="s">
+        <v>60</v>
+      </c>
+      <c r="F457" t="s">
+        <v>596</v>
+      </c>
+      <c r="G457" t="s">
+        <v>676</v>
+      </c>
+      <c r="H457" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="458" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A458">
+        <v>1241</v>
+      </c>
+      <c r="B458" t="s">
+        <v>55</v>
+      </c>
+      <c r="C458" t="s">
+        <v>53</v>
+      </c>
+      <c r="D458" t="s">
+        <v>59</v>
+      </c>
+      <c r="E458" t="s">
+        <v>60</v>
+      </c>
+      <c r="F458" t="s">
+        <v>596</v>
+      </c>
+      <c r="G458" t="s">
+        <v>678</v>
+      </c>
+      <c r="H458" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="459" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A459">
+        <v>1242</v>
+      </c>
+      <c r="B459" t="s">
+        <v>55</v>
+      </c>
+      <c r="C459" t="s">
+        <v>53</v>
+      </c>
+      <c r="D459" t="s">
+        <v>59</v>
+      </c>
+      <c r="E459" t="s">
+        <v>60</v>
+      </c>
+      <c r="F459" t="s">
+        <v>596</v>
+      </c>
+      <c r="G459" t="s">
+        <v>680</v>
+      </c>
+      <c r="H459" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="460" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A460">
+        <v>1243</v>
+      </c>
+      <c r="B460" t="s">
+        <v>55</v>
+      </c>
+      <c r="C460" t="s">
+        <v>53</v>
+      </c>
+      <c r="D460" t="s">
+        <v>59</v>
+      </c>
+      <c r="E460" t="s">
+        <v>60</v>
+      </c>
+      <c r="F460" t="s">
+        <v>596</v>
+      </c>
+      <c r="G460" t="s">
+        <v>682</v>
+      </c>
+      <c r="H460" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="461" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A461">
+        <v>1244</v>
+      </c>
+      <c r="B461" t="s">
+        <v>55</v>
+      </c>
+      <c r="C461" t="s">
+        <v>53</v>
+      </c>
+      <c r="D461" t="s">
+        <v>59</v>
+      </c>
+      <c r="E461" t="s">
+        <v>60</v>
+      </c>
+      <c r="F461" t="s">
+        <v>596</v>
+      </c>
+      <c r="G461" t="s">
+        <v>684</v>
+      </c>
+      <c r="H461" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="462" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A462">
+        <v>1245</v>
+      </c>
+      <c r="B462" t="s">
+        <v>55</v>
+      </c>
+      <c r="C462" t="s">
+        <v>53</v>
+      </c>
+      <c r="D462" t="s">
+        <v>59</v>
+      </c>
+      <c r="E462" t="s">
+        <v>60</v>
+      </c>
+      <c r="F462" t="s">
+        <v>596</v>
+      </c>
+      <c r="G462" t="s">
+        <v>686</v>
+      </c>
+      <c r="H462" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="463" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A463">
+        <v>1246</v>
+      </c>
+      <c r="B463" t="s">
+        <v>55</v>
+      </c>
+      <c r="C463" t="s">
+        <v>53</v>
+      </c>
+      <c r="D463" t="s">
+        <v>59</v>
+      </c>
+      <c r="E463" t="s">
+        <v>60</v>
+      </c>
+      <c r="F463" t="s">
+        <v>596</v>
+      </c>
+      <c r="G463" t="s">
+        <v>688</v>
+      </c>
+      <c r="H463" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="464" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A464">
+        <v>1247</v>
+      </c>
+      <c r="B464" t="s">
+        <v>55</v>
+      </c>
+      <c r="C464" t="s">
+        <v>53</v>
+      </c>
+      <c r="D464" t="s">
+        <v>59</v>
+      </c>
+      <c r="E464" t="s">
+        <v>60</v>
+      </c>
+      <c r="F464" t="s">
+        <v>596</v>
+      </c>
+      <c r="G464" t="s">
+        <v>690</v>
+      </c>
+      <c r="H464" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="465" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A465">
+        <v>1248</v>
+      </c>
+      <c r="B465" t="s">
+        <v>55</v>
+      </c>
+      <c r="C465" t="s">
+        <v>53</v>
+      </c>
+      <c r="D465" t="s">
+        <v>59</v>
+      </c>
+      <c r="E465" t="s">
+        <v>60</v>
+      </c>
+      <c r="F465" t="s">
+        <v>596</v>
+      </c>
+      <c r="G465" t="s">
+        <v>692</v>
+      </c>
+      <c r="H465" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="466" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A466">
+        <v>1249</v>
+      </c>
+      <c r="B466" t="s">
+        <v>55</v>
+      </c>
+      <c r="C466" t="s">
+        <v>53</v>
+      </c>
+      <c r="D466" t="s">
+        <v>59</v>
+      </c>
+      <c r="E466" t="s">
+        <v>60</v>
+      </c>
+      <c r="F466" t="s">
+        <v>596</v>
+      </c>
+      <c r="G466" t="s">
+        <v>694</v>
+      </c>
+      <c r="H466" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="467" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A467">
+        <v>1250</v>
+      </c>
+      <c r="B467" t="s">
+        <v>55</v>
+      </c>
+      <c r="C467" t="s">
+        <v>53</v>
+      </c>
+      <c r="D467" t="s">
+        <v>59</v>
+      </c>
+      <c r="E467" t="s">
+        <v>60</v>
+      </c>
+      <c r="F467" t="s">
+        <v>596</v>
+      </c>
+      <c r="G467" t="s">
+        <v>696</v>
+      </c>
+      <c r="H467" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="468" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A468">
+        <v>1251</v>
+      </c>
+      <c r="B468" t="s">
+        <v>55</v>
+      </c>
+      <c r="C468" t="s">
+        <v>53</v>
+      </c>
+      <c r="D468" t="s">
+        <v>59</v>
+      </c>
+      <c r="E468" t="s">
+        <v>60</v>
+      </c>
+      <c r="F468" t="s">
+        <v>596</v>
+      </c>
+      <c r="G468" t="s">
+        <v>698</v>
+      </c>
+      <c r="H468" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="469" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A469">
+        <v>1252</v>
+      </c>
+      <c r="B469" t="s">
+        <v>55</v>
+      </c>
+      <c r="C469" t="s">
+        <v>53</v>
+      </c>
+      <c r="D469" t="s">
+        <v>59</v>
+      </c>
+      <c r="E469" t="s">
+        <v>60</v>
+      </c>
+      <c r="F469" t="s">
+        <v>596</v>
+      </c>
+      <c r="G469" t="s">
+        <v>700</v>
+      </c>
+      <c r="H469" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="470" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A470">
+        <v>1253</v>
+      </c>
+      <c r="B470" t="s">
+        <v>55</v>
+      </c>
+      <c r="C470" t="s">
+        <v>53</v>
+      </c>
+      <c r="D470" t="s">
+        <v>59</v>
+      </c>
+      <c r="E470" t="s">
+        <v>60</v>
+      </c>
+      <c r="F470" t="s">
+        <v>596</v>
+      </c>
+      <c r="G470" t="s">
+        <v>702</v>
+      </c>
+      <c r="H470" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="471" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A471">
+        <v>1254</v>
+      </c>
+      <c r="B471" t="s">
+        <v>55</v>
+      </c>
+      <c r="C471" t="s">
+        <v>53</v>
+      </c>
+      <c r="D471" t="s">
+        <v>59</v>
+      </c>
+      <c r="E471" t="s">
+        <v>60</v>
+      </c>
+      <c r="F471" t="s">
+        <v>596</v>
+      </c>
+      <c r="G471" t="s">
+        <v>704</v>
+      </c>
+      <c r="H471" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="472" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A472">
+        <v>1255</v>
+      </c>
+      <c r="B472" t="s">
+        <v>54</v>
+      </c>
+      <c r="C472" t="s">
+        <v>53</v>
+      </c>
+      <c r="D472" t="s">
+        <v>59</v>
+      </c>
+      <c r="E472" t="s">
+        <v>62</v>
+      </c>
+      <c r="F472" t="s">
+        <v>596</v>
+      </c>
+      <c r="G472" t="s">
+        <v>706</v>
+      </c>
+      <c r="H472" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="473" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A473">
+        <v>1256</v>
+      </c>
+      <c r="B473" t="s">
+        <v>54</v>
+      </c>
+      <c r="C473" t="s">
+        <v>53</v>
+      </c>
+      <c r="D473" t="s">
+        <v>59</v>
+      </c>
+      <c r="E473" t="s">
+        <v>62</v>
+      </c>
+      <c r="F473" t="s">
+        <v>596</v>
+      </c>
+      <c r="G473" t="s">
+        <v>708</v>
+      </c>
+      <c r="H473" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="474" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A474">
+        <v>1257</v>
+      </c>
+      <c r="B474" t="s">
+        <v>54</v>
+      </c>
+      <c r="C474" t="s">
+        <v>53</v>
+      </c>
+      <c r="D474" t="s">
+        <v>59</v>
+      </c>
+      <c r="E474" t="s">
+        <v>62</v>
+      </c>
+      <c r="F474" t="s">
+        <v>596</v>
+      </c>
+      <c r="G474" t="s">
+        <v>710</v>
+      </c>
+      <c r="H474" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="475" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A475">
+        <v>1258</v>
+      </c>
+      <c r="B475" t="s">
+        <v>54</v>
+      </c>
+      <c r="C475" t="s">
+        <v>53</v>
+      </c>
+      <c r="D475" t="s">
+        <v>59</v>
+      </c>
+      <c r="E475" t="s">
+        <v>62</v>
+      </c>
+      <c r="F475" t="s">
+        <v>596</v>
+      </c>
+      <c r="G475" t="s">
+        <v>712</v>
+      </c>
+      <c r="H475" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="476" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A476">
+        <v>1259</v>
+      </c>
+      <c r="B476" t="s">
+        <v>54</v>
+      </c>
+      <c r="C476" t="s">
+        <v>53</v>
+      </c>
+      <c r="D476" t="s">
+        <v>59</v>
+      </c>
+      <c r="E476" t="s">
+        <v>62</v>
+      </c>
+      <c r="F476" t="s">
+        <v>596</v>
+      </c>
+      <c r="G476" t="s">
+        <v>714</v>
+      </c>
+      <c r="H476" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="477" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A477">
+        <v>1260</v>
+      </c>
+      <c r="B477" t="s">
+        <v>54</v>
+      </c>
+      <c r="C477" t="s">
+        <v>53</v>
+      </c>
+      <c r="D477" t="s">
+        <v>59</v>
+      </c>
+      <c r="E477" t="s">
+        <v>62</v>
+      </c>
+      <c r="F477" t="s">
+        <v>596</v>
+      </c>
+      <c r="G477" t="s">
+        <v>716</v>
+      </c>
+      <c r="H477" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="478" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A478">
+        <v>1261</v>
+      </c>
+      <c r="B478" t="s">
+        <v>54</v>
+      </c>
+      <c r="C478" t="s">
+        <v>53</v>
+      </c>
+      <c r="D478" t="s">
+        <v>59</v>
+      </c>
+      <c r="E478" t="s">
+        <v>62</v>
+      </c>
+      <c r="F478" t="s">
+        <v>596</v>
+      </c>
+      <c r="G478" t="s">
+        <v>718</v>
+      </c>
+      <c r="H478" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="479" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A479">
+        <v>1262</v>
+      </c>
+      <c r="B479" t="s">
+        <v>54</v>
+      </c>
+      <c r="C479" t="s">
+        <v>53</v>
+      </c>
+      <c r="D479" t="s">
+        <v>59</v>
+      </c>
+      <c r="E479" t="s">
+        <v>62</v>
+      </c>
+      <c r="F479" t="s">
+        <v>596</v>
+      </c>
+      <c r="G479" t="s">
+        <v>362</v>
+      </c>
+      <c r="H479" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="480" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A480">
+        <v>1263</v>
+      </c>
+      <c r="B480" t="s">
+        <v>54</v>
+      </c>
+      <c r="C480" t="s">
+        <v>53</v>
+      </c>
+      <c r="D480" t="s">
+        <v>59</v>
+      </c>
+      <c r="E480" t="s">
+        <v>62</v>
+      </c>
+      <c r="F480" t="s">
+        <v>596</v>
+      </c>
+      <c r="G480" t="s">
+        <v>721</v>
+      </c>
+      <c r="H480" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="481" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A481">
+        <v>1264</v>
+      </c>
+      <c r="B481" t="s">
+        <v>54</v>
+      </c>
+      <c r="C481" t="s">
+        <v>53</v>
+      </c>
+      <c r="D481" t="s">
+        <v>59</v>
+      </c>
+      <c r="E481" t="s">
+        <v>62</v>
+      </c>
+      <c r="F481" t="s">
+        <v>596</v>
+      </c>
+      <c r="G481" t="s">
+        <v>6</v>
+      </c>
+      <c r="H481" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="482" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A482">
+        <v>1265</v>
+      </c>
+      <c r="B482" t="s">
+        <v>54</v>
+      </c>
+      <c r="C482" t="s">
+        <v>53</v>
+      </c>
+      <c r="D482" t="s">
+        <v>59</v>
+      </c>
+      <c r="E482" t="s">
+        <v>62</v>
+      </c>
+      <c r="F482" t="s">
+        <v>596</v>
+      </c>
+      <c r="G482" t="s">
+        <v>724</v>
+      </c>
+      <c r="H482" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="483" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A483">
+        <v>1266</v>
+      </c>
+      <c r="B483" t="s">
+        <v>54</v>
+      </c>
+      <c r="C483" t="s">
+        <v>53</v>
+      </c>
+      <c r="D483" t="s">
+        <v>59</v>
+      </c>
+      <c r="E483" t="s">
+        <v>62</v>
+      </c>
+      <c r="F483" t="s">
+        <v>596</v>
+      </c>
+      <c r="G483" t="s">
+        <v>726</v>
+      </c>
+      <c r="H483" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="484" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A484">
+        <v>1267</v>
+      </c>
+      <c r="B484" t="s">
+        <v>54</v>
+      </c>
+      <c r="C484" t="s">
+        <v>53</v>
+      </c>
+      <c r="D484" t="s">
+        <v>59</v>
+      </c>
+      <c r="E484" t="s">
+        <v>62</v>
+      </c>
+      <c r="F484" t="s">
+        <v>596</v>
+      </c>
+      <c r="G484" t="s">
+        <v>728</v>
+      </c>
+      <c r="H484" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="485" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A485">
+        <v>1268</v>
+      </c>
+      <c r="B485" t="s">
+        <v>54</v>
+      </c>
+      <c r="C485" t="s">
+        <v>53</v>
+      </c>
+      <c r="D485" t="s">
+        <v>59</v>
+      </c>
+      <c r="E485" t="s">
+        <v>62</v>
+      </c>
+      <c r="F485" t="s">
+        <v>596</v>
+      </c>
+      <c r="G485" t="s">
+        <v>730</v>
+      </c>
+      <c r="H485" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="486" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A486">
+        <v>1269</v>
+      </c>
+      <c r="B486" t="s">
+        <v>54</v>
+      </c>
+      <c r="C486" t="s">
+        <v>53</v>
+      </c>
+      <c r="D486" t="s">
+        <v>59</v>
+      </c>
+      <c r="E486" t="s">
+        <v>62</v>
+      </c>
+      <c r="F486" t="s">
+        <v>596</v>
+      </c>
+      <c r="G486" t="s">
+        <v>732</v>
+      </c>
+      <c r="H486" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="487" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A487">
+        <v>1270</v>
+      </c>
+      <c r="B487" t="s">
+        <v>54</v>
+      </c>
+      <c r="C487" t="s">
+        <v>53</v>
+      </c>
+      <c r="D487" t="s">
+        <v>59</v>
+      </c>
+      <c r="E487" t="s">
+        <v>62</v>
+      </c>
+      <c r="F487" t="s">
+        <v>596</v>
+      </c>
+      <c r="G487" t="s">
+        <v>734</v>
+      </c>
+      <c r="H487" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="488" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A488">
+        <v>1271</v>
+      </c>
+      <c r="B488" t="s">
+        <v>54</v>
+      </c>
+      <c r="C488" t="s">
+        <v>53</v>
+      </c>
+      <c r="D488" t="s">
+        <v>59</v>
+      </c>
+      <c r="E488" t="s">
+        <v>62</v>
+      </c>
+      <c r="F488" t="s">
+        <v>596</v>
+      </c>
+      <c r="G488" t="s">
+        <v>736</v>
+      </c>
+      <c r="H488" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="489" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A489">
+        <v>1272</v>
+      </c>
+      <c r="B489" t="s">
+        <v>54</v>
+      </c>
+      <c r="C489" t="s">
+        <v>53</v>
+      </c>
+      <c r="D489" t="s">
+        <v>59</v>
+      </c>
+      <c r="E489" t="s">
+        <v>62</v>
+      </c>
+      <c r="F489" t="s">
+        <v>596</v>
+      </c>
+      <c r="G489" t="s">
+        <v>738</v>
+      </c>
+      <c r="H489" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="490" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A490">
+        <v>1273</v>
+      </c>
+      <c r="B490" t="s">
+        <v>54</v>
+      </c>
+      <c r="C490" t="s">
+        <v>53</v>
+      </c>
+      <c r="D490" t="s">
+        <v>59</v>
+      </c>
+      <c r="E490" t="s">
+        <v>62</v>
+      </c>
+      <c r="F490" t="s">
+        <v>596</v>
+      </c>
+      <c r="G490" t="s">
+        <v>740</v>
+      </c>
+      <c r="H490" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="491" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A491">
+        <v>1274</v>
+      </c>
+      <c r="B491" t="s">
+        <v>54</v>
+      </c>
+      <c r="C491" t="s">
+        <v>53</v>
+      </c>
+      <c r="D491" t="s">
+        <v>59</v>
+      </c>
+      <c r="E491" t="s">
+        <v>62</v>
+      </c>
+      <c r="F491" t="s">
+        <v>596</v>
+      </c>
+      <c r="G491" t="s">
+        <v>742</v>
+      </c>
+      <c r="H491" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="492" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A492">
+        <v>1275</v>
+      </c>
+      <c r="B492" t="s">
+        <v>54</v>
+      </c>
+      <c r="C492" t="s">
+        <v>53</v>
+      </c>
+      <c r="D492" t="s">
+        <v>59</v>
+      </c>
+      <c r="E492" t="s">
+        <v>62</v>
+      </c>
+      <c r="F492" t="s">
+        <v>596</v>
+      </c>
+      <c r="G492" t="s">
+        <v>744</v>
+      </c>
+      <c r="H492" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="493" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A493">
+        <v>1276</v>
+      </c>
+      <c r="B493" t="s">
+        <v>54</v>
+      </c>
+      <c r="C493" t="s">
+        <v>53</v>
+      </c>
+      <c r="D493" t="s">
+        <v>59</v>
+      </c>
+      <c r="E493" t="s">
+        <v>62</v>
+      </c>
+      <c r="F493" t="s">
+        <v>596</v>
+      </c>
+      <c r="G493" t="s">
+        <v>746</v>
+      </c>
+      <c r="H493" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="494" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A494">
+        <v>1277</v>
+      </c>
+      <c r="B494" t="s">
+        <v>54</v>
+      </c>
+      <c r="C494" t="s">
+        <v>53</v>
+      </c>
+      <c r="D494" t="s">
+        <v>59</v>
+      </c>
+      <c r="E494" t="s">
+        <v>62</v>
+      </c>
+      <c r="F494" t="s">
+        <v>596</v>
+      </c>
+      <c r="G494" t="s">
+        <v>748</v>
+      </c>
+      <c r="H494" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="495" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A495">
+        <v>1278</v>
+      </c>
+      <c r="B495" t="s">
+        <v>54</v>
+      </c>
+      <c r="C495" t="s">
+        <v>53</v>
+      </c>
+      <c r="D495" t="s">
+        <v>59</v>
+      </c>
+      <c r="E495" t="s">
+        <v>62</v>
+      </c>
+      <c r="F495" t="s">
+        <v>596</v>
+      </c>
+      <c r="G495" t="s">
+        <v>750</v>
+      </c>
+      <c r="H495" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="496" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A496">
+        <v>1279</v>
+      </c>
+      <c r="B496" t="s">
+        <v>54</v>
+      </c>
+      <c r="C496" t="s">
+        <v>53</v>
+      </c>
+      <c r="D496" t="s">
+        <v>59</v>
+      </c>
+      <c r="E496" t="s">
+        <v>62</v>
+      </c>
+      <c r="F496" t="s">
+        <v>596</v>
+      </c>
+      <c r="G496" t="s">
+        <v>752</v>
+      </c>
+      <c r="H496" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="497" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A497">
+        <v>1280</v>
+      </c>
+      <c r="B497" t="s">
+        <v>54</v>
+      </c>
+      <c r="C497" t="s">
+        <v>53</v>
+      </c>
+      <c r="D497" t="s">
+        <v>59</v>
+      </c>
+      <c r="E497" t="s">
+        <v>62</v>
+      </c>
+      <c r="F497" t="s">
+        <v>596</v>
+      </c>
+      <c r="G497" t="s">
+        <v>754</v>
+      </c>
+      <c r="H497" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="498" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A498">
+        <v>1281</v>
+      </c>
+      <c r="B498" t="s">
+        <v>54</v>
+      </c>
+      <c r="C498" t="s">
+        <v>53</v>
+      </c>
+      <c r="D498" t="s">
+        <v>59</v>
+      </c>
+      <c r="E498" t="s">
+        <v>62</v>
+      </c>
+      <c r="F498" t="s">
+        <v>596</v>
+      </c>
+      <c r="G498" t="s">
+        <v>756</v>
+      </c>
+      <c r="H498" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="499" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A499">
+        <v>1282</v>
+      </c>
+      <c r="B499" t="s">
+        <v>54</v>
+      </c>
+      <c r="C499" t="s">
+        <v>53</v>
+      </c>
+      <c r="D499" t="s">
+        <v>59</v>
+      </c>
+      <c r="E499" t="s">
+        <v>62</v>
+      </c>
+      <c r="F499" t="s">
+        <v>596</v>
+      </c>
+      <c r="G499" t="s">
+        <v>758</v>
+      </c>
+      <c r="H499" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="500" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A500">
+        <v>1283</v>
+      </c>
+      <c r="B500" t="s">
+        <v>54</v>
+      </c>
+      <c r="C500" t="s">
+        <v>53</v>
+      </c>
+      <c r="D500" t="s">
+        <v>59</v>
+      </c>
+      <c r="E500" t="s">
+        <v>62</v>
+      </c>
+      <c r="F500" t="s">
+        <v>596</v>
+      </c>
+      <c r="G500" t="s">
+        <v>760</v>
+      </c>
+      <c r="H500" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="501" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A501">
+        <v>1284</v>
+      </c>
+      <c r="B501" t="s">
+        <v>54</v>
+      </c>
+      <c r="C501" t="s">
+        <v>53</v>
+      </c>
+      <c r="D501" t="s">
+        <v>59</v>
+      </c>
+      <c r="E501" t="s">
+        <v>62</v>
+      </c>
+      <c r="F501" t="s">
+        <v>596</v>
+      </c>
+      <c r="G501" t="s">
+        <v>762</v>
+      </c>
+      <c r="H501" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="502" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A502">
+        <v>1285</v>
+      </c>
+      <c r="B502" t="s">
+        <v>54</v>
+      </c>
+      <c r="C502" t="s">
+        <v>53</v>
+      </c>
+      <c r="D502" t="s">
+        <v>59</v>
+      </c>
+      <c r="E502" t="s">
+        <v>62</v>
+      </c>
+      <c r="F502" t="s">
+        <v>596</v>
+      </c>
+      <c r="G502" t="s">
+        <v>692</v>
+      </c>
+      <c r="H502" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="503" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A503">
+        <v>1286</v>
+      </c>
+      <c r="B503" t="s">
+        <v>54</v>
+      </c>
+      <c r="C503" t="s">
+        <v>53</v>
+      </c>
+      <c r="D503" t="s">
+        <v>59</v>
+      </c>
+      <c r="E503" t="s">
+        <v>62</v>
+      </c>
+      <c r="F503" t="s">
+        <v>596</v>
+      </c>
+      <c r="G503" t="s">
+        <v>764</v>
+      </c>
+      <c r="H503" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="504" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A504">
+        <v>1287</v>
+      </c>
+      <c r="B504" t="s">
+        <v>54</v>
+      </c>
+      <c r="C504" t="s">
+        <v>53</v>
+      </c>
+      <c r="D504" t="s">
+        <v>59</v>
+      </c>
+      <c r="E504" t="s">
+        <v>62</v>
+      </c>
+      <c r="F504" t="s">
+        <v>596</v>
+      </c>
+      <c r="G504" t="s">
+        <v>766</v>
+      </c>
+      <c r="H504" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="505" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A505">
+        <v>1288</v>
+      </c>
+      <c r="B505" t="s">
+        <v>54</v>
+      </c>
+      <c r="C505" t="s">
+        <v>53</v>
+      </c>
+      <c r="D505" t="s">
+        <v>59</v>
+      </c>
+      <c r="E505" t="s">
+        <v>62</v>
+      </c>
+      <c r="F505" t="s">
+        <v>596</v>
+      </c>
+      <c r="G505" t="s">
+        <v>768</v>
+      </c>
+      <c r="H505" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="506" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A506">
+        <v>1289</v>
+      </c>
+      <c r="B506" t="s">
+        <v>54</v>
+      </c>
+      <c r="C506" t="s">
+        <v>53</v>
+      </c>
+      <c r="D506" t="s">
+        <v>59</v>
+      </c>
+      <c r="E506" t="s">
+        <v>62</v>
+      </c>
+      <c r="F506" t="s">
+        <v>596</v>
+      </c>
+      <c r="G506" t="s">
+        <v>770</v>
+      </c>
+      <c r="H506" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="507" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A507">
+        <v>1290</v>
+      </c>
+      <c r="B507" t="s">
+        <v>54</v>
+      </c>
+      <c r="C507" t="s">
+        <v>53</v>
+      </c>
+      <c r="D507" t="s">
+        <v>59</v>
+      </c>
+      <c r="E507" t="s">
+        <v>62</v>
+      </c>
+      <c r="F507" t="s">
+        <v>596</v>
+      </c>
+      <c r="G507" t="s">
+        <v>772</v>
+      </c>
+      <c r="H507" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="508" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A508">
+        <v>1291</v>
+      </c>
+      <c r="B508" t="s">
+        <v>54</v>
+      </c>
+      <c r="C508" t="s">
+        <v>53</v>
+      </c>
+      <c r="D508" t="s">
+        <v>59</v>
+      </c>
+      <c r="E508" t="s">
+        <v>62</v>
+      </c>
+      <c r="F508" t="s">
+        <v>596</v>
+      </c>
+      <c r="G508" t="s">
+        <v>704</v>
+      </c>
+      <c r="H508" t="s">
+        <v>774</v>
       </c>
     </row>
   </sheetData>

</xml_diff>